<commit_message>
Add role manage pages.
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -25,10 +25,10 @@
     <author>joe.feng@hotmail.com</author>
   </authors>
   <commentList>
-    <comment ref="C22" authorId="0" shapeId="0">
+    <comment ref="C25" authorId="0" shapeId="0">
       <text/>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0">
+    <comment ref="G25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
   <si>
     <t>Comments</t>
   </si>
@@ -843,6 +843,27 @@
   <si>
     <t>/departments/$id/employees?page=1&amp;pageSize=10</t>
   </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Get roles by page</t>
+  </si>
+  <si>
+    <t>/roles?page=1&amp;pageSize=10</t>
+  </si>
+  <si>
+    <t>{
+ "count": 100,
+ "roles":[{
+   "id": 1,
+   "name": "",
+   "category": "",
+   "creator": "",
+   "remark": ""
+  }]
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -1053,7 +1074,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1254,6 +1275,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1627,11 +1651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IX45"/>
+  <dimension ref="A1:IX48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -5173,14 +5197,24 @@
       <c r="IX14" s="35"/>
     </row>
     <row r="15" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="A15" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>25</v>
+      </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37"/>
       <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
+      <c r="H15" s="39" t="s">
+        <v>129</v>
+      </c>
       <c r="I15" s="37"/>
       <c r="J15" s="39"/>
       <c r="K15" s="37"/>
@@ -5432,278 +5466,278 @@
       <c r="IW15" s="12"/>
       <c r="IX15" s="12"/>
     </row>
-    <row r="16" spans="1:258" s="36" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="35"/>
-      <c r="AF16" s="35"/>
-      <c r="AG16" s="35"/>
-      <c r="AH16" s="35"/>
-      <c r="AI16" s="35"/>
-      <c r="AJ16" s="35"/>
-      <c r="AK16" s="35"/>
-      <c r="AL16" s="35"/>
-      <c r="AM16" s="35"/>
-      <c r="AN16" s="35"/>
-      <c r="AO16" s="35"/>
-      <c r="AP16" s="35"/>
-      <c r="AQ16" s="35"/>
-      <c r="AR16" s="35"/>
-      <c r="AS16" s="35"/>
-      <c r="AT16" s="35"/>
-      <c r="AU16" s="35"/>
-      <c r="AV16" s="35"/>
-      <c r="AW16" s="35"/>
-      <c r="AX16" s="35"/>
-      <c r="AY16" s="35"/>
-      <c r="AZ16" s="35"/>
-      <c r="BA16" s="35"/>
-      <c r="BB16" s="35"/>
-      <c r="BC16" s="35"/>
-      <c r="BD16" s="35"/>
-      <c r="BE16" s="35"/>
-      <c r="BF16" s="35"/>
-      <c r="BG16" s="35"/>
-      <c r="BH16" s="35"/>
-      <c r="BI16" s="35"/>
-      <c r="BJ16" s="35"/>
-      <c r="BK16" s="35"/>
-      <c r="BL16" s="35"/>
-      <c r="BM16" s="35"/>
-      <c r="BN16" s="35"/>
-      <c r="BO16" s="35"/>
-      <c r="BP16" s="35"/>
-      <c r="BQ16" s="35"/>
-      <c r="BR16" s="35"/>
-      <c r="BS16" s="35"/>
-      <c r="BT16" s="35"/>
-      <c r="BU16" s="35"/>
-      <c r="BV16" s="35"/>
-      <c r="BW16" s="35"/>
-      <c r="BX16" s="35"/>
-      <c r="BY16" s="35"/>
-      <c r="BZ16" s="35"/>
-      <c r="CA16" s="35"/>
-      <c r="CB16" s="35"/>
-      <c r="CC16" s="35"/>
-      <c r="CD16" s="35"/>
-      <c r="CE16" s="35"/>
-      <c r="CF16" s="35"/>
-      <c r="CG16" s="35"/>
-      <c r="CH16" s="35"/>
-      <c r="CI16" s="35"/>
-      <c r="CJ16" s="35"/>
-      <c r="CK16" s="35"/>
-      <c r="CL16" s="35"/>
-      <c r="CM16" s="35"/>
-      <c r="CN16" s="35"/>
-      <c r="CO16" s="35"/>
-      <c r="CP16" s="35"/>
-      <c r="CQ16" s="35"/>
-      <c r="CR16" s="35"/>
-      <c r="CS16" s="35"/>
-      <c r="CT16" s="35"/>
-      <c r="CU16" s="35"/>
-      <c r="CV16" s="35"/>
-      <c r="CW16" s="35"/>
-      <c r="CX16" s="35"/>
-      <c r="CY16" s="35"/>
-      <c r="CZ16" s="35"/>
-      <c r="DA16" s="35"/>
-      <c r="DB16" s="35"/>
-      <c r="DC16" s="35"/>
-      <c r="DD16" s="35"/>
-      <c r="DE16" s="35"/>
-      <c r="DF16" s="35"/>
-      <c r="DG16" s="35"/>
-      <c r="DH16" s="35"/>
-      <c r="DI16" s="35"/>
-      <c r="DJ16" s="35"/>
-      <c r="DK16" s="35"/>
-      <c r="DL16" s="35"/>
-      <c r="DM16" s="35"/>
-      <c r="DN16" s="35"/>
-      <c r="DO16" s="35"/>
-      <c r="DP16" s="35"/>
-      <c r="DQ16" s="35"/>
-      <c r="DR16" s="35"/>
-      <c r="DS16" s="35"/>
-      <c r="DT16" s="35"/>
-      <c r="DU16" s="35"/>
-      <c r="DV16" s="35"/>
-      <c r="DW16" s="35"/>
-      <c r="DX16" s="35"/>
-      <c r="DY16" s="35"/>
-      <c r="DZ16" s="35"/>
-      <c r="EA16" s="35"/>
-      <c r="EB16" s="35"/>
-      <c r="EC16" s="35"/>
-      <c r="ED16" s="35"/>
-      <c r="EE16" s="35"/>
-      <c r="EF16" s="35"/>
-      <c r="EG16" s="35"/>
-      <c r="EH16" s="35"/>
-      <c r="EI16" s="35"/>
-      <c r="EJ16" s="35"/>
-      <c r="EK16" s="35"/>
-      <c r="EL16" s="35"/>
-      <c r="EM16" s="35"/>
-      <c r="EN16" s="35"/>
-      <c r="EO16" s="35"/>
-      <c r="EP16" s="35"/>
-      <c r="EQ16" s="35"/>
-      <c r="ER16" s="35"/>
-      <c r="ES16" s="35"/>
-      <c r="ET16" s="35"/>
-      <c r="EU16" s="35"/>
-      <c r="EV16" s="35"/>
-      <c r="EW16" s="35"/>
-      <c r="EX16" s="35"/>
-      <c r="EY16" s="35"/>
-      <c r="EZ16" s="35"/>
-      <c r="FA16" s="35"/>
-      <c r="FB16" s="35"/>
-      <c r="FC16" s="35"/>
-      <c r="FD16" s="35"/>
-      <c r="FE16" s="35"/>
-      <c r="FF16" s="35"/>
-      <c r="FG16" s="35"/>
-      <c r="FH16" s="35"/>
-      <c r="FI16" s="35"/>
-      <c r="FJ16" s="35"/>
-      <c r="FK16" s="35"/>
-      <c r="FL16" s="35"/>
-      <c r="FM16" s="35"/>
-      <c r="FN16" s="35"/>
-      <c r="FO16" s="35"/>
-      <c r="FP16" s="35"/>
-      <c r="FQ16" s="35"/>
-      <c r="FR16" s="35"/>
-      <c r="FS16" s="35"/>
-      <c r="FT16" s="35"/>
-      <c r="FU16" s="35"/>
-      <c r="FV16" s="35"/>
-      <c r="FW16" s="35"/>
-      <c r="FX16" s="35"/>
-      <c r="FY16" s="35"/>
-      <c r="FZ16" s="35"/>
-      <c r="GA16" s="35"/>
-      <c r="GB16" s="35"/>
-      <c r="GC16" s="35"/>
-      <c r="GD16" s="35"/>
-      <c r="GE16" s="35"/>
-      <c r="GF16" s="35"/>
-      <c r="GG16" s="35"/>
-      <c r="GH16" s="35"/>
-      <c r="GI16" s="35"/>
-      <c r="GJ16" s="35"/>
-      <c r="GK16" s="35"/>
-      <c r="GL16" s="35"/>
-      <c r="GM16" s="35"/>
-      <c r="GN16" s="35"/>
-      <c r="GO16" s="35"/>
-      <c r="GP16" s="35"/>
-      <c r="GQ16" s="35"/>
-      <c r="GR16" s="35"/>
-      <c r="GS16" s="35"/>
-      <c r="GT16" s="35"/>
-      <c r="GU16" s="35"/>
-      <c r="GV16" s="35"/>
-      <c r="GW16" s="35"/>
-      <c r="GX16" s="35"/>
-      <c r="GY16" s="35"/>
-      <c r="GZ16" s="35"/>
-      <c r="HA16" s="35"/>
-      <c r="HB16" s="35"/>
-      <c r="HC16" s="35"/>
-      <c r="HD16" s="35"/>
-      <c r="HE16" s="35"/>
-      <c r="HF16" s="35"/>
-      <c r="HG16" s="35"/>
-      <c r="HH16" s="35"/>
-      <c r="HI16" s="35"/>
-      <c r="HJ16" s="35"/>
-      <c r="HK16" s="35"/>
-      <c r="HL16" s="35"/>
-      <c r="HM16" s="35"/>
-      <c r="HN16" s="35"/>
-      <c r="HO16" s="35"/>
-      <c r="HP16" s="35"/>
-      <c r="HQ16" s="35"/>
-      <c r="HR16" s="35"/>
-      <c r="HS16" s="35"/>
-      <c r="HT16" s="35"/>
-      <c r="HU16" s="35"/>
-      <c r="HV16" s="35"/>
-      <c r="HW16" s="35"/>
-      <c r="HX16" s="35"/>
-      <c r="HY16" s="35"/>
-      <c r="HZ16" s="35"/>
-      <c r="IA16" s="35"/>
-      <c r="IB16" s="35"/>
-      <c r="IC16" s="35"/>
-      <c r="ID16" s="35"/>
-      <c r="IE16" s="35"/>
-      <c r="IF16" s="35"/>
-      <c r="IG16" s="35"/>
-      <c r="IH16" s="35"/>
-      <c r="II16" s="35"/>
-      <c r="IJ16" s="35"/>
-      <c r="IK16" s="35"/>
-      <c r="IL16" s="35"/>
-      <c r="IM16" s="35"/>
-      <c r="IN16" s="35"/>
-      <c r="IO16" s="35"/>
-      <c r="IP16" s="35"/>
-      <c r="IQ16" s="35"/>
-      <c r="IR16" s="35"/>
-      <c r="IS16" s="35"/>
-      <c r="IT16" s="35"/>
-      <c r="IU16" s="35"/>
-      <c r="IV16" s="35"/>
-      <c r="IW16" s="35"/>
-      <c r="IX16" s="35"/>
+    <row r="16" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="65"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="12"/>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="AW16" s="12"/>
+      <c r="AX16" s="12"/>
+      <c r="AY16" s="12"/>
+      <c r="AZ16" s="12"/>
+      <c r="BA16" s="12"/>
+      <c r="BB16" s="12"/>
+      <c r="BC16" s="12"/>
+      <c r="BD16" s="12"/>
+      <c r="BE16" s="12"/>
+      <c r="BF16" s="12"/>
+      <c r="BG16" s="12"/>
+      <c r="BH16" s="12"/>
+      <c r="BI16" s="12"/>
+      <c r="BJ16" s="12"/>
+      <c r="BK16" s="12"/>
+      <c r="BL16" s="12"/>
+      <c r="BM16" s="12"/>
+      <c r="BN16" s="12"/>
+      <c r="BO16" s="12"/>
+      <c r="BP16" s="12"/>
+      <c r="BQ16" s="12"/>
+      <c r="BR16" s="12"/>
+      <c r="BS16" s="12"/>
+      <c r="BT16" s="12"/>
+      <c r="BU16" s="12"/>
+      <c r="BV16" s="12"/>
+      <c r="BW16" s="12"/>
+      <c r="BX16" s="12"/>
+      <c r="BY16" s="12"/>
+      <c r="BZ16" s="12"/>
+      <c r="CA16" s="12"/>
+      <c r="CB16" s="12"/>
+      <c r="CC16" s="12"/>
+      <c r="CD16" s="12"/>
+      <c r="CE16" s="12"/>
+      <c r="CF16" s="12"/>
+      <c r="CG16" s="12"/>
+      <c r="CH16" s="12"/>
+      <c r="CI16" s="12"/>
+      <c r="CJ16" s="12"/>
+      <c r="CK16" s="12"/>
+      <c r="CL16" s="12"/>
+      <c r="CM16" s="12"/>
+      <c r="CN16" s="12"/>
+      <c r="CO16" s="12"/>
+      <c r="CP16" s="12"/>
+      <c r="CQ16" s="12"/>
+      <c r="CR16" s="12"/>
+      <c r="CS16" s="12"/>
+      <c r="CT16" s="12"/>
+      <c r="CU16" s="12"/>
+      <c r="CV16" s="12"/>
+      <c r="CW16" s="12"/>
+      <c r="CX16" s="12"/>
+      <c r="CY16" s="12"/>
+      <c r="CZ16" s="12"/>
+      <c r="DA16" s="12"/>
+      <c r="DB16" s="12"/>
+      <c r="DC16" s="12"/>
+      <c r="DD16" s="12"/>
+      <c r="DE16" s="12"/>
+      <c r="DF16" s="12"/>
+      <c r="DG16" s="12"/>
+      <c r="DH16" s="12"/>
+      <c r="DI16" s="12"/>
+      <c r="DJ16" s="12"/>
+      <c r="DK16" s="12"/>
+      <c r="DL16" s="12"/>
+      <c r="DM16" s="12"/>
+      <c r="DN16" s="12"/>
+      <c r="DO16" s="12"/>
+      <c r="DP16" s="12"/>
+      <c r="DQ16" s="12"/>
+      <c r="DR16" s="12"/>
+      <c r="DS16" s="12"/>
+      <c r="DT16" s="12"/>
+      <c r="DU16" s="12"/>
+      <c r="DV16" s="12"/>
+      <c r="DW16" s="12"/>
+      <c r="DX16" s="12"/>
+      <c r="DY16" s="12"/>
+      <c r="DZ16" s="12"/>
+      <c r="EA16" s="12"/>
+      <c r="EB16" s="12"/>
+      <c r="EC16" s="12"/>
+      <c r="ED16" s="12"/>
+      <c r="EE16" s="12"/>
+      <c r="EF16" s="12"/>
+      <c r="EG16" s="12"/>
+      <c r="EH16" s="12"/>
+      <c r="EI16" s="12"/>
+      <c r="EJ16" s="12"/>
+      <c r="EK16" s="12"/>
+      <c r="EL16" s="12"/>
+      <c r="EM16" s="12"/>
+      <c r="EN16" s="12"/>
+      <c r="EO16" s="12"/>
+      <c r="EP16" s="12"/>
+      <c r="EQ16" s="12"/>
+      <c r="ER16" s="12"/>
+      <c r="ES16" s="12"/>
+      <c r="ET16" s="12"/>
+      <c r="EU16" s="12"/>
+      <c r="EV16" s="12"/>
+      <c r="EW16" s="12"/>
+      <c r="EX16" s="12"/>
+      <c r="EY16" s="12"/>
+      <c r="EZ16" s="12"/>
+      <c r="FA16" s="12"/>
+      <c r="FB16" s="12"/>
+      <c r="FC16" s="12"/>
+      <c r="FD16" s="12"/>
+      <c r="FE16" s="12"/>
+      <c r="FF16" s="12"/>
+      <c r="FG16" s="12"/>
+      <c r="FH16" s="12"/>
+      <c r="FI16" s="12"/>
+      <c r="FJ16" s="12"/>
+      <c r="FK16" s="12"/>
+      <c r="FL16" s="12"/>
+      <c r="FM16" s="12"/>
+      <c r="FN16" s="12"/>
+      <c r="FO16" s="12"/>
+      <c r="FP16" s="12"/>
+      <c r="FQ16" s="12"/>
+      <c r="FR16" s="12"/>
+      <c r="FS16" s="12"/>
+      <c r="FT16" s="12"/>
+      <c r="FU16" s="12"/>
+      <c r="FV16" s="12"/>
+      <c r="FW16" s="12"/>
+      <c r="FX16" s="12"/>
+      <c r="FY16" s="12"/>
+      <c r="FZ16" s="12"/>
+      <c r="GA16" s="12"/>
+      <c r="GB16" s="12"/>
+      <c r="GC16" s="12"/>
+      <c r="GD16" s="12"/>
+      <c r="GE16" s="12"/>
+      <c r="GF16" s="12"/>
+      <c r="GG16" s="12"/>
+      <c r="GH16" s="12"/>
+      <c r="GI16" s="12"/>
+      <c r="GJ16" s="12"/>
+      <c r="GK16" s="12"/>
+      <c r="GL16" s="12"/>
+      <c r="GM16" s="12"/>
+      <c r="GN16" s="12"/>
+      <c r="GO16" s="12"/>
+      <c r="GP16" s="12"/>
+      <c r="GQ16" s="12"/>
+      <c r="GR16" s="12"/>
+      <c r="GS16" s="12"/>
+      <c r="GT16" s="12"/>
+      <c r="GU16" s="12"/>
+      <c r="GV16" s="12"/>
+      <c r="GW16" s="12"/>
+      <c r="GX16" s="12"/>
+      <c r="GY16" s="12"/>
+      <c r="GZ16" s="12"/>
+      <c r="HA16" s="12"/>
+      <c r="HB16" s="12"/>
+      <c r="HC16" s="12"/>
+      <c r="HD16" s="12"/>
+      <c r="HE16" s="12"/>
+      <c r="HF16" s="12"/>
+      <c r="HG16" s="12"/>
+      <c r="HH16" s="12"/>
+      <c r="HI16" s="12"/>
+      <c r="HJ16" s="12"/>
+      <c r="HK16" s="12"/>
+      <c r="HL16" s="12"/>
+      <c r="HM16" s="12"/>
+      <c r="HN16" s="12"/>
+      <c r="HO16" s="12"/>
+      <c r="HP16" s="12"/>
+      <c r="HQ16" s="12"/>
+      <c r="HR16" s="12"/>
+      <c r="HS16" s="12"/>
+      <c r="HT16" s="12"/>
+      <c r="HU16" s="12"/>
+      <c r="HV16" s="12"/>
+      <c r="HW16" s="12"/>
+      <c r="HX16" s="12"/>
+      <c r="HY16" s="12"/>
+      <c r="HZ16" s="12"/>
+      <c r="IA16" s="12"/>
+      <c r="IB16" s="12"/>
+      <c r="IC16" s="12"/>
+      <c r="ID16" s="12"/>
+      <c r="IE16" s="12"/>
+      <c r="IF16" s="12"/>
+      <c r="IG16" s="12"/>
+      <c r="IH16" s="12"/>
+      <c r="II16" s="12"/>
+      <c r="IJ16" s="12"/>
+      <c r="IK16" s="12"/>
+      <c r="IL16" s="12"/>
+      <c r="IM16" s="12"/>
+      <c r="IN16" s="12"/>
+      <c r="IO16" s="12"/>
+      <c r="IP16" s="12"/>
+      <c r="IQ16" s="12"/>
+      <c r="IR16" s="12"/>
+      <c r="IS16" s="12"/>
+      <c r="IT16" s="12"/>
+      <c r="IU16" s="12"/>
+      <c r="IV16" s="12"/>
+      <c r="IW16" s="12"/>
+      <c r="IX16" s="12"/>
     </row>
     <row r="17" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="30"/>
+      <c r="A17" s="65"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
@@ -5953,13 +5987,13 @@
       <c r="IX17" s="12"/>
     </row>
     <row r="18" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="11"/>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
@@ -6212,278 +6246,278 @@
       <c r="IW18" s="12"/>
       <c r="IX18" s="12"/>
     </row>
-    <row r="19" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="12"/>
-      <c r="AG19" s="12"/>
-      <c r="AH19" s="12"/>
-      <c r="AI19" s="12"/>
-      <c r="AJ19" s="12"/>
-      <c r="AK19" s="12"/>
-      <c r="AL19" s="12"/>
-      <c r="AM19" s="12"/>
-      <c r="AN19" s="12"/>
-      <c r="AO19" s="12"/>
-      <c r="AP19" s="12"/>
-      <c r="AQ19" s="12"/>
-      <c r="AR19" s="12"/>
-      <c r="AS19" s="12"/>
-      <c r="AT19" s="12"/>
-      <c r="AU19" s="12"/>
-      <c r="AV19" s="12"/>
-      <c r="AW19" s="12"/>
-      <c r="AX19" s="12"/>
-      <c r="AY19" s="12"/>
-      <c r="AZ19" s="12"/>
-      <c r="BA19" s="12"/>
-      <c r="BB19" s="12"/>
-      <c r="BC19" s="12"/>
-      <c r="BD19" s="12"/>
-      <c r="BE19" s="12"/>
-      <c r="BF19" s="12"/>
-      <c r="BG19" s="12"/>
-      <c r="BH19" s="12"/>
-      <c r="BI19" s="12"/>
-      <c r="BJ19" s="12"/>
-      <c r="BK19" s="12"/>
-      <c r="BL19" s="12"/>
-      <c r="BM19" s="12"/>
-      <c r="BN19" s="12"/>
-      <c r="BO19" s="12"/>
-      <c r="BP19" s="12"/>
-      <c r="BQ19" s="12"/>
-      <c r="BR19" s="12"/>
-      <c r="BS19" s="12"/>
-      <c r="BT19" s="12"/>
-      <c r="BU19" s="12"/>
-      <c r="BV19" s="12"/>
-      <c r="BW19" s="12"/>
-      <c r="BX19" s="12"/>
-      <c r="BY19" s="12"/>
-      <c r="BZ19" s="12"/>
-      <c r="CA19" s="12"/>
-      <c r="CB19" s="12"/>
-      <c r="CC19" s="12"/>
-      <c r="CD19" s="12"/>
-      <c r="CE19" s="12"/>
-      <c r="CF19" s="12"/>
-      <c r="CG19" s="12"/>
-      <c r="CH19" s="12"/>
-      <c r="CI19" s="12"/>
-      <c r="CJ19" s="12"/>
-      <c r="CK19" s="12"/>
-      <c r="CL19" s="12"/>
-      <c r="CM19" s="12"/>
-      <c r="CN19" s="12"/>
-      <c r="CO19" s="12"/>
-      <c r="CP19" s="12"/>
-      <c r="CQ19" s="12"/>
-      <c r="CR19" s="12"/>
-      <c r="CS19" s="12"/>
-      <c r="CT19" s="12"/>
-      <c r="CU19" s="12"/>
-      <c r="CV19" s="12"/>
-      <c r="CW19" s="12"/>
-      <c r="CX19" s="12"/>
-      <c r="CY19" s="12"/>
-      <c r="CZ19" s="12"/>
-      <c r="DA19" s="12"/>
-      <c r="DB19" s="12"/>
-      <c r="DC19" s="12"/>
-      <c r="DD19" s="12"/>
-      <c r="DE19" s="12"/>
-      <c r="DF19" s="12"/>
-      <c r="DG19" s="12"/>
-      <c r="DH19" s="12"/>
-      <c r="DI19" s="12"/>
-      <c r="DJ19" s="12"/>
-      <c r="DK19" s="12"/>
-      <c r="DL19" s="12"/>
-      <c r="DM19" s="12"/>
-      <c r="DN19" s="12"/>
-      <c r="DO19" s="12"/>
-      <c r="DP19" s="12"/>
-      <c r="DQ19" s="12"/>
-      <c r="DR19" s="12"/>
-      <c r="DS19" s="12"/>
-      <c r="DT19" s="12"/>
-      <c r="DU19" s="12"/>
-      <c r="DV19" s="12"/>
-      <c r="DW19" s="12"/>
-      <c r="DX19" s="12"/>
-      <c r="DY19" s="12"/>
-      <c r="DZ19" s="12"/>
-      <c r="EA19" s="12"/>
-      <c r="EB19" s="12"/>
-      <c r="EC19" s="12"/>
-      <c r="ED19" s="12"/>
-      <c r="EE19" s="12"/>
-      <c r="EF19" s="12"/>
-      <c r="EG19" s="12"/>
-      <c r="EH19" s="12"/>
-      <c r="EI19" s="12"/>
-      <c r="EJ19" s="12"/>
-      <c r="EK19" s="12"/>
-      <c r="EL19" s="12"/>
-      <c r="EM19" s="12"/>
-      <c r="EN19" s="12"/>
-      <c r="EO19" s="12"/>
-      <c r="EP19" s="12"/>
-      <c r="EQ19" s="12"/>
-      <c r="ER19" s="12"/>
-      <c r="ES19" s="12"/>
-      <c r="ET19" s="12"/>
-      <c r="EU19" s="12"/>
-      <c r="EV19" s="12"/>
-      <c r="EW19" s="12"/>
-      <c r="EX19" s="12"/>
-      <c r="EY19" s="12"/>
-      <c r="EZ19" s="12"/>
-      <c r="FA19" s="12"/>
-      <c r="FB19" s="12"/>
-      <c r="FC19" s="12"/>
-      <c r="FD19" s="12"/>
-      <c r="FE19" s="12"/>
-      <c r="FF19" s="12"/>
-      <c r="FG19" s="12"/>
-      <c r="FH19" s="12"/>
-      <c r="FI19" s="12"/>
-      <c r="FJ19" s="12"/>
-      <c r="FK19" s="12"/>
-      <c r="FL19" s="12"/>
-      <c r="FM19" s="12"/>
-      <c r="FN19" s="12"/>
-      <c r="FO19" s="12"/>
-      <c r="FP19" s="12"/>
-      <c r="FQ19" s="12"/>
-      <c r="FR19" s="12"/>
-      <c r="FS19" s="12"/>
-      <c r="FT19" s="12"/>
-      <c r="FU19" s="12"/>
-      <c r="FV19" s="12"/>
-      <c r="FW19" s="12"/>
-      <c r="FX19" s="12"/>
-      <c r="FY19" s="12"/>
-      <c r="FZ19" s="12"/>
-      <c r="GA19" s="12"/>
-      <c r="GB19" s="12"/>
-      <c r="GC19" s="12"/>
-      <c r="GD19" s="12"/>
-      <c r="GE19" s="12"/>
-      <c r="GF19" s="12"/>
-      <c r="GG19" s="12"/>
-      <c r="GH19" s="12"/>
-      <c r="GI19" s="12"/>
-      <c r="GJ19" s="12"/>
-      <c r="GK19" s="12"/>
-      <c r="GL19" s="12"/>
-      <c r="GM19" s="12"/>
-      <c r="GN19" s="12"/>
-      <c r="GO19" s="12"/>
-      <c r="GP19" s="12"/>
-      <c r="GQ19" s="12"/>
-      <c r="GR19" s="12"/>
-      <c r="GS19" s="12"/>
-      <c r="GT19" s="12"/>
-      <c r="GU19" s="12"/>
-      <c r="GV19" s="12"/>
-      <c r="GW19" s="12"/>
-      <c r="GX19" s="12"/>
-      <c r="GY19" s="12"/>
-      <c r="GZ19" s="12"/>
-      <c r="HA19" s="12"/>
-      <c r="HB19" s="12"/>
-      <c r="HC19" s="12"/>
-      <c r="HD19" s="12"/>
-      <c r="HE19" s="12"/>
-      <c r="HF19" s="12"/>
-      <c r="HG19" s="12"/>
-      <c r="HH19" s="12"/>
-      <c r="HI19" s="12"/>
-      <c r="HJ19" s="12"/>
-      <c r="HK19" s="12"/>
-      <c r="HL19" s="12"/>
-      <c r="HM19" s="12"/>
-      <c r="HN19" s="12"/>
-      <c r="HO19" s="12"/>
-      <c r="HP19" s="12"/>
-      <c r="HQ19" s="12"/>
-      <c r="HR19" s="12"/>
-      <c r="HS19" s="12"/>
-      <c r="HT19" s="12"/>
-      <c r="HU19" s="12"/>
-      <c r="HV19" s="12"/>
-      <c r="HW19" s="12"/>
-      <c r="HX19" s="12"/>
-      <c r="HY19" s="12"/>
-      <c r="HZ19" s="12"/>
-      <c r="IA19" s="12"/>
-      <c r="IB19" s="12"/>
-      <c r="IC19" s="12"/>
-      <c r="ID19" s="12"/>
-      <c r="IE19" s="12"/>
-      <c r="IF19" s="12"/>
-      <c r="IG19" s="12"/>
-      <c r="IH19" s="12"/>
-      <c r="II19" s="12"/>
-      <c r="IJ19" s="12"/>
-      <c r="IK19" s="12"/>
-      <c r="IL19" s="12"/>
-      <c r="IM19" s="12"/>
-      <c r="IN19" s="12"/>
-      <c r="IO19" s="12"/>
-      <c r="IP19" s="12"/>
-      <c r="IQ19" s="12"/>
-      <c r="IR19" s="12"/>
-      <c r="IS19" s="12"/>
-      <c r="IT19" s="12"/>
-      <c r="IU19" s="12"/>
-      <c r="IV19" s="12"/>
-      <c r="IW19" s="12"/>
-      <c r="IX19" s="12"/>
+    <row r="19" spans="1:258" s="36" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="40"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
+      <c r="X19" s="35"/>
+      <c r="Y19" s="35"/>
+      <c r="Z19" s="35"/>
+      <c r="AA19" s="35"/>
+      <c r="AB19" s="35"/>
+      <c r="AC19" s="35"/>
+      <c r="AD19" s="35"/>
+      <c r="AE19" s="35"/>
+      <c r="AF19" s="35"/>
+      <c r="AG19" s="35"/>
+      <c r="AH19" s="35"/>
+      <c r="AI19" s="35"/>
+      <c r="AJ19" s="35"/>
+      <c r="AK19" s="35"/>
+      <c r="AL19" s="35"/>
+      <c r="AM19" s="35"/>
+      <c r="AN19" s="35"/>
+      <c r="AO19" s="35"/>
+      <c r="AP19" s="35"/>
+      <c r="AQ19" s="35"/>
+      <c r="AR19" s="35"/>
+      <c r="AS19" s="35"/>
+      <c r="AT19" s="35"/>
+      <c r="AU19" s="35"/>
+      <c r="AV19" s="35"/>
+      <c r="AW19" s="35"/>
+      <c r="AX19" s="35"/>
+      <c r="AY19" s="35"/>
+      <c r="AZ19" s="35"/>
+      <c r="BA19" s="35"/>
+      <c r="BB19" s="35"/>
+      <c r="BC19" s="35"/>
+      <c r="BD19" s="35"/>
+      <c r="BE19" s="35"/>
+      <c r="BF19" s="35"/>
+      <c r="BG19" s="35"/>
+      <c r="BH19" s="35"/>
+      <c r="BI19" s="35"/>
+      <c r="BJ19" s="35"/>
+      <c r="BK19" s="35"/>
+      <c r="BL19" s="35"/>
+      <c r="BM19" s="35"/>
+      <c r="BN19" s="35"/>
+      <c r="BO19" s="35"/>
+      <c r="BP19" s="35"/>
+      <c r="BQ19" s="35"/>
+      <c r="BR19" s="35"/>
+      <c r="BS19" s="35"/>
+      <c r="BT19" s="35"/>
+      <c r="BU19" s="35"/>
+      <c r="BV19" s="35"/>
+      <c r="BW19" s="35"/>
+      <c r="BX19" s="35"/>
+      <c r="BY19" s="35"/>
+      <c r="BZ19" s="35"/>
+      <c r="CA19" s="35"/>
+      <c r="CB19" s="35"/>
+      <c r="CC19" s="35"/>
+      <c r="CD19" s="35"/>
+      <c r="CE19" s="35"/>
+      <c r="CF19" s="35"/>
+      <c r="CG19" s="35"/>
+      <c r="CH19" s="35"/>
+      <c r="CI19" s="35"/>
+      <c r="CJ19" s="35"/>
+      <c r="CK19" s="35"/>
+      <c r="CL19" s="35"/>
+      <c r="CM19" s="35"/>
+      <c r="CN19" s="35"/>
+      <c r="CO19" s="35"/>
+      <c r="CP19" s="35"/>
+      <c r="CQ19" s="35"/>
+      <c r="CR19" s="35"/>
+      <c r="CS19" s="35"/>
+      <c r="CT19" s="35"/>
+      <c r="CU19" s="35"/>
+      <c r="CV19" s="35"/>
+      <c r="CW19" s="35"/>
+      <c r="CX19" s="35"/>
+      <c r="CY19" s="35"/>
+      <c r="CZ19" s="35"/>
+      <c r="DA19" s="35"/>
+      <c r="DB19" s="35"/>
+      <c r="DC19" s="35"/>
+      <c r="DD19" s="35"/>
+      <c r="DE19" s="35"/>
+      <c r="DF19" s="35"/>
+      <c r="DG19" s="35"/>
+      <c r="DH19" s="35"/>
+      <c r="DI19" s="35"/>
+      <c r="DJ19" s="35"/>
+      <c r="DK19" s="35"/>
+      <c r="DL19" s="35"/>
+      <c r="DM19" s="35"/>
+      <c r="DN19" s="35"/>
+      <c r="DO19" s="35"/>
+      <c r="DP19" s="35"/>
+      <c r="DQ19" s="35"/>
+      <c r="DR19" s="35"/>
+      <c r="DS19" s="35"/>
+      <c r="DT19" s="35"/>
+      <c r="DU19" s="35"/>
+      <c r="DV19" s="35"/>
+      <c r="DW19" s="35"/>
+      <c r="DX19" s="35"/>
+      <c r="DY19" s="35"/>
+      <c r="DZ19" s="35"/>
+      <c r="EA19" s="35"/>
+      <c r="EB19" s="35"/>
+      <c r="EC19" s="35"/>
+      <c r="ED19" s="35"/>
+      <c r="EE19" s="35"/>
+      <c r="EF19" s="35"/>
+      <c r="EG19" s="35"/>
+      <c r="EH19" s="35"/>
+      <c r="EI19" s="35"/>
+      <c r="EJ19" s="35"/>
+      <c r="EK19" s="35"/>
+      <c r="EL19" s="35"/>
+      <c r="EM19" s="35"/>
+      <c r="EN19" s="35"/>
+      <c r="EO19" s="35"/>
+      <c r="EP19" s="35"/>
+      <c r="EQ19" s="35"/>
+      <c r="ER19" s="35"/>
+      <c r="ES19" s="35"/>
+      <c r="ET19" s="35"/>
+      <c r="EU19" s="35"/>
+      <c r="EV19" s="35"/>
+      <c r="EW19" s="35"/>
+      <c r="EX19" s="35"/>
+      <c r="EY19" s="35"/>
+      <c r="EZ19" s="35"/>
+      <c r="FA19" s="35"/>
+      <c r="FB19" s="35"/>
+      <c r="FC19" s="35"/>
+      <c r="FD19" s="35"/>
+      <c r="FE19" s="35"/>
+      <c r="FF19" s="35"/>
+      <c r="FG19" s="35"/>
+      <c r="FH19" s="35"/>
+      <c r="FI19" s="35"/>
+      <c r="FJ19" s="35"/>
+      <c r="FK19" s="35"/>
+      <c r="FL19" s="35"/>
+      <c r="FM19" s="35"/>
+      <c r="FN19" s="35"/>
+      <c r="FO19" s="35"/>
+      <c r="FP19" s="35"/>
+      <c r="FQ19" s="35"/>
+      <c r="FR19" s="35"/>
+      <c r="FS19" s="35"/>
+      <c r="FT19" s="35"/>
+      <c r="FU19" s="35"/>
+      <c r="FV19" s="35"/>
+      <c r="FW19" s="35"/>
+      <c r="FX19" s="35"/>
+      <c r="FY19" s="35"/>
+      <c r="FZ19" s="35"/>
+      <c r="GA19" s="35"/>
+      <c r="GB19" s="35"/>
+      <c r="GC19" s="35"/>
+      <c r="GD19" s="35"/>
+      <c r="GE19" s="35"/>
+      <c r="GF19" s="35"/>
+      <c r="GG19" s="35"/>
+      <c r="GH19" s="35"/>
+      <c r="GI19" s="35"/>
+      <c r="GJ19" s="35"/>
+      <c r="GK19" s="35"/>
+      <c r="GL19" s="35"/>
+      <c r="GM19" s="35"/>
+      <c r="GN19" s="35"/>
+      <c r="GO19" s="35"/>
+      <c r="GP19" s="35"/>
+      <c r="GQ19" s="35"/>
+      <c r="GR19" s="35"/>
+      <c r="GS19" s="35"/>
+      <c r="GT19" s="35"/>
+      <c r="GU19" s="35"/>
+      <c r="GV19" s="35"/>
+      <c r="GW19" s="35"/>
+      <c r="GX19" s="35"/>
+      <c r="GY19" s="35"/>
+      <c r="GZ19" s="35"/>
+      <c r="HA19" s="35"/>
+      <c r="HB19" s="35"/>
+      <c r="HC19" s="35"/>
+      <c r="HD19" s="35"/>
+      <c r="HE19" s="35"/>
+      <c r="HF19" s="35"/>
+      <c r="HG19" s="35"/>
+      <c r="HH19" s="35"/>
+      <c r="HI19" s="35"/>
+      <c r="HJ19" s="35"/>
+      <c r="HK19" s="35"/>
+      <c r="HL19" s="35"/>
+      <c r="HM19" s="35"/>
+      <c r="HN19" s="35"/>
+      <c r="HO19" s="35"/>
+      <c r="HP19" s="35"/>
+      <c r="HQ19" s="35"/>
+      <c r="HR19" s="35"/>
+      <c r="HS19" s="35"/>
+      <c r="HT19" s="35"/>
+      <c r="HU19" s="35"/>
+      <c r="HV19" s="35"/>
+      <c r="HW19" s="35"/>
+      <c r="HX19" s="35"/>
+      <c r="HY19" s="35"/>
+      <c r="HZ19" s="35"/>
+      <c r="IA19" s="35"/>
+      <c r="IB19" s="35"/>
+      <c r="IC19" s="35"/>
+      <c r="ID19" s="35"/>
+      <c r="IE19" s="35"/>
+      <c r="IF19" s="35"/>
+      <c r="IG19" s="35"/>
+      <c r="IH19" s="35"/>
+      <c r="II19" s="35"/>
+      <c r="IJ19" s="35"/>
+      <c r="IK19" s="35"/>
+      <c r="IL19" s="35"/>
+      <c r="IM19" s="35"/>
+      <c r="IN19" s="35"/>
+      <c r="IO19" s="35"/>
+      <c r="IP19" s="35"/>
+      <c r="IQ19" s="35"/>
+      <c r="IR19" s="35"/>
+      <c r="IS19" s="35"/>
+      <c r="IT19" s="35"/>
+      <c r="IU19" s="35"/>
+      <c r="IV19" s="35"/>
+      <c r="IW19" s="35"/>
+      <c r="IX19" s="35"/>
     </row>
     <row r="20" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="50"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
@@ -6732,278 +6766,278 @@
       <c r="IW20" s="12"/>
       <c r="IX20" s="12"/>
     </row>
-    <row r="21" spans="1:258" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="35"/>
-      <c r="AF21" s="35"/>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="35"/>
-      <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
-      <c r="AR21" s="35"/>
-      <c r="AS21" s="35"/>
-      <c r="AT21" s="35"/>
-      <c r="AU21" s="35"/>
-      <c r="AV21" s="35"/>
-      <c r="AW21" s="35"/>
-      <c r="AX21" s="35"/>
-      <c r="AY21" s="35"/>
-      <c r="AZ21" s="35"/>
-      <c r="BA21" s="35"/>
-      <c r="BB21" s="35"/>
-      <c r="BC21" s="35"/>
-      <c r="BD21" s="35"/>
-      <c r="BE21" s="35"/>
-      <c r="BF21" s="35"/>
-      <c r="BG21" s="35"/>
-      <c r="BH21" s="35"/>
-      <c r="BI21" s="35"/>
-      <c r="BJ21" s="35"/>
-      <c r="BK21" s="35"/>
-      <c r="BL21" s="35"/>
-      <c r="BM21" s="35"/>
-      <c r="BN21" s="35"/>
-      <c r="BO21" s="35"/>
-      <c r="BP21" s="35"/>
-      <c r="BQ21" s="35"/>
-      <c r="BR21" s="35"/>
-      <c r="BS21" s="35"/>
-      <c r="BT21" s="35"/>
-      <c r="BU21" s="35"/>
-      <c r="BV21" s="35"/>
-      <c r="BW21" s="35"/>
-      <c r="BX21" s="35"/>
-      <c r="BY21" s="35"/>
-      <c r="BZ21" s="35"/>
-      <c r="CA21" s="35"/>
-      <c r="CB21" s="35"/>
-      <c r="CC21" s="35"/>
-      <c r="CD21" s="35"/>
-      <c r="CE21" s="35"/>
-      <c r="CF21" s="35"/>
-      <c r="CG21" s="35"/>
-      <c r="CH21" s="35"/>
-      <c r="CI21" s="35"/>
-      <c r="CJ21" s="35"/>
-      <c r="CK21" s="35"/>
-      <c r="CL21" s="35"/>
-      <c r="CM21" s="35"/>
-      <c r="CN21" s="35"/>
-      <c r="CO21" s="35"/>
-      <c r="CP21" s="35"/>
-      <c r="CQ21" s="35"/>
-      <c r="CR21" s="35"/>
-      <c r="CS21" s="35"/>
-      <c r="CT21" s="35"/>
-      <c r="CU21" s="35"/>
-      <c r="CV21" s="35"/>
-      <c r="CW21" s="35"/>
-      <c r="CX21" s="35"/>
-      <c r="CY21" s="35"/>
-      <c r="CZ21" s="35"/>
-      <c r="DA21" s="35"/>
-      <c r="DB21" s="35"/>
-      <c r="DC21" s="35"/>
-      <c r="DD21" s="35"/>
-      <c r="DE21" s="35"/>
-      <c r="DF21" s="35"/>
-      <c r="DG21" s="35"/>
-      <c r="DH21" s="35"/>
-      <c r="DI21" s="35"/>
-      <c r="DJ21" s="35"/>
-      <c r="DK21" s="35"/>
-      <c r="DL21" s="35"/>
-      <c r="DM21" s="35"/>
-      <c r="DN21" s="35"/>
-      <c r="DO21" s="35"/>
-      <c r="DP21" s="35"/>
-      <c r="DQ21" s="35"/>
-      <c r="DR21" s="35"/>
-      <c r="DS21" s="35"/>
-      <c r="DT21" s="35"/>
-      <c r="DU21" s="35"/>
-      <c r="DV21" s="35"/>
-      <c r="DW21" s="35"/>
-      <c r="DX21" s="35"/>
-      <c r="DY21" s="35"/>
-      <c r="DZ21" s="35"/>
-      <c r="EA21" s="35"/>
-      <c r="EB21" s="35"/>
-      <c r="EC21" s="35"/>
-      <c r="ED21" s="35"/>
-      <c r="EE21" s="35"/>
-      <c r="EF21" s="35"/>
-      <c r="EG21" s="35"/>
-      <c r="EH21" s="35"/>
-      <c r="EI21" s="35"/>
-      <c r="EJ21" s="35"/>
-      <c r="EK21" s="35"/>
-      <c r="EL21" s="35"/>
-      <c r="EM21" s="35"/>
-      <c r="EN21" s="35"/>
-      <c r="EO21" s="35"/>
-      <c r="EP21" s="35"/>
-      <c r="EQ21" s="35"/>
-      <c r="ER21" s="35"/>
-      <c r="ES21" s="35"/>
-      <c r="ET21" s="35"/>
-      <c r="EU21" s="35"/>
-      <c r="EV21" s="35"/>
-      <c r="EW21" s="35"/>
-      <c r="EX21" s="35"/>
-      <c r="EY21" s="35"/>
-      <c r="EZ21" s="35"/>
-      <c r="FA21" s="35"/>
-      <c r="FB21" s="35"/>
-      <c r="FC21" s="35"/>
-      <c r="FD21" s="35"/>
-      <c r="FE21" s="35"/>
-      <c r="FF21" s="35"/>
-      <c r="FG21" s="35"/>
-      <c r="FH21" s="35"/>
-      <c r="FI21" s="35"/>
-      <c r="FJ21" s="35"/>
-      <c r="FK21" s="35"/>
-      <c r="FL21" s="35"/>
-      <c r="FM21" s="35"/>
-      <c r="FN21" s="35"/>
-      <c r="FO21" s="35"/>
-      <c r="FP21" s="35"/>
-      <c r="FQ21" s="35"/>
-      <c r="FR21" s="35"/>
-      <c r="FS21" s="35"/>
-      <c r="FT21" s="35"/>
-      <c r="FU21" s="35"/>
-      <c r="FV21" s="35"/>
-      <c r="FW21" s="35"/>
-      <c r="FX21" s="35"/>
-      <c r="FY21" s="35"/>
-      <c r="FZ21" s="35"/>
-      <c r="GA21" s="35"/>
-      <c r="GB21" s="35"/>
-      <c r="GC21" s="35"/>
-      <c r="GD21" s="35"/>
-      <c r="GE21" s="35"/>
-      <c r="GF21" s="35"/>
-      <c r="GG21" s="35"/>
-      <c r="GH21" s="35"/>
-      <c r="GI21" s="35"/>
-      <c r="GJ21" s="35"/>
-      <c r="GK21" s="35"/>
-      <c r="GL21" s="35"/>
-      <c r="GM21" s="35"/>
-      <c r="GN21" s="35"/>
-      <c r="GO21" s="35"/>
-      <c r="GP21" s="35"/>
-      <c r="GQ21" s="35"/>
-      <c r="GR21" s="35"/>
-      <c r="GS21" s="35"/>
-      <c r="GT21" s="35"/>
-      <c r="GU21" s="35"/>
-      <c r="GV21" s="35"/>
-      <c r="GW21" s="35"/>
-      <c r="GX21" s="35"/>
-      <c r="GY21" s="35"/>
-      <c r="GZ21" s="35"/>
-      <c r="HA21" s="35"/>
-      <c r="HB21" s="35"/>
-      <c r="HC21" s="35"/>
-      <c r="HD21" s="35"/>
-      <c r="HE21" s="35"/>
-      <c r="HF21" s="35"/>
-      <c r="HG21" s="35"/>
-      <c r="HH21" s="35"/>
-      <c r="HI21" s="35"/>
-      <c r="HJ21" s="35"/>
-      <c r="HK21" s="35"/>
-      <c r="HL21" s="35"/>
-      <c r="HM21" s="35"/>
-      <c r="HN21" s="35"/>
-      <c r="HO21" s="35"/>
-      <c r="HP21" s="35"/>
-      <c r="HQ21" s="35"/>
-      <c r="HR21" s="35"/>
-      <c r="HS21" s="35"/>
-      <c r="HT21" s="35"/>
-      <c r="HU21" s="35"/>
-      <c r="HV21" s="35"/>
-      <c r="HW21" s="35"/>
-      <c r="HX21" s="35"/>
-      <c r="HY21" s="35"/>
-      <c r="HZ21" s="35"/>
-      <c r="IA21" s="35"/>
-      <c r="IB21" s="35"/>
-      <c r="IC21" s="35"/>
-      <c r="ID21" s="35"/>
-      <c r="IE21" s="35"/>
-      <c r="IF21" s="35"/>
-      <c r="IG21" s="35"/>
-      <c r="IH21" s="35"/>
-      <c r="II21" s="35"/>
-      <c r="IJ21" s="35"/>
-      <c r="IK21" s="35"/>
-      <c r="IL21" s="35"/>
-      <c r="IM21" s="35"/>
-      <c r="IN21" s="35"/>
-      <c r="IO21" s="35"/>
-      <c r="IP21" s="35"/>
-      <c r="IQ21" s="35"/>
-      <c r="IR21" s="35"/>
-      <c r="IS21" s="35"/>
-      <c r="IT21" s="35"/>
-      <c r="IU21" s="35"/>
-      <c r="IV21" s="35"/>
-      <c r="IW21" s="35"/>
-      <c r="IX21" s="35"/>
+    <row r="21" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="63"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="12"/>
+      <c r="AC21" s="12"/>
+      <c r="AD21" s="12"/>
+      <c r="AE21" s="12"/>
+      <c r="AF21" s="12"/>
+      <c r="AG21" s="12"/>
+      <c r="AH21" s="12"/>
+      <c r="AI21" s="12"/>
+      <c r="AJ21" s="12"/>
+      <c r="AK21" s="12"/>
+      <c r="AL21" s="12"/>
+      <c r="AM21" s="12"/>
+      <c r="AN21" s="12"/>
+      <c r="AO21" s="12"/>
+      <c r="AP21" s="12"/>
+      <c r="AQ21" s="12"/>
+      <c r="AR21" s="12"/>
+      <c r="AS21" s="12"/>
+      <c r="AT21" s="12"/>
+      <c r="AU21" s="12"/>
+      <c r="AV21" s="12"/>
+      <c r="AW21" s="12"/>
+      <c r="AX21" s="12"/>
+      <c r="AY21" s="12"/>
+      <c r="AZ21" s="12"/>
+      <c r="BA21" s="12"/>
+      <c r="BB21" s="12"/>
+      <c r="BC21" s="12"/>
+      <c r="BD21" s="12"/>
+      <c r="BE21" s="12"/>
+      <c r="BF21" s="12"/>
+      <c r="BG21" s="12"/>
+      <c r="BH21" s="12"/>
+      <c r="BI21" s="12"/>
+      <c r="BJ21" s="12"/>
+      <c r="BK21" s="12"/>
+      <c r="BL21" s="12"/>
+      <c r="BM21" s="12"/>
+      <c r="BN21" s="12"/>
+      <c r="BO21" s="12"/>
+      <c r="BP21" s="12"/>
+      <c r="BQ21" s="12"/>
+      <c r="BR21" s="12"/>
+      <c r="BS21" s="12"/>
+      <c r="BT21" s="12"/>
+      <c r="BU21" s="12"/>
+      <c r="BV21" s="12"/>
+      <c r="BW21" s="12"/>
+      <c r="BX21" s="12"/>
+      <c r="BY21" s="12"/>
+      <c r="BZ21" s="12"/>
+      <c r="CA21" s="12"/>
+      <c r="CB21" s="12"/>
+      <c r="CC21" s="12"/>
+      <c r="CD21" s="12"/>
+      <c r="CE21" s="12"/>
+      <c r="CF21" s="12"/>
+      <c r="CG21" s="12"/>
+      <c r="CH21" s="12"/>
+      <c r="CI21" s="12"/>
+      <c r="CJ21" s="12"/>
+      <c r="CK21" s="12"/>
+      <c r="CL21" s="12"/>
+      <c r="CM21" s="12"/>
+      <c r="CN21" s="12"/>
+      <c r="CO21" s="12"/>
+      <c r="CP21" s="12"/>
+      <c r="CQ21" s="12"/>
+      <c r="CR21" s="12"/>
+      <c r="CS21" s="12"/>
+      <c r="CT21" s="12"/>
+      <c r="CU21" s="12"/>
+      <c r="CV21" s="12"/>
+      <c r="CW21" s="12"/>
+      <c r="CX21" s="12"/>
+      <c r="CY21" s="12"/>
+      <c r="CZ21" s="12"/>
+      <c r="DA21" s="12"/>
+      <c r="DB21" s="12"/>
+      <c r="DC21" s="12"/>
+      <c r="DD21" s="12"/>
+      <c r="DE21" s="12"/>
+      <c r="DF21" s="12"/>
+      <c r="DG21" s="12"/>
+      <c r="DH21" s="12"/>
+      <c r="DI21" s="12"/>
+      <c r="DJ21" s="12"/>
+      <c r="DK21" s="12"/>
+      <c r="DL21" s="12"/>
+      <c r="DM21" s="12"/>
+      <c r="DN21" s="12"/>
+      <c r="DO21" s="12"/>
+      <c r="DP21" s="12"/>
+      <c r="DQ21" s="12"/>
+      <c r="DR21" s="12"/>
+      <c r="DS21" s="12"/>
+      <c r="DT21" s="12"/>
+      <c r="DU21" s="12"/>
+      <c r="DV21" s="12"/>
+      <c r="DW21" s="12"/>
+      <c r="DX21" s="12"/>
+      <c r="DY21" s="12"/>
+      <c r="DZ21" s="12"/>
+      <c r="EA21" s="12"/>
+      <c r="EB21" s="12"/>
+      <c r="EC21" s="12"/>
+      <c r="ED21" s="12"/>
+      <c r="EE21" s="12"/>
+      <c r="EF21" s="12"/>
+      <c r="EG21" s="12"/>
+      <c r="EH21" s="12"/>
+      <c r="EI21" s="12"/>
+      <c r="EJ21" s="12"/>
+      <c r="EK21" s="12"/>
+      <c r="EL21" s="12"/>
+      <c r="EM21" s="12"/>
+      <c r="EN21" s="12"/>
+      <c r="EO21" s="12"/>
+      <c r="EP21" s="12"/>
+      <c r="EQ21" s="12"/>
+      <c r="ER21" s="12"/>
+      <c r="ES21" s="12"/>
+      <c r="ET21" s="12"/>
+      <c r="EU21" s="12"/>
+      <c r="EV21" s="12"/>
+      <c r="EW21" s="12"/>
+      <c r="EX21" s="12"/>
+      <c r="EY21" s="12"/>
+      <c r="EZ21" s="12"/>
+      <c r="FA21" s="12"/>
+      <c r="FB21" s="12"/>
+      <c r="FC21" s="12"/>
+      <c r="FD21" s="12"/>
+      <c r="FE21" s="12"/>
+      <c r="FF21" s="12"/>
+      <c r="FG21" s="12"/>
+      <c r="FH21" s="12"/>
+      <c r="FI21" s="12"/>
+      <c r="FJ21" s="12"/>
+      <c r="FK21" s="12"/>
+      <c r="FL21" s="12"/>
+      <c r="FM21" s="12"/>
+      <c r="FN21" s="12"/>
+      <c r="FO21" s="12"/>
+      <c r="FP21" s="12"/>
+      <c r="FQ21" s="12"/>
+      <c r="FR21" s="12"/>
+      <c r="FS21" s="12"/>
+      <c r="FT21" s="12"/>
+      <c r="FU21" s="12"/>
+      <c r="FV21" s="12"/>
+      <c r="FW21" s="12"/>
+      <c r="FX21" s="12"/>
+      <c r="FY21" s="12"/>
+      <c r="FZ21" s="12"/>
+      <c r="GA21" s="12"/>
+      <c r="GB21" s="12"/>
+      <c r="GC21" s="12"/>
+      <c r="GD21" s="12"/>
+      <c r="GE21" s="12"/>
+      <c r="GF21" s="12"/>
+      <c r="GG21" s="12"/>
+      <c r="GH21" s="12"/>
+      <c r="GI21" s="12"/>
+      <c r="GJ21" s="12"/>
+      <c r="GK21" s="12"/>
+      <c r="GL21" s="12"/>
+      <c r="GM21" s="12"/>
+      <c r="GN21" s="12"/>
+      <c r="GO21" s="12"/>
+      <c r="GP21" s="12"/>
+      <c r="GQ21" s="12"/>
+      <c r="GR21" s="12"/>
+      <c r="GS21" s="12"/>
+      <c r="GT21" s="12"/>
+      <c r="GU21" s="12"/>
+      <c r="GV21" s="12"/>
+      <c r="GW21" s="12"/>
+      <c r="GX21" s="12"/>
+      <c r="GY21" s="12"/>
+      <c r="GZ21" s="12"/>
+      <c r="HA21" s="12"/>
+      <c r="HB21" s="12"/>
+      <c r="HC21" s="12"/>
+      <c r="HD21" s="12"/>
+      <c r="HE21" s="12"/>
+      <c r="HF21" s="12"/>
+      <c r="HG21" s="12"/>
+      <c r="HH21" s="12"/>
+      <c r="HI21" s="12"/>
+      <c r="HJ21" s="12"/>
+      <c r="HK21" s="12"/>
+      <c r="HL21" s="12"/>
+      <c r="HM21" s="12"/>
+      <c r="HN21" s="12"/>
+      <c r="HO21" s="12"/>
+      <c r="HP21" s="12"/>
+      <c r="HQ21" s="12"/>
+      <c r="HR21" s="12"/>
+      <c r="HS21" s="12"/>
+      <c r="HT21" s="12"/>
+      <c r="HU21" s="12"/>
+      <c r="HV21" s="12"/>
+      <c r="HW21" s="12"/>
+      <c r="HX21" s="12"/>
+      <c r="HY21" s="12"/>
+      <c r="HZ21" s="12"/>
+      <c r="IA21" s="12"/>
+      <c r="IB21" s="12"/>
+      <c r="IC21" s="12"/>
+      <c r="ID21" s="12"/>
+      <c r="IE21" s="12"/>
+      <c r="IF21" s="12"/>
+      <c r="IG21" s="12"/>
+      <c r="IH21" s="12"/>
+      <c r="II21" s="12"/>
+      <c r="IJ21" s="12"/>
+      <c r="IK21" s="12"/>
+      <c r="IL21" s="12"/>
+      <c r="IM21" s="12"/>
+      <c r="IN21" s="12"/>
+      <c r="IO21" s="12"/>
+      <c r="IP21" s="12"/>
+      <c r="IQ21" s="12"/>
+      <c r="IR21" s="12"/>
+      <c r="IS21" s="12"/>
+      <c r="IT21" s="12"/>
+      <c r="IU21" s="12"/>
+      <c r="IV21" s="12"/>
+      <c r="IW21" s="12"/>
+      <c r="IX21" s="12"/>
     </row>
     <row r="22" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="64"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="30"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="28"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
@@ -7253,7 +7287,7 @@
       <c r="IX22" s="12"/>
     </row>
     <row r="23" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="65"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -7261,9 +7295,9 @@
       <c r="F23" s="9"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="9"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
@@ -7512,648 +7546,1392 @@
       <c r="IW23" s="12"/>
       <c r="IX23" s="12"/>
     </row>
-    <row r="24" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="66"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
+    <row r="24" spans="1:258" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="35"/>
+      <c r="AC24" s="35"/>
+      <c r="AD24" s="35"/>
+      <c r="AE24" s="35"/>
+      <c r="AF24" s="35"/>
+      <c r="AG24" s="35"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+      <c r="AN24" s="35"/>
+      <c r="AO24" s="35"/>
+      <c r="AP24" s="35"/>
+      <c r="AQ24" s="35"/>
+      <c r="AR24" s="35"/>
+      <c r="AS24" s="35"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="35"/>
+      <c r="AV24" s="35"/>
+      <c r="AW24" s="35"/>
+      <c r="AX24" s="35"/>
+      <c r="AY24" s="35"/>
+      <c r="AZ24" s="35"/>
+      <c r="BA24" s="35"/>
+      <c r="BB24" s="35"/>
+      <c r="BC24" s="35"/>
+      <c r="BD24" s="35"/>
+      <c r="BE24" s="35"/>
+      <c r="BF24" s="35"/>
+      <c r="BG24" s="35"/>
+      <c r="BH24" s="35"/>
+      <c r="BI24" s="35"/>
+      <c r="BJ24" s="35"/>
+      <c r="BK24" s="35"/>
+      <c r="BL24" s="35"/>
+      <c r="BM24" s="35"/>
+      <c r="BN24" s="35"/>
+      <c r="BO24" s="35"/>
+      <c r="BP24" s="35"/>
+      <c r="BQ24" s="35"/>
+      <c r="BR24" s="35"/>
+      <c r="BS24" s="35"/>
+      <c r="BT24" s="35"/>
+      <c r="BU24" s="35"/>
+      <c r="BV24" s="35"/>
+      <c r="BW24" s="35"/>
+      <c r="BX24" s="35"/>
+      <c r="BY24" s="35"/>
+      <c r="BZ24" s="35"/>
+      <c r="CA24" s="35"/>
+      <c r="CB24" s="35"/>
+      <c r="CC24" s="35"/>
+      <c r="CD24" s="35"/>
+      <c r="CE24" s="35"/>
+      <c r="CF24" s="35"/>
+      <c r="CG24" s="35"/>
+      <c r="CH24" s="35"/>
+      <c r="CI24" s="35"/>
+      <c r="CJ24" s="35"/>
+      <c r="CK24" s="35"/>
+      <c r="CL24" s="35"/>
+      <c r="CM24" s="35"/>
+      <c r="CN24" s="35"/>
+      <c r="CO24" s="35"/>
+      <c r="CP24" s="35"/>
+      <c r="CQ24" s="35"/>
+      <c r="CR24" s="35"/>
+      <c r="CS24" s="35"/>
+      <c r="CT24" s="35"/>
+      <c r="CU24" s="35"/>
+      <c r="CV24" s="35"/>
+      <c r="CW24" s="35"/>
+      <c r="CX24" s="35"/>
+      <c r="CY24" s="35"/>
+      <c r="CZ24" s="35"/>
+      <c r="DA24" s="35"/>
+      <c r="DB24" s="35"/>
+      <c r="DC24" s="35"/>
+      <c r="DD24" s="35"/>
+      <c r="DE24" s="35"/>
+      <c r="DF24" s="35"/>
+      <c r="DG24" s="35"/>
+      <c r="DH24" s="35"/>
+      <c r="DI24" s="35"/>
+      <c r="DJ24" s="35"/>
+      <c r="DK24" s="35"/>
+      <c r="DL24" s="35"/>
+      <c r="DM24" s="35"/>
+      <c r="DN24" s="35"/>
+      <c r="DO24" s="35"/>
+      <c r="DP24" s="35"/>
+      <c r="DQ24" s="35"/>
+      <c r="DR24" s="35"/>
+      <c r="DS24" s="35"/>
+      <c r="DT24" s="35"/>
+      <c r="DU24" s="35"/>
+      <c r="DV24" s="35"/>
+      <c r="DW24" s="35"/>
+      <c r="DX24" s="35"/>
+      <c r="DY24" s="35"/>
+      <c r="DZ24" s="35"/>
+      <c r="EA24" s="35"/>
+      <c r="EB24" s="35"/>
+      <c r="EC24" s="35"/>
+      <c r="ED24" s="35"/>
+      <c r="EE24" s="35"/>
+      <c r="EF24" s="35"/>
+      <c r="EG24" s="35"/>
+      <c r="EH24" s="35"/>
+      <c r="EI24" s="35"/>
+      <c r="EJ24" s="35"/>
+      <c r="EK24" s="35"/>
+      <c r="EL24" s="35"/>
+      <c r="EM24" s="35"/>
+      <c r="EN24" s="35"/>
+      <c r="EO24" s="35"/>
+      <c r="EP24" s="35"/>
+      <c r="EQ24" s="35"/>
+      <c r="ER24" s="35"/>
+      <c r="ES24" s="35"/>
+      <c r="ET24" s="35"/>
+      <c r="EU24" s="35"/>
+      <c r="EV24" s="35"/>
+      <c r="EW24" s="35"/>
+      <c r="EX24" s="35"/>
+      <c r="EY24" s="35"/>
+      <c r="EZ24" s="35"/>
+      <c r="FA24" s="35"/>
+      <c r="FB24" s="35"/>
+      <c r="FC24" s="35"/>
+      <c r="FD24" s="35"/>
+      <c r="FE24" s="35"/>
+      <c r="FF24" s="35"/>
+      <c r="FG24" s="35"/>
+      <c r="FH24" s="35"/>
+      <c r="FI24" s="35"/>
+      <c r="FJ24" s="35"/>
+      <c r="FK24" s="35"/>
+      <c r="FL24" s="35"/>
+      <c r="FM24" s="35"/>
+      <c r="FN24" s="35"/>
+      <c r="FO24" s="35"/>
+      <c r="FP24" s="35"/>
+      <c r="FQ24" s="35"/>
+      <c r="FR24" s="35"/>
+      <c r="FS24" s="35"/>
+      <c r="FT24" s="35"/>
+      <c r="FU24" s="35"/>
+      <c r="FV24" s="35"/>
+      <c r="FW24" s="35"/>
+      <c r="FX24" s="35"/>
+      <c r="FY24" s="35"/>
+      <c r="FZ24" s="35"/>
+      <c r="GA24" s="35"/>
+      <c r="GB24" s="35"/>
+      <c r="GC24" s="35"/>
+      <c r="GD24" s="35"/>
+      <c r="GE24" s="35"/>
+      <c r="GF24" s="35"/>
+      <c r="GG24" s="35"/>
+      <c r="GH24" s="35"/>
+      <c r="GI24" s="35"/>
+      <c r="GJ24" s="35"/>
+      <c r="GK24" s="35"/>
+      <c r="GL24" s="35"/>
+      <c r="GM24" s="35"/>
+      <c r="GN24" s="35"/>
+      <c r="GO24" s="35"/>
+      <c r="GP24" s="35"/>
+      <c r="GQ24" s="35"/>
+      <c r="GR24" s="35"/>
+      <c r="GS24" s="35"/>
+      <c r="GT24" s="35"/>
+      <c r="GU24" s="35"/>
+      <c r="GV24" s="35"/>
+      <c r="GW24" s="35"/>
+      <c r="GX24" s="35"/>
+      <c r="GY24" s="35"/>
+      <c r="GZ24" s="35"/>
+      <c r="HA24" s="35"/>
+      <c r="HB24" s="35"/>
+      <c r="HC24" s="35"/>
+      <c r="HD24" s="35"/>
+      <c r="HE24" s="35"/>
+      <c r="HF24" s="35"/>
+      <c r="HG24" s="35"/>
+      <c r="HH24" s="35"/>
+      <c r="HI24" s="35"/>
+      <c r="HJ24" s="35"/>
+      <c r="HK24" s="35"/>
+      <c r="HL24" s="35"/>
+      <c r="HM24" s="35"/>
+      <c r="HN24" s="35"/>
+      <c r="HO24" s="35"/>
+      <c r="HP24" s="35"/>
+      <c r="HQ24" s="35"/>
+      <c r="HR24" s="35"/>
+      <c r="HS24" s="35"/>
+      <c r="HT24" s="35"/>
+      <c r="HU24" s="35"/>
+      <c r="HV24" s="35"/>
+      <c r="HW24" s="35"/>
+      <c r="HX24" s="35"/>
+      <c r="HY24" s="35"/>
+      <c r="HZ24" s="35"/>
+      <c r="IA24" s="35"/>
+      <c r="IB24" s="35"/>
+      <c r="IC24" s="35"/>
+      <c r="ID24" s="35"/>
+      <c r="IE24" s="35"/>
+      <c r="IF24" s="35"/>
+      <c r="IG24" s="35"/>
+      <c r="IH24" s="35"/>
+      <c r="II24" s="35"/>
+      <c r="IJ24" s="35"/>
+      <c r="IK24" s="35"/>
+      <c r="IL24" s="35"/>
+      <c r="IM24" s="35"/>
+      <c r="IN24" s="35"/>
+      <c r="IO24" s="35"/>
+      <c r="IP24" s="35"/>
+      <c r="IQ24" s="35"/>
+      <c r="IR24" s="35"/>
+      <c r="IS24" s="35"/>
+      <c r="IT24" s="35"/>
+      <c r="IU24" s="35"/>
+      <c r="IV24" s="35"/>
+      <c r="IW24" s="35"/>
+      <c r="IX24" s="35"/>
     </row>
-    <row r="25" spans="1:258" s="48" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="46"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="46"/>
-      <c r="AB25" s="46"/>
-      <c r="AC25" s="46"/>
-      <c r="AD25" s="46"/>
-      <c r="AE25" s="46"/>
-      <c r="AF25" s="46"/>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="46"/>
-      <c r="AK25" s="46"/>
-      <c r="AL25" s="46"/>
-      <c r="AM25" s="46"/>
-      <c r="AN25" s="46"/>
-      <c r="AO25" s="46"/>
-      <c r="AP25" s="46"/>
-      <c r="AQ25" s="46"/>
-      <c r="AR25" s="46"/>
-      <c r="AS25" s="46"/>
-      <c r="AT25" s="46"/>
-      <c r="AU25" s="46"/>
-      <c r="AV25" s="46"/>
-      <c r="AW25" s="46"/>
-      <c r="AX25" s="46"/>
-      <c r="AY25" s="46"/>
-      <c r="AZ25" s="46"/>
-      <c r="BA25" s="46"/>
-      <c r="BB25" s="46"/>
-      <c r="BC25" s="46"/>
-      <c r="BD25" s="46"/>
-      <c r="BE25" s="46"/>
-      <c r="BF25" s="46"/>
-      <c r="BG25" s="46"/>
-      <c r="BH25" s="46"/>
-      <c r="BI25" s="46"/>
-      <c r="BJ25" s="46"/>
-      <c r="BK25" s="46"/>
-      <c r="BL25" s="46"/>
-      <c r="BM25" s="46"/>
-      <c r="BN25" s="46"/>
-      <c r="BO25" s="46"/>
-      <c r="BP25" s="46"/>
-      <c r="BQ25" s="46"/>
-      <c r="BR25" s="46"/>
-      <c r="BS25" s="46"/>
-      <c r="BT25" s="46"/>
-      <c r="BU25" s="46"/>
-      <c r="BV25" s="46"/>
-      <c r="BW25" s="46"/>
-      <c r="BX25" s="46"/>
-      <c r="BY25" s="46"/>
-      <c r="BZ25" s="46"/>
-      <c r="CA25" s="46"/>
-      <c r="CB25" s="46"/>
-      <c r="CC25" s="46"/>
-      <c r="CD25" s="46"/>
-      <c r="CE25" s="46"/>
-      <c r="CF25" s="46"/>
-      <c r="CG25" s="46"/>
-      <c r="CH25" s="46"/>
-      <c r="CI25" s="46"/>
-      <c r="CJ25" s="46"/>
-      <c r="CK25" s="46"/>
-      <c r="CL25" s="46"/>
-      <c r="CM25" s="46"/>
-      <c r="CN25" s="46"/>
-      <c r="CO25" s="46"/>
-      <c r="CP25" s="46"/>
-      <c r="CQ25" s="46"/>
-      <c r="CR25" s="46"/>
-      <c r="CS25" s="46"/>
-      <c r="CT25" s="46"/>
-      <c r="CU25" s="46"/>
-      <c r="CV25" s="46"/>
-      <c r="CW25" s="46"/>
-      <c r="CX25" s="46"/>
-      <c r="CY25" s="46"/>
-      <c r="CZ25" s="46"/>
-      <c r="DA25" s="46"/>
-      <c r="DB25" s="46"/>
-      <c r="DC25" s="46"/>
-      <c r="DD25" s="46"/>
-      <c r="DE25" s="46"/>
-      <c r="DF25" s="46"/>
-      <c r="DG25" s="46"/>
-      <c r="DH25" s="46"/>
-      <c r="DI25" s="46"/>
-      <c r="DJ25" s="46"/>
-      <c r="DK25" s="46"/>
-      <c r="DL25" s="46"/>
-      <c r="DM25" s="46"/>
-      <c r="DN25" s="46"/>
-      <c r="DO25" s="46"/>
-      <c r="DP25" s="46"/>
-      <c r="DQ25" s="46"/>
-      <c r="DR25" s="46"/>
-      <c r="DS25" s="46"/>
-      <c r="DT25" s="46"/>
-      <c r="DU25" s="46"/>
-      <c r="DV25" s="46"/>
-      <c r="DW25" s="46"/>
-      <c r="DX25" s="46"/>
-      <c r="DY25" s="46"/>
-      <c r="DZ25" s="46"/>
-      <c r="EA25" s="46"/>
-      <c r="EB25" s="46"/>
-      <c r="EC25" s="46"/>
-      <c r="ED25" s="46"/>
-      <c r="EE25" s="46"/>
-      <c r="EF25" s="46"/>
-      <c r="EG25" s="46"/>
-      <c r="EH25" s="46"/>
-      <c r="EI25" s="46"/>
-      <c r="EJ25" s="46"/>
-      <c r="EK25" s="46"/>
-      <c r="EL25" s="46"/>
-      <c r="EM25" s="46"/>
-      <c r="EN25" s="46"/>
-      <c r="EO25" s="46"/>
-      <c r="EP25" s="46"/>
-      <c r="EQ25" s="46"/>
-      <c r="ER25" s="46"/>
-      <c r="ES25" s="46"/>
-      <c r="ET25" s="46"/>
-      <c r="EU25" s="46"/>
-      <c r="EV25" s="46"/>
-      <c r="EW25" s="46"/>
-      <c r="EX25" s="46"/>
-      <c r="EY25" s="46"/>
-      <c r="EZ25" s="46"/>
-      <c r="FA25" s="46"/>
-      <c r="FB25" s="46"/>
-      <c r="FC25" s="46"/>
-      <c r="FD25" s="46"/>
-      <c r="FE25" s="46"/>
-      <c r="FF25" s="46"/>
-      <c r="FG25" s="46"/>
-      <c r="FH25" s="46"/>
-      <c r="FI25" s="46"/>
-      <c r="FJ25" s="46"/>
-      <c r="FK25" s="46"/>
-      <c r="FL25" s="46"/>
-      <c r="FM25" s="46"/>
-      <c r="FN25" s="46"/>
-      <c r="FO25" s="46"/>
-      <c r="FP25" s="46"/>
-      <c r="FQ25" s="46"/>
-      <c r="FR25" s="46"/>
-      <c r="FS25" s="46"/>
-      <c r="FT25" s="46"/>
-      <c r="FU25" s="46"/>
-      <c r="FV25" s="46"/>
-      <c r="FW25" s="46"/>
-      <c r="FX25" s="46"/>
-      <c r="FY25" s="46"/>
-      <c r="FZ25" s="46"/>
-      <c r="GA25" s="46"/>
-      <c r="GB25" s="46"/>
-      <c r="GC25" s="46"/>
-      <c r="GD25" s="46"/>
-      <c r="GE25" s="46"/>
-      <c r="GF25" s="46"/>
-      <c r="GG25" s="46"/>
-      <c r="GH25" s="46"/>
-      <c r="GI25" s="46"/>
-      <c r="GJ25" s="46"/>
-      <c r="GK25" s="46"/>
-      <c r="GL25" s="46"/>
-      <c r="GM25" s="46"/>
-      <c r="GN25" s="46"/>
-      <c r="GO25" s="46"/>
-      <c r="GP25" s="46"/>
-      <c r="GQ25" s="46"/>
-      <c r="GR25" s="46"/>
-      <c r="GS25" s="46"/>
-      <c r="GT25" s="46"/>
-      <c r="GU25" s="46"/>
-      <c r="GV25" s="46"/>
-      <c r="GW25" s="46"/>
-      <c r="GX25" s="46"/>
-      <c r="GY25" s="46"/>
-      <c r="GZ25" s="46"/>
-      <c r="HA25" s="46"/>
-      <c r="HB25" s="46"/>
-      <c r="HC25" s="46"/>
-      <c r="HD25" s="46"/>
-      <c r="HE25" s="46"/>
-      <c r="HF25" s="46"/>
-      <c r="HG25" s="46"/>
-      <c r="HH25" s="46"/>
-      <c r="HI25" s="46"/>
-      <c r="HJ25" s="46"/>
-      <c r="HK25" s="46"/>
-      <c r="HL25" s="46"/>
-      <c r="HM25" s="46"/>
-      <c r="HN25" s="46"/>
-      <c r="HO25" s="46"/>
-      <c r="HP25" s="46"/>
-      <c r="HQ25" s="46"/>
-      <c r="HR25" s="46"/>
-      <c r="HS25" s="46"/>
-      <c r="HT25" s="46"/>
-      <c r="HU25" s="46"/>
-      <c r="HV25" s="46"/>
-      <c r="HW25" s="46"/>
-      <c r="HX25" s="46"/>
-      <c r="HY25" s="46"/>
-      <c r="HZ25" s="46"/>
-      <c r="IA25" s="46"/>
-      <c r="IB25" s="46"/>
-      <c r="IC25" s="46"/>
-      <c r="ID25" s="46"/>
-      <c r="IE25" s="46"/>
-      <c r="IF25" s="46"/>
-      <c r="IG25" s="46"/>
-      <c r="IH25" s="46"/>
-      <c r="II25" s="46"/>
-      <c r="IJ25" s="46"/>
-      <c r="IK25" s="46"/>
-      <c r="IL25" s="46"/>
-      <c r="IM25" s="46"/>
-      <c r="IN25" s="46"/>
-      <c r="IO25" s="46"/>
-      <c r="IP25" s="46"/>
-      <c r="IQ25" s="46"/>
-      <c r="IR25" s="46"/>
-      <c r="IS25" s="46"/>
-      <c r="IT25" s="46"/>
-      <c r="IU25" s="46"/>
-      <c r="IV25" s="46"/>
-      <c r="IW25" s="46"/>
-      <c r="IX25" s="46"/>
+    <row r="25" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="64"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AD25" s="12"/>
+      <c r="AE25" s="12"/>
+      <c r="AF25" s="12"/>
+      <c r="AG25" s="12"/>
+      <c r="AH25" s="12"/>
+      <c r="AI25" s="12"/>
+      <c r="AJ25" s="12"/>
+      <c r="AK25" s="12"/>
+      <c r="AL25" s="12"/>
+      <c r="AM25" s="12"/>
+      <c r="AN25" s="12"/>
+      <c r="AO25" s="12"/>
+      <c r="AP25" s="12"/>
+      <c r="AQ25" s="12"/>
+      <c r="AR25" s="12"/>
+      <c r="AS25" s="12"/>
+      <c r="AT25" s="12"/>
+      <c r="AU25" s="12"/>
+      <c r="AV25" s="12"/>
+      <c r="AW25" s="12"/>
+      <c r="AX25" s="12"/>
+      <c r="AY25" s="12"/>
+      <c r="AZ25" s="12"/>
+      <c r="BA25" s="12"/>
+      <c r="BB25" s="12"/>
+      <c r="BC25" s="12"/>
+      <c r="BD25" s="12"/>
+      <c r="BE25" s="12"/>
+      <c r="BF25" s="12"/>
+      <c r="BG25" s="12"/>
+      <c r="BH25" s="12"/>
+      <c r="BI25" s="12"/>
+      <c r="BJ25" s="12"/>
+      <c r="BK25" s="12"/>
+      <c r="BL25" s="12"/>
+      <c r="BM25" s="12"/>
+      <c r="BN25" s="12"/>
+      <c r="BO25" s="12"/>
+      <c r="BP25" s="12"/>
+      <c r="BQ25" s="12"/>
+      <c r="BR25" s="12"/>
+      <c r="BS25" s="12"/>
+      <c r="BT25" s="12"/>
+      <c r="BU25" s="12"/>
+      <c r="BV25" s="12"/>
+      <c r="BW25" s="12"/>
+      <c r="BX25" s="12"/>
+      <c r="BY25" s="12"/>
+      <c r="BZ25" s="12"/>
+      <c r="CA25" s="12"/>
+      <c r="CB25" s="12"/>
+      <c r="CC25" s="12"/>
+      <c r="CD25" s="12"/>
+      <c r="CE25" s="12"/>
+      <c r="CF25" s="12"/>
+      <c r="CG25" s="12"/>
+      <c r="CH25" s="12"/>
+      <c r="CI25" s="12"/>
+      <c r="CJ25" s="12"/>
+      <c r="CK25" s="12"/>
+      <c r="CL25" s="12"/>
+      <c r="CM25" s="12"/>
+      <c r="CN25" s="12"/>
+      <c r="CO25" s="12"/>
+      <c r="CP25" s="12"/>
+      <c r="CQ25" s="12"/>
+      <c r="CR25" s="12"/>
+      <c r="CS25" s="12"/>
+      <c r="CT25" s="12"/>
+      <c r="CU25" s="12"/>
+      <c r="CV25" s="12"/>
+      <c r="CW25" s="12"/>
+      <c r="CX25" s="12"/>
+      <c r="CY25" s="12"/>
+      <c r="CZ25" s="12"/>
+      <c r="DA25" s="12"/>
+      <c r="DB25" s="12"/>
+      <c r="DC25" s="12"/>
+      <c r="DD25" s="12"/>
+      <c r="DE25" s="12"/>
+      <c r="DF25" s="12"/>
+      <c r="DG25" s="12"/>
+      <c r="DH25" s="12"/>
+      <c r="DI25" s="12"/>
+      <c r="DJ25" s="12"/>
+      <c r="DK25" s="12"/>
+      <c r="DL25" s="12"/>
+      <c r="DM25" s="12"/>
+      <c r="DN25" s="12"/>
+      <c r="DO25" s="12"/>
+      <c r="DP25" s="12"/>
+      <c r="DQ25" s="12"/>
+      <c r="DR25" s="12"/>
+      <c r="DS25" s="12"/>
+      <c r="DT25" s="12"/>
+      <c r="DU25" s="12"/>
+      <c r="DV25" s="12"/>
+      <c r="DW25" s="12"/>
+      <c r="DX25" s="12"/>
+      <c r="DY25" s="12"/>
+      <c r="DZ25" s="12"/>
+      <c r="EA25" s="12"/>
+      <c r="EB25" s="12"/>
+      <c r="EC25" s="12"/>
+      <c r="ED25" s="12"/>
+      <c r="EE25" s="12"/>
+      <c r="EF25" s="12"/>
+      <c r="EG25" s="12"/>
+      <c r="EH25" s="12"/>
+      <c r="EI25" s="12"/>
+      <c r="EJ25" s="12"/>
+      <c r="EK25" s="12"/>
+      <c r="EL25" s="12"/>
+      <c r="EM25" s="12"/>
+      <c r="EN25" s="12"/>
+      <c r="EO25" s="12"/>
+      <c r="EP25" s="12"/>
+      <c r="EQ25" s="12"/>
+      <c r="ER25" s="12"/>
+      <c r="ES25" s="12"/>
+      <c r="ET25" s="12"/>
+      <c r="EU25" s="12"/>
+      <c r="EV25" s="12"/>
+      <c r="EW25" s="12"/>
+      <c r="EX25" s="12"/>
+      <c r="EY25" s="12"/>
+      <c r="EZ25" s="12"/>
+      <c r="FA25" s="12"/>
+      <c r="FB25" s="12"/>
+      <c r="FC25" s="12"/>
+      <c r="FD25" s="12"/>
+      <c r="FE25" s="12"/>
+      <c r="FF25" s="12"/>
+      <c r="FG25" s="12"/>
+      <c r="FH25" s="12"/>
+      <c r="FI25" s="12"/>
+      <c r="FJ25" s="12"/>
+      <c r="FK25" s="12"/>
+      <c r="FL25" s="12"/>
+      <c r="FM25" s="12"/>
+      <c r="FN25" s="12"/>
+      <c r="FO25" s="12"/>
+      <c r="FP25" s="12"/>
+      <c r="FQ25" s="12"/>
+      <c r="FR25" s="12"/>
+      <c r="FS25" s="12"/>
+      <c r="FT25" s="12"/>
+      <c r="FU25" s="12"/>
+      <c r="FV25" s="12"/>
+      <c r="FW25" s="12"/>
+      <c r="FX25" s="12"/>
+      <c r="FY25" s="12"/>
+      <c r="FZ25" s="12"/>
+      <c r="GA25" s="12"/>
+      <c r="GB25" s="12"/>
+      <c r="GC25" s="12"/>
+      <c r="GD25" s="12"/>
+      <c r="GE25" s="12"/>
+      <c r="GF25" s="12"/>
+      <c r="GG25" s="12"/>
+      <c r="GH25" s="12"/>
+      <c r="GI25" s="12"/>
+      <c r="GJ25" s="12"/>
+      <c r="GK25" s="12"/>
+      <c r="GL25" s="12"/>
+      <c r="GM25" s="12"/>
+      <c r="GN25" s="12"/>
+      <c r="GO25" s="12"/>
+      <c r="GP25" s="12"/>
+      <c r="GQ25" s="12"/>
+      <c r="GR25" s="12"/>
+      <c r="GS25" s="12"/>
+      <c r="GT25" s="12"/>
+      <c r="GU25" s="12"/>
+      <c r="GV25" s="12"/>
+      <c r="GW25" s="12"/>
+      <c r="GX25" s="12"/>
+      <c r="GY25" s="12"/>
+      <c r="GZ25" s="12"/>
+      <c r="HA25" s="12"/>
+      <c r="HB25" s="12"/>
+      <c r="HC25" s="12"/>
+      <c r="HD25" s="12"/>
+      <c r="HE25" s="12"/>
+      <c r="HF25" s="12"/>
+      <c r="HG25" s="12"/>
+      <c r="HH25" s="12"/>
+      <c r="HI25" s="12"/>
+      <c r="HJ25" s="12"/>
+      <c r="HK25" s="12"/>
+      <c r="HL25" s="12"/>
+      <c r="HM25" s="12"/>
+      <c r="HN25" s="12"/>
+      <c r="HO25" s="12"/>
+      <c r="HP25" s="12"/>
+      <c r="HQ25" s="12"/>
+      <c r="HR25" s="12"/>
+      <c r="HS25" s="12"/>
+      <c r="HT25" s="12"/>
+      <c r="HU25" s="12"/>
+      <c r="HV25" s="12"/>
+      <c r="HW25" s="12"/>
+      <c r="HX25" s="12"/>
+      <c r="HY25" s="12"/>
+      <c r="HZ25" s="12"/>
+      <c r="IA25" s="12"/>
+      <c r="IB25" s="12"/>
+      <c r="IC25" s="12"/>
+      <c r="ID25" s="12"/>
+      <c r="IE25" s="12"/>
+      <c r="IF25" s="12"/>
+      <c r="IG25" s="12"/>
+      <c r="IH25" s="12"/>
+      <c r="II25" s="12"/>
+      <c r="IJ25" s="12"/>
+      <c r="IK25" s="12"/>
+      <c r="IL25" s="12"/>
+      <c r="IM25" s="12"/>
+      <c r="IN25" s="12"/>
+      <c r="IO25" s="12"/>
+      <c r="IP25" s="12"/>
+      <c r="IQ25" s="12"/>
+      <c r="IR25" s="12"/>
+      <c r="IS25" s="12"/>
+      <c r="IT25" s="12"/>
+      <c r="IU25" s="12"/>
+      <c r="IV25" s="12"/>
+      <c r="IW25" s="12"/>
+      <c r="IX25" s="12"/>
     </row>
-    <row r="26" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="58"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
+    <row r="26" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="65"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AJ26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AL26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="12"/>
+      <c r="AQ26" s="12"/>
+      <c r="AR26" s="12"/>
+      <c r="AS26" s="12"/>
+      <c r="AT26" s="12"/>
+      <c r="AU26" s="12"/>
+      <c r="AV26" s="12"/>
+      <c r="AW26" s="12"/>
+      <c r="AX26" s="12"/>
+      <c r="AY26" s="12"/>
+      <c r="AZ26" s="12"/>
+      <c r="BA26" s="12"/>
+      <c r="BB26" s="12"/>
+      <c r="BC26" s="12"/>
+      <c r="BD26" s="12"/>
+      <c r="BE26" s="12"/>
+      <c r="BF26" s="12"/>
+      <c r="BG26" s="12"/>
+      <c r="BH26" s="12"/>
+      <c r="BI26" s="12"/>
+      <c r="BJ26" s="12"/>
+      <c r="BK26" s="12"/>
+      <c r="BL26" s="12"/>
+      <c r="BM26" s="12"/>
+      <c r="BN26" s="12"/>
+      <c r="BO26" s="12"/>
+      <c r="BP26" s="12"/>
+      <c r="BQ26" s="12"/>
+      <c r="BR26" s="12"/>
+      <c r="BS26" s="12"/>
+      <c r="BT26" s="12"/>
+      <c r="BU26" s="12"/>
+      <c r="BV26" s="12"/>
+      <c r="BW26" s="12"/>
+      <c r="BX26" s="12"/>
+      <c r="BY26" s="12"/>
+      <c r="BZ26" s="12"/>
+      <c r="CA26" s="12"/>
+      <c r="CB26" s="12"/>
+      <c r="CC26" s="12"/>
+      <c r="CD26" s="12"/>
+      <c r="CE26" s="12"/>
+      <c r="CF26" s="12"/>
+      <c r="CG26" s="12"/>
+      <c r="CH26" s="12"/>
+      <c r="CI26" s="12"/>
+      <c r="CJ26" s="12"/>
+      <c r="CK26" s="12"/>
+      <c r="CL26" s="12"/>
+      <c r="CM26" s="12"/>
+      <c r="CN26" s="12"/>
+      <c r="CO26" s="12"/>
+      <c r="CP26" s="12"/>
+      <c r="CQ26" s="12"/>
+      <c r="CR26" s="12"/>
+      <c r="CS26" s="12"/>
+      <c r="CT26" s="12"/>
+      <c r="CU26" s="12"/>
+      <c r="CV26" s="12"/>
+      <c r="CW26" s="12"/>
+      <c r="CX26" s="12"/>
+      <c r="CY26" s="12"/>
+      <c r="CZ26" s="12"/>
+      <c r="DA26" s="12"/>
+      <c r="DB26" s="12"/>
+      <c r="DC26" s="12"/>
+      <c r="DD26" s="12"/>
+      <c r="DE26" s="12"/>
+      <c r="DF26" s="12"/>
+      <c r="DG26" s="12"/>
+      <c r="DH26" s="12"/>
+      <c r="DI26" s="12"/>
+      <c r="DJ26" s="12"/>
+      <c r="DK26" s="12"/>
+      <c r="DL26" s="12"/>
+      <c r="DM26" s="12"/>
+      <c r="DN26" s="12"/>
+      <c r="DO26" s="12"/>
+      <c r="DP26" s="12"/>
+      <c r="DQ26" s="12"/>
+      <c r="DR26" s="12"/>
+      <c r="DS26" s="12"/>
+      <c r="DT26" s="12"/>
+      <c r="DU26" s="12"/>
+      <c r="DV26" s="12"/>
+      <c r="DW26" s="12"/>
+      <c r="DX26" s="12"/>
+      <c r="DY26" s="12"/>
+      <c r="DZ26" s="12"/>
+      <c r="EA26" s="12"/>
+      <c r="EB26" s="12"/>
+      <c r="EC26" s="12"/>
+      <c r="ED26" s="12"/>
+      <c r="EE26" s="12"/>
+      <c r="EF26" s="12"/>
+      <c r="EG26" s="12"/>
+      <c r="EH26" s="12"/>
+      <c r="EI26" s="12"/>
+      <c r="EJ26" s="12"/>
+      <c r="EK26" s="12"/>
+      <c r="EL26" s="12"/>
+      <c r="EM26" s="12"/>
+      <c r="EN26" s="12"/>
+      <c r="EO26" s="12"/>
+      <c r="EP26" s="12"/>
+      <c r="EQ26" s="12"/>
+      <c r="ER26" s="12"/>
+      <c r="ES26" s="12"/>
+      <c r="ET26" s="12"/>
+      <c r="EU26" s="12"/>
+      <c r="EV26" s="12"/>
+      <c r="EW26" s="12"/>
+      <c r="EX26" s="12"/>
+      <c r="EY26" s="12"/>
+      <c r="EZ26" s="12"/>
+      <c r="FA26" s="12"/>
+      <c r="FB26" s="12"/>
+      <c r="FC26" s="12"/>
+      <c r="FD26" s="12"/>
+      <c r="FE26" s="12"/>
+      <c r="FF26" s="12"/>
+      <c r="FG26" s="12"/>
+      <c r="FH26" s="12"/>
+      <c r="FI26" s="12"/>
+      <c r="FJ26" s="12"/>
+      <c r="FK26" s="12"/>
+      <c r="FL26" s="12"/>
+      <c r="FM26" s="12"/>
+      <c r="FN26" s="12"/>
+      <c r="FO26" s="12"/>
+      <c r="FP26" s="12"/>
+      <c r="FQ26" s="12"/>
+      <c r="FR26" s="12"/>
+      <c r="FS26" s="12"/>
+      <c r="FT26" s="12"/>
+      <c r="FU26" s="12"/>
+      <c r="FV26" s="12"/>
+      <c r="FW26" s="12"/>
+      <c r="FX26" s="12"/>
+      <c r="FY26" s="12"/>
+      <c r="FZ26" s="12"/>
+      <c r="GA26" s="12"/>
+      <c r="GB26" s="12"/>
+      <c r="GC26" s="12"/>
+      <c r="GD26" s="12"/>
+      <c r="GE26" s="12"/>
+      <c r="GF26" s="12"/>
+      <c r="GG26" s="12"/>
+      <c r="GH26" s="12"/>
+      <c r="GI26" s="12"/>
+      <c r="GJ26" s="12"/>
+      <c r="GK26" s="12"/>
+      <c r="GL26" s="12"/>
+      <c r="GM26" s="12"/>
+      <c r="GN26" s="12"/>
+      <c r="GO26" s="12"/>
+      <c r="GP26" s="12"/>
+      <c r="GQ26" s="12"/>
+      <c r="GR26" s="12"/>
+      <c r="GS26" s="12"/>
+      <c r="GT26" s="12"/>
+      <c r="GU26" s="12"/>
+      <c r="GV26" s="12"/>
+      <c r="GW26" s="12"/>
+      <c r="GX26" s="12"/>
+      <c r="GY26" s="12"/>
+      <c r="GZ26" s="12"/>
+      <c r="HA26" s="12"/>
+      <c r="HB26" s="12"/>
+      <c r="HC26" s="12"/>
+      <c r="HD26" s="12"/>
+      <c r="HE26" s="12"/>
+      <c r="HF26" s="12"/>
+      <c r="HG26" s="12"/>
+      <c r="HH26" s="12"/>
+      <c r="HI26" s="12"/>
+      <c r="HJ26" s="12"/>
+      <c r="HK26" s="12"/>
+      <c r="HL26" s="12"/>
+      <c r="HM26" s="12"/>
+      <c r="HN26" s="12"/>
+      <c r="HO26" s="12"/>
+      <c r="HP26" s="12"/>
+      <c r="HQ26" s="12"/>
+      <c r="HR26" s="12"/>
+      <c r="HS26" s="12"/>
+      <c r="HT26" s="12"/>
+      <c r="HU26" s="12"/>
+      <c r="HV26" s="12"/>
+      <c r="HW26" s="12"/>
+      <c r="HX26" s="12"/>
+      <c r="HY26" s="12"/>
+      <c r="HZ26" s="12"/>
+      <c r="IA26" s="12"/>
+      <c r="IB26" s="12"/>
+      <c r="IC26" s="12"/>
+      <c r="ID26" s="12"/>
+      <c r="IE26" s="12"/>
+      <c r="IF26" s="12"/>
+      <c r="IG26" s="12"/>
+      <c r="IH26" s="12"/>
+      <c r="II26" s="12"/>
+      <c r="IJ26" s="12"/>
+      <c r="IK26" s="12"/>
+      <c r="IL26" s="12"/>
+      <c r="IM26" s="12"/>
+      <c r="IN26" s="12"/>
+      <c r="IO26" s="12"/>
+      <c r="IP26" s="12"/>
+      <c r="IQ26" s="12"/>
+      <c r="IR26" s="12"/>
+      <c r="IS26" s="12"/>
+      <c r="IT26" s="12"/>
+      <c r="IU26" s="12"/>
+      <c r="IV26" s="12"/>
+      <c r="IW26" s="12"/>
+      <c r="IX26" s="12"/>
     </row>
     <row r="27" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="25"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
     </row>
-    <row r="28" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
+    <row r="28" spans="1:258" s="48" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="46"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="46"/>
+      <c r="Z28" s="46"/>
+      <c r="AA28" s="46"/>
+      <c r="AB28" s="46"/>
+      <c r="AC28" s="46"/>
+      <c r="AD28" s="46"/>
+      <c r="AE28" s="46"/>
+      <c r="AF28" s="46"/>
+      <c r="AG28" s="46"/>
+      <c r="AH28" s="46"/>
+      <c r="AI28" s="46"/>
+      <c r="AJ28" s="46"/>
+      <c r="AK28" s="46"/>
+      <c r="AL28" s="46"/>
+      <c r="AM28" s="46"/>
+      <c r="AN28" s="46"/>
+      <c r="AO28" s="46"/>
+      <c r="AP28" s="46"/>
+      <c r="AQ28" s="46"/>
+      <c r="AR28" s="46"/>
+      <c r="AS28" s="46"/>
+      <c r="AT28" s="46"/>
+      <c r="AU28" s="46"/>
+      <c r="AV28" s="46"/>
+      <c r="AW28" s="46"/>
+      <c r="AX28" s="46"/>
+      <c r="AY28" s="46"/>
+      <c r="AZ28" s="46"/>
+      <c r="BA28" s="46"/>
+      <c r="BB28" s="46"/>
+      <c r="BC28" s="46"/>
+      <c r="BD28" s="46"/>
+      <c r="BE28" s="46"/>
+      <c r="BF28" s="46"/>
+      <c r="BG28" s="46"/>
+      <c r="BH28" s="46"/>
+      <c r="BI28" s="46"/>
+      <c r="BJ28" s="46"/>
+      <c r="BK28" s="46"/>
+      <c r="BL28" s="46"/>
+      <c r="BM28" s="46"/>
+      <c r="BN28" s="46"/>
+      <c r="BO28" s="46"/>
+      <c r="BP28" s="46"/>
+      <c r="BQ28" s="46"/>
+      <c r="BR28" s="46"/>
+      <c r="BS28" s="46"/>
+      <c r="BT28" s="46"/>
+      <c r="BU28" s="46"/>
+      <c r="BV28" s="46"/>
+      <c r="BW28" s="46"/>
+      <c r="BX28" s="46"/>
+      <c r="BY28" s="46"/>
+      <c r="BZ28" s="46"/>
+      <c r="CA28" s="46"/>
+      <c r="CB28" s="46"/>
+      <c r="CC28" s="46"/>
+      <c r="CD28" s="46"/>
+      <c r="CE28" s="46"/>
+      <c r="CF28" s="46"/>
+      <c r="CG28" s="46"/>
+      <c r="CH28" s="46"/>
+      <c r="CI28" s="46"/>
+      <c r="CJ28" s="46"/>
+      <c r="CK28" s="46"/>
+      <c r="CL28" s="46"/>
+      <c r="CM28" s="46"/>
+      <c r="CN28" s="46"/>
+      <c r="CO28" s="46"/>
+      <c r="CP28" s="46"/>
+      <c r="CQ28" s="46"/>
+      <c r="CR28" s="46"/>
+      <c r="CS28" s="46"/>
+      <c r="CT28" s="46"/>
+      <c r="CU28" s="46"/>
+      <c r="CV28" s="46"/>
+      <c r="CW28" s="46"/>
+      <c r="CX28" s="46"/>
+      <c r="CY28" s="46"/>
+      <c r="CZ28" s="46"/>
+      <c r="DA28" s="46"/>
+      <c r="DB28" s="46"/>
+      <c r="DC28" s="46"/>
+      <c r="DD28" s="46"/>
+      <c r="DE28" s="46"/>
+      <c r="DF28" s="46"/>
+      <c r="DG28" s="46"/>
+      <c r="DH28" s="46"/>
+      <c r="DI28" s="46"/>
+      <c r="DJ28" s="46"/>
+      <c r="DK28" s="46"/>
+      <c r="DL28" s="46"/>
+      <c r="DM28" s="46"/>
+      <c r="DN28" s="46"/>
+      <c r="DO28" s="46"/>
+      <c r="DP28" s="46"/>
+      <c r="DQ28" s="46"/>
+      <c r="DR28" s="46"/>
+      <c r="DS28" s="46"/>
+      <c r="DT28" s="46"/>
+      <c r="DU28" s="46"/>
+      <c r="DV28" s="46"/>
+      <c r="DW28" s="46"/>
+      <c r="DX28" s="46"/>
+      <c r="DY28" s="46"/>
+      <c r="DZ28" s="46"/>
+      <c r="EA28" s="46"/>
+      <c r="EB28" s="46"/>
+      <c r="EC28" s="46"/>
+      <c r="ED28" s="46"/>
+      <c r="EE28" s="46"/>
+      <c r="EF28" s="46"/>
+      <c r="EG28" s="46"/>
+      <c r="EH28" s="46"/>
+      <c r="EI28" s="46"/>
+      <c r="EJ28" s="46"/>
+      <c r="EK28" s="46"/>
+      <c r="EL28" s="46"/>
+      <c r="EM28" s="46"/>
+      <c r="EN28" s="46"/>
+      <c r="EO28" s="46"/>
+      <c r="EP28" s="46"/>
+      <c r="EQ28" s="46"/>
+      <c r="ER28" s="46"/>
+      <c r="ES28" s="46"/>
+      <c r="ET28" s="46"/>
+      <c r="EU28" s="46"/>
+      <c r="EV28" s="46"/>
+      <c r="EW28" s="46"/>
+      <c r="EX28" s="46"/>
+      <c r="EY28" s="46"/>
+      <c r="EZ28" s="46"/>
+      <c r="FA28" s="46"/>
+      <c r="FB28" s="46"/>
+      <c r="FC28" s="46"/>
+      <c r="FD28" s="46"/>
+      <c r="FE28" s="46"/>
+      <c r="FF28" s="46"/>
+      <c r="FG28" s="46"/>
+      <c r="FH28" s="46"/>
+      <c r="FI28" s="46"/>
+      <c r="FJ28" s="46"/>
+      <c r="FK28" s="46"/>
+      <c r="FL28" s="46"/>
+      <c r="FM28" s="46"/>
+      <c r="FN28" s="46"/>
+      <c r="FO28" s="46"/>
+      <c r="FP28" s="46"/>
+      <c r="FQ28" s="46"/>
+      <c r="FR28" s="46"/>
+      <c r="FS28" s="46"/>
+      <c r="FT28" s="46"/>
+      <c r="FU28" s="46"/>
+      <c r="FV28" s="46"/>
+      <c r="FW28" s="46"/>
+      <c r="FX28" s="46"/>
+      <c r="FY28" s="46"/>
+      <c r="FZ28" s="46"/>
+      <c r="GA28" s="46"/>
+      <c r="GB28" s="46"/>
+      <c r="GC28" s="46"/>
+      <c r="GD28" s="46"/>
+      <c r="GE28" s="46"/>
+      <c r="GF28" s="46"/>
+      <c r="GG28" s="46"/>
+      <c r="GH28" s="46"/>
+      <c r="GI28" s="46"/>
+      <c r="GJ28" s="46"/>
+      <c r="GK28" s="46"/>
+      <c r="GL28" s="46"/>
+      <c r="GM28" s="46"/>
+      <c r="GN28" s="46"/>
+      <c r="GO28" s="46"/>
+      <c r="GP28" s="46"/>
+      <c r="GQ28" s="46"/>
+      <c r="GR28" s="46"/>
+      <c r="GS28" s="46"/>
+      <c r="GT28" s="46"/>
+      <c r="GU28" s="46"/>
+      <c r="GV28" s="46"/>
+      <c r="GW28" s="46"/>
+      <c r="GX28" s="46"/>
+      <c r="GY28" s="46"/>
+      <c r="GZ28" s="46"/>
+      <c r="HA28" s="46"/>
+      <c r="HB28" s="46"/>
+      <c r="HC28" s="46"/>
+      <c r="HD28" s="46"/>
+      <c r="HE28" s="46"/>
+      <c r="HF28" s="46"/>
+      <c r="HG28" s="46"/>
+      <c r="HH28" s="46"/>
+      <c r="HI28" s="46"/>
+      <c r="HJ28" s="46"/>
+      <c r="HK28" s="46"/>
+      <c r="HL28" s="46"/>
+      <c r="HM28" s="46"/>
+      <c r="HN28" s="46"/>
+      <c r="HO28" s="46"/>
+      <c r="HP28" s="46"/>
+      <c r="HQ28" s="46"/>
+      <c r="HR28" s="46"/>
+      <c r="HS28" s="46"/>
+      <c r="HT28" s="46"/>
+      <c r="HU28" s="46"/>
+      <c r="HV28" s="46"/>
+      <c r="HW28" s="46"/>
+      <c r="HX28" s="46"/>
+      <c r="HY28" s="46"/>
+      <c r="HZ28" s="46"/>
+      <c r="IA28" s="46"/>
+      <c r="IB28" s="46"/>
+      <c r="IC28" s="46"/>
+      <c r="ID28" s="46"/>
+      <c r="IE28" s="46"/>
+      <c r="IF28" s="46"/>
+      <c r="IG28" s="46"/>
+      <c r="IH28" s="46"/>
+      <c r="II28" s="46"/>
+      <c r="IJ28" s="46"/>
+      <c r="IK28" s="46"/>
+      <c r="IL28" s="46"/>
+      <c r="IM28" s="46"/>
+      <c r="IN28" s="46"/>
+      <c r="IO28" s="46"/>
+      <c r="IP28" s="46"/>
+      <c r="IQ28" s="46"/>
+      <c r="IR28" s="46"/>
+      <c r="IS28" s="46"/>
+      <c r="IT28" s="46"/>
+      <c r="IU28" s="46"/>
+      <c r="IV28" s="46"/>
+      <c r="IW28" s="46"/>
+      <c r="IX28" s="46"/>
     </row>
     <row r="29" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="45"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
-    <row r="30" spans="1:258" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="46"/>
-      <c r="V30" s="46"/>
-      <c r="W30" s="46"/>
-      <c r="X30" s="46"/>
-      <c r="Y30" s="46"/>
-      <c r="Z30" s="46"/>
-      <c r="AA30" s="46"/>
-      <c r="AB30" s="46"/>
-      <c r="AC30" s="46"/>
-      <c r="AD30" s="46"/>
-      <c r="AE30" s="46"/>
-      <c r="AF30" s="46"/>
-      <c r="AG30" s="46"/>
-      <c r="AH30" s="46"/>
-      <c r="AI30" s="46"/>
-      <c r="AJ30" s="46"/>
-      <c r="AK30" s="46"/>
-      <c r="AL30" s="46"/>
-      <c r="AM30" s="46"/>
-      <c r="AN30" s="46"/>
-      <c r="AO30" s="46"/>
-      <c r="AP30" s="46"/>
-      <c r="AQ30" s="46"/>
-      <c r="AR30" s="46"/>
-      <c r="AS30" s="46"/>
-      <c r="AT30" s="46"/>
-      <c r="AU30" s="46"/>
-      <c r="AV30" s="46"/>
-      <c r="AW30" s="46"/>
-      <c r="AX30" s="46"/>
-      <c r="AY30" s="46"/>
-      <c r="AZ30" s="46"/>
-      <c r="BA30" s="46"/>
-      <c r="BB30" s="46"/>
-      <c r="BC30" s="46"/>
-      <c r="BD30" s="46"/>
-      <c r="BE30" s="46"/>
-      <c r="BF30" s="46"/>
-      <c r="BG30" s="46"/>
-      <c r="BH30" s="46"/>
-      <c r="BI30" s="46"/>
-      <c r="BJ30" s="46"/>
-      <c r="BK30" s="46"/>
-      <c r="BL30" s="46"/>
-      <c r="BM30" s="46"/>
-      <c r="BN30" s="46"/>
-      <c r="BO30" s="46"/>
-      <c r="BP30" s="46"/>
-      <c r="BQ30" s="46"/>
-      <c r="BR30" s="46"/>
-      <c r="BS30" s="46"/>
-      <c r="BT30" s="46"/>
-      <c r="BU30" s="46"/>
-      <c r="BV30" s="46"/>
-      <c r="BW30" s="46"/>
-      <c r="BX30" s="46"/>
-      <c r="BY30" s="46"/>
-      <c r="BZ30" s="46"/>
-      <c r="CA30" s="46"/>
-      <c r="CB30" s="46"/>
-      <c r="CC30" s="46"/>
-      <c r="CD30" s="46"/>
-      <c r="CE30" s="46"/>
-      <c r="CF30" s="46"/>
-      <c r="CG30" s="46"/>
-      <c r="CH30" s="46"/>
-      <c r="CI30" s="46"/>
-      <c r="CJ30" s="46"/>
-      <c r="CK30" s="46"/>
-      <c r="CL30" s="46"/>
-      <c r="CM30" s="46"/>
-      <c r="CN30" s="46"/>
-      <c r="CO30" s="46"/>
-      <c r="CP30" s="46"/>
-      <c r="CQ30" s="46"/>
-      <c r="CR30" s="46"/>
-      <c r="CS30" s="46"/>
-      <c r="CT30" s="46"/>
-      <c r="CU30" s="46"/>
-      <c r="CV30" s="46"/>
-      <c r="CW30" s="46"/>
-      <c r="CX30" s="46"/>
-      <c r="CY30" s="46"/>
-      <c r="CZ30" s="46"/>
-      <c r="DA30" s="46"/>
-      <c r="DB30" s="46"/>
-      <c r="DC30" s="46"/>
-      <c r="DD30" s="46"/>
-      <c r="DE30" s="46"/>
-      <c r="DF30" s="46"/>
-      <c r="DG30" s="46"/>
-      <c r="DH30" s="46"/>
-      <c r="DI30" s="46"/>
-      <c r="DJ30" s="46"/>
-      <c r="DK30" s="46"/>
-      <c r="DL30" s="46"/>
-      <c r="DM30" s="46"/>
-      <c r="DN30" s="46"/>
-      <c r="DO30" s="46"/>
-      <c r="DP30" s="46"/>
-      <c r="DQ30" s="46"/>
-      <c r="DR30" s="46"/>
-      <c r="DS30" s="46"/>
-      <c r="DT30" s="46"/>
-      <c r="DU30" s="46"/>
-      <c r="DV30" s="46"/>
-      <c r="DW30" s="46"/>
-      <c r="DX30" s="46"/>
-      <c r="DY30" s="46"/>
-      <c r="DZ30" s="46"/>
-      <c r="EA30" s="46"/>
-      <c r="EB30" s="46"/>
-      <c r="EC30" s="46"/>
-      <c r="ED30" s="46"/>
-      <c r="EE30" s="46"/>
-      <c r="EF30" s="46"/>
-      <c r="EG30" s="46"/>
-      <c r="EH30" s="46"/>
-      <c r="EI30" s="46"/>
-      <c r="EJ30" s="46"/>
-      <c r="EK30" s="46"/>
-      <c r="EL30" s="46"/>
-      <c r="EM30" s="46"/>
-      <c r="EN30" s="46"/>
-      <c r="EO30" s="46"/>
-      <c r="EP30" s="46"/>
-      <c r="EQ30" s="46"/>
-      <c r="ER30" s="46"/>
-      <c r="ES30" s="46"/>
-      <c r="ET30" s="46"/>
-      <c r="EU30" s="46"/>
-      <c r="EV30" s="46"/>
-      <c r="EW30" s="46"/>
-      <c r="EX30" s="46"/>
-      <c r="EY30" s="46"/>
-      <c r="EZ30" s="46"/>
-      <c r="FA30" s="46"/>
-      <c r="FB30" s="46"/>
-      <c r="FC30" s="46"/>
-      <c r="FD30" s="46"/>
-      <c r="FE30" s="46"/>
-      <c r="FF30" s="46"/>
-      <c r="FG30" s="46"/>
-      <c r="FH30" s="46"/>
-      <c r="FI30" s="46"/>
-      <c r="FJ30" s="46"/>
-      <c r="FK30" s="46"/>
-      <c r="FL30" s="46"/>
-      <c r="FM30" s="46"/>
-      <c r="FN30" s="46"/>
-      <c r="FO30" s="46"/>
-      <c r="FP30" s="46"/>
-      <c r="FQ30" s="46"/>
-      <c r="FR30" s="46"/>
-      <c r="FS30" s="46"/>
-      <c r="FT30" s="46"/>
-      <c r="FU30" s="46"/>
-      <c r="FV30" s="46"/>
-      <c r="FW30" s="46"/>
-      <c r="FX30" s="46"/>
-      <c r="FY30" s="46"/>
-      <c r="FZ30" s="46"/>
-      <c r="GA30" s="46"/>
-      <c r="GB30" s="46"/>
-      <c r="GC30" s="46"/>
-      <c r="GD30" s="46"/>
-      <c r="GE30" s="46"/>
-      <c r="GF30" s="46"/>
-      <c r="GG30" s="46"/>
-      <c r="GH30" s="46"/>
-      <c r="GI30" s="46"/>
-      <c r="GJ30" s="46"/>
-      <c r="GK30" s="46"/>
-      <c r="GL30" s="46"/>
-      <c r="GM30" s="46"/>
-      <c r="GN30" s="46"/>
-      <c r="GO30" s="46"/>
-      <c r="GP30" s="46"/>
-      <c r="GQ30" s="46"/>
-      <c r="GR30" s="46"/>
-      <c r="GS30" s="46"/>
-      <c r="GT30" s="46"/>
-      <c r="GU30" s="46"/>
-      <c r="GV30" s="46"/>
-      <c r="GW30" s="46"/>
-      <c r="GX30" s="46"/>
-      <c r="GY30" s="46"/>
-      <c r="GZ30" s="46"/>
-      <c r="HA30" s="46"/>
-      <c r="HB30" s="46"/>
-      <c r="HC30" s="46"/>
-      <c r="HD30" s="46"/>
-      <c r="HE30" s="46"/>
-      <c r="HF30" s="46"/>
-      <c r="HG30" s="46"/>
-      <c r="HH30" s="46"/>
-      <c r="HI30" s="46"/>
-      <c r="HJ30" s="46"/>
-      <c r="HK30" s="46"/>
-      <c r="HL30" s="46"/>
-      <c r="HM30" s="46"/>
-      <c r="HN30" s="46"/>
-      <c r="HO30" s="46"/>
-      <c r="HP30" s="46"/>
-      <c r="HQ30" s="46"/>
-      <c r="HR30" s="46"/>
-      <c r="HS30" s="46"/>
-      <c r="HT30" s="46"/>
-      <c r="HU30" s="46"/>
-      <c r="HV30" s="46"/>
-      <c r="HW30" s="46"/>
-      <c r="HX30" s="46"/>
-      <c r="HY30" s="46"/>
-      <c r="HZ30" s="46"/>
-      <c r="IA30" s="46"/>
-      <c r="IB30" s="46"/>
-      <c r="IC30" s="46"/>
-      <c r="ID30" s="46"/>
-      <c r="IE30" s="46"/>
-      <c r="IF30" s="46"/>
-      <c r="IG30" s="46"/>
-      <c r="IH30" s="46"/>
-      <c r="II30" s="46"/>
-      <c r="IJ30" s="46"/>
-      <c r="IK30" s="46"/>
-      <c r="IL30" s="46"/>
-      <c r="IM30" s="46"/>
-      <c r="IN30" s="46"/>
-      <c r="IO30" s="46"/>
-      <c r="IP30" s="46"/>
-      <c r="IQ30" s="46"/>
-      <c r="IR30" s="46"/>
-      <c r="IS30" s="46"/>
-      <c r="IT30" s="46"/>
-      <c r="IU30" s="46"/>
-      <c r="IV30" s="46"/>
-      <c r="IW30" s="46"/>
-      <c r="IX30" s="46"/>
+    <row r="30" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="59"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="25"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="58"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="45"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
     </row>
-    <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
+    <row r="33" spans="1:258" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="49"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="X33" s="46"/>
+      <c r="Y33" s="46"/>
+      <c r="Z33" s="46"/>
+      <c r="AA33" s="46"/>
+      <c r="AB33" s="46"/>
+      <c r="AC33" s="46"/>
+      <c r="AD33" s="46"/>
+      <c r="AE33" s="46"/>
+      <c r="AF33" s="46"/>
+      <c r="AG33" s="46"/>
+      <c r="AH33" s="46"/>
+      <c r="AI33" s="46"/>
+      <c r="AJ33" s="46"/>
+      <c r="AK33" s="46"/>
+      <c r="AL33" s="46"/>
+      <c r="AM33" s="46"/>
+      <c r="AN33" s="46"/>
+      <c r="AO33" s="46"/>
+      <c r="AP33" s="46"/>
+      <c r="AQ33" s="46"/>
+      <c r="AR33" s="46"/>
+      <c r="AS33" s="46"/>
+      <c r="AT33" s="46"/>
+      <c r="AU33" s="46"/>
+      <c r="AV33" s="46"/>
+      <c r="AW33" s="46"/>
+      <c r="AX33" s="46"/>
+      <c r="AY33" s="46"/>
+      <c r="AZ33" s="46"/>
+      <c r="BA33" s="46"/>
+      <c r="BB33" s="46"/>
+      <c r="BC33" s="46"/>
+      <c r="BD33" s="46"/>
+      <c r="BE33" s="46"/>
+      <c r="BF33" s="46"/>
+      <c r="BG33" s="46"/>
+      <c r="BH33" s="46"/>
+      <c r="BI33" s="46"/>
+      <c r="BJ33" s="46"/>
+      <c r="BK33" s="46"/>
+      <c r="BL33" s="46"/>
+      <c r="BM33" s="46"/>
+      <c r="BN33" s="46"/>
+      <c r="BO33" s="46"/>
+      <c r="BP33" s="46"/>
+      <c r="BQ33" s="46"/>
+      <c r="BR33" s="46"/>
+      <c r="BS33" s="46"/>
+      <c r="BT33" s="46"/>
+      <c r="BU33" s="46"/>
+      <c r="BV33" s="46"/>
+      <c r="BW33" s="46"/>
+      <c r="BX33" s="46"/>
+      <c r="BY33" s="46"/>
+      <c r="BZ33" s="46"/>
+      <c r="CA33" s="46"/>
+      <c r="CB33" s="46"/>
+      <c r="CC33" s="46"/>
+      <c r="CD33" s="46"/>
+      <c r="CE33" s="46"/>
+      <c r="CF33" s="46"/>
+      <c r="CG33" s="46"/>
+      <c r="CH33" s="46"/>
+      <c r="CI33" s="46"/>
+      <c r="CJ33" s="46"/>
+      <c r="CK33" s="46"/>
+      <c r="CL33" s="46"/>
+      <c r="CM33" s="46"/>
+      <c r="CN33" s="46"/>
+      <c r="CO33" s="46"/>
+      <c r="CP33" s="46"/>
+      <c r="CQ33" s="46"/>
+      <c r="CR33" s="46"/>
+      <c r="CS33" s="46"/>
+      <c r="CT33" s="46"/>
+      <c r="CU33" s="46"/>
+      <c r="CV33" s="46"/>
+      <c r="CW33" s="46"/>
+      <c r="CX33" s="46"/>
+      <c r="CY33" s="46"/>
+      <c r="CZ33" s="46"/>
+      <c r="DA33" s="46"/>
+      <c r="DB33" s="46"/>
+      <c r="DC33" s="46"/>
+      <c r="DD33" s="46"/>
+      <c r="DE33" s="46"/>
+      <c r="DF33" s="46"/>
+      <c r="DG33" s="46"/>
+      <c r="DH33" s="46"/>
+      <c r="DI33" s="46"/>
+      <c r="DJ33" s="46"/>
+      <c r="DK33" s="46"/>
+      <c r="DL33" s="46"/>
+      <c r="DM33" s="46"/>
+      <c r="DN33" s="46"/>
+      <c r="DO33" s="46"/>
+      <c r="DP33" s="46"/>
+      <c r="DQ33" s="46"/>
+      <c r="DR33" s="46"/>
+      <c r="DS33" s="46"/>
+      <c r="DT33" s="46"/>
+      <c r="DU33" s="46"/>
+      <c r="DV33" s="46"/>
+      <c r="DW33" s="46"/>
+      <c r="DX33" s="46"/>
+      <c r="DY33" s="46"/>
+      <c r="DZ33" s="46"/>
+      <c r="EA33" s="46"/>
+      <c r="EB33" s="46"/>
+      <c r="EC33" s="46"/>
+      <c r="ED33" s="46"/>
+      <c r="EE33" s="46"/>
+      <c r="EF33" s="46"/>
+      <c r="EG33" s="46"/>
+      <c r="EH33" s="46"/>
+      <c r="EI33" s="46"/>
+      <c r="EJ33" s="46"/>
+      <c r="EK33" s="46"/>
+      <c r="EL33" s="46"/>
+      <c r="EM33" s="46"/>
+      <c r="EN33" s="46"/>
+      <c r="EO33" s="46"/>
+      <c r="EP33" s="46"/>
+      <c r="EQ33" s="46"/>
+      <c r="ER33" s="46"/>
+      <c r="ES33" s="46"/>
+      <c r="ET33" s="46"/>
+      <c r="EU33" s="46"/>
+      <c r="EV33" s="46"/>
+      <c r="EW33" s="46"/>
+      <c r="EX33" s="46"/>
+      <c r="EY33" s="46"/>
+      <c r="EZ33" s="46"/>
+      <c r="FA33" s="46"/>
+      <c r="FB33" s="46"/>
+      <c r="FC33" s="46"/>
+      <c r="FD33" s="46"/>
+      <c r="FE33" s="46"/>
+      <c r="FF33" s="46"/>
+      <c r="FG33" s="46"/>
+      <c r="FH33" s="46"/>
+      <c r="FI33" s="46"/>
+      <c r="FJ33" s="46"/>
+      <c r="FK33" s="46"/>
+      <c r="FL33" s="46"/>
+      <c r="FM33" s="46"/>
+      <c r="FN33" s="46"/>
+      <c r="FO33" s="46"/>
+      <c r="FP33" s="46"/>
+      <c r="FQ33" s="46"/>
+      <c r="FR33" s="46"/>
+      <c r="FS33" s="46"/>
+      <c r="FT33" s="46"/>
+      <c r="FU33" s="46"/>
+      <c r="FV33" s="46"/>
+      <c r="FW33" s="46"/>
+      <c r="FX33" s="46"/>
+      <c r="FY33" s="46"/>
+      <c r="FZ33" s="46"/>
+      <c r="GA33" s="46"/>
+      <c r="GB33" s="46"/>
+      <c r="GC33" s="46"/>
+      <c r="GD33" s="46"/>
+      <c r="GE33" s="46"/>
+      <c r="GF33" s="46"/>
+      <c r="GG33" s="46"/>
+      <c r="GH33" s="46"/>
+      <c r="GI33" s="46"/>
+      <c r="GJ33" s="46"/>
+      <c r="GK33" s="46"/>
+      <c r="GL33" s="46"/>
+      <c r="GM33" s="46"/>
+      <c r="GN33" s="46"/>
+      <c r="GO33" s="46"/>
+      <c r="GP33" s="46"/>
+      <c r="GQ33" s="46"/>
+      <c r="GR33" s="46"/>
+      <c r="GS33" s="46"/>
+      <c r="GT33" s="46"/>
+      <c r="GU33" s="46"/>
+      <c r="GV33" s="46"/>
+      <c r="GW33" s="46"/>
+      <c r="GX33" s="46"/>
+      <c r="GY33" s="46"/>
+      <c r="GZ33" s="46"/>
+      <c r="HA33" s="46"/>
+      <c r="HB33" s="46"/>
+      <c r="HC33" s="46"/>
+      <c r="HD33" s="46"/>
+      <c r="HE33" s="46"/>
+      <c r="HF33" s="46"/>
+      <c r="HG33" s="46"/>
+      <c r="HH33" s="46"/>
+      <c r="HI33" s="46"/>
+      <c r="HJ33" s="46"/>
+      <c r="HK33" s="46"/>
+      <c r="HL33" s="46"/>
+      <c r="HM33" s="46"/>
+      <c r="HN33" s="46"/>
+      <c r="HO33" s="46"/>
+      <c r="HP33" s="46"/>
+      <c r="HQ33" s="46"/>
+      <c r="HR33" s="46"/>
+      <c r="HS33" s="46"/>
+      <c r="HT33" s="46"/>
+      <c r="HU33" s="46"/>
+      <c r="HV33" s="46"/>
+      <c r="HW33" s="46"/>
+      <c r="HX33" s="46"/>
+      <c r="HY33" s="46"/>
+      <c r="HZ33" s="46"/>
+      <c r="IA33" s="46"/>
+      <c r="IB33" s="46"/>
+      <c r="IC33" s="46"/>
+      <c r="ID33" s="46"/>
+      <c r="IE33" s="46"/>
+      <c r="IF33" s="46"/>
+      <c r="IG33" s="46"/>
+      <c r="IH33" s="46"/>
+      <c r="II33" s="46"/>
+      <c r="IJ33" s="46"/>
+      <c r="IK33" s="46"/>
+      <c r="IL33" s="46"/>
+      <c r="IM33" s="46"/>
+      <c r="IN33" s="46"/>
+      <c r="IO33" s="46"/>
+      <c r="IP33" s="46"/>
+      <c r="IQ33" s="46"/>
+      <c r="IR33" s="46"/>
+      <c r="IS33" s="46"/>
+      <c r="IT33" s="46"/>
+      <c r="IU33" s="46"/>
+      <c r="IV33" s="46"/>
+      <c r="IW33" s="46"/>
+      <c r="IX33" s="46"/>
     </row>
-    <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
+    <row r="34" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="58"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
     </row>
-    <row r="35" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="59"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
-      <c r="G35" s="11"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="25"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26"/>
     </row>
-    <row r="36" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
+    <row r="36" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="59"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
@@ -8164,80 +8942,80 @@
       <c r="I36" s="26"/>
       <c r="J36" s="26"/>
     </row>
-    <row r="37" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="58"/>
+    <row r="37" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="59"/>
       <c r="B37" s="25"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
       <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
+      <c r="H37" s="11"/>
       <c r="I37" s="26"/>
       <c r="J37" s="26"/>
     </row>
-    <row r="38" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="25"/>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
     </row>
-    <row r="39" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="59"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="9"/>
+    <row r="39" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="60"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
       <c r="G39" s="25"/>
-      <c r="H39" s="11"/>
+      <c r="H39" s="25"/>
       <c r="I39" s="26"/>
       <c r="J39" s="26"/>
     </row>
-    <row r="40" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
+    <row r="40" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="58"/>
       <c r="B40" s="25"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="25"/>
-      <c r="H40" s="26"/>
+      <c r="H40" s="25"/>
       <c r="I40" s="26"/>
       <c r="J40" s="26"/>
     </row>
-    <row r="41" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="26"/>
+    <row r="41" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="59"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="26"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
       <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="26"/>
       <c r="J41" s="26"/>
     </row>
-    <row r="42" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
+    <row r="42" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="59"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="26"/>
+      <c r="H42" s="11"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
     </row>
-    <row r="43" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24"/>
+    <row r="43" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="59"/>
       <c r="B43" s="25"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -8248,19 +9026,19 @@
       <c r="I43" s="26"/>
       <c r="J43" s="26"/>
     </row>
-    <row r="44" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
+    <row r="44" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="60"/>
       <c r="B44" s="25"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="26"/>
+      <c r="H44" s="25"/>
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
     </row>
-    <row r="45" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="24"/>
       <c r="B45" s="25"/>
       <c r="C45" s="26"/>
@@ -8272,15 +9050,52 @@
       <c r="I45" s="26"/>
       <c r="J45" s="26"/>
     </row>
+    <row r="46" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+    </row>
+    <row r="48" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="24"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
1. Add role manage pages. 2. Add some new feature
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="133">
   <si>
     <t>Comments</t>
   </si>
@@ -864,6 +864,28 @@
   }]
 }</t>
   </si>
+  <si>
+    <t>/permission-categories</t>
+  </si>
+  <si>
+    <t>Get all permission categories</t>
+  </si>
+  <si>
+    <t>{
+                "permissionCategories": [
+                    {
+                       "id": 1,
+                        "name": '督办',
+                        "permissions": [
+                            {
+                                "id": 1,
+                                "name": '督办_默认权限'
+                            }
+                        ]
+                    }
+                ]
+            }</t>
+  </si>
 </sst>
 </file>
 
@@ -1240,6 +1262,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1275,9 +1300,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,7 +1677,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -2775,7 +2797,7 @@
       <c r="IX5" s="35"/>
     </row>
     <row r="6" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -3045,7 +3067,7 @@
       <c r="IX6" s="12"/>
     </row>
     <row r="7" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="56"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="11" t="s">
         <v>117</v>
       </c>
@@ -3313,7 +3335,7 @@
       <c r="IX7" s="12"/>
     </row>
     <row r="8" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="29" t="s">
         <v>106</v>
       </c>
@@ -3581,7 +3603,7 @@
       <c r="IX8" s="12"/>
     </row>
     <row r="9" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="11" t="s">
         <v>107</v>
       </c>
@@ -3853,7 +3875,7 @@
       <c r="IX9" s="12"/>
     </row>
     <row r="10" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="56"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="11" t="s">
         <v>121</v>
       </c>
@@ -4123,7 +4145,7 @@
       <c r="IX10" s="12"/>
     </row>
     <row r="11" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="11" t="s">
         <v>108</v>
       </c>
@@ -4395,7 +4417,7 @@
       <c r="IX11" s="12"/>
     </row>
     <row r="12" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="56"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="11" t="s">
         <v>123</v>
       </c>
@@ -4665,7 +4687,7 @@
       <c r="IX12" s="12"/>
     </row>
     <row r="13" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="11" t="s">
         <v>112</v>
       </c>
@@ -5197,7 +5219,7 @@
       <c r="IX14" s="35"/>
     </row>
     <row r="15" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="65" t="s">
         <v>126</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -5467,14 +5489,22 @@
       <c r="IX15" s="12"/>
     </row>
     <row r="16" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="65"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="11"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="I16" s="9"/>
       <c r="J16" s="11"/>
       <c r="K16" s="9"/>
@@ -5727,13 +5757,13 @@
       <c r="IX16" s="12"/>
     </row>
     <row r="17" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="65"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="67"/>
+      <c r="G17" s="55"/>
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
       <c r="J17" s="11"/>
@@ -5987,13 +6017,13 @@
       <c r="IX17" s="12"/>
     </row>
     <row r="18" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="66"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="67"/>
+      <c r="G18" s="55"/>
       <c r="H18" s="11"/>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
@@ -6507,7 +6537,7 @@
       <c r="IX19" s="35"/>
     </row>
     <row r="20" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="30"/>
@@ -6767,7 +6797,7 @@
       <c r="IX20" s="12"/>
     </row>
     <row r="21" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -7027,7 +7057,7 @@
       <c r="IX21" s="12"/>
     </row>
     <row r="22" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="29"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -7807,7 +7837,7 @@
       <c r="IX24" s="35"/>
     </row>
     <row r="25" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="64"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="D25" s="30"/>
@@ -8067,7 +8097,7 @@
       <c r="IX25" s="12"/>
     </row>
     <row r="26" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="65"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -8327,7 +8357,7 @@
       <c r="IX26" s="12"/>
     </row>
     <row r="27" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="66"/>
+      <c r="A27" s="67"/>
       <c r="B27" s="29"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
@@ -8600,7 +8630,7 @@
       <c r="IX28" s="46"/>
     </row>
     <row r="29" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="58"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="32"/>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
@@ -8612,7 +8642,7 @@
       <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="59"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="11"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -8623,7 +8653,7 @@
       <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="59"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="11"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
@@ -8635,7 +8665,7 @@
       <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="29"/>
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
@@ -8907,7 +8937,7 @@
       <c r="IX33" s="46"/>
     </row>
     <row r="34" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="58"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="44"/>
       <c r="C34" s="45"/>
       <c r="D34" s="45"/>
@@ -8919,7 +8949,7 @@
       <c r="J34" s="45"/>
     </row>
     <row r="35" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="59"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -8931,7 +8961,7 @@
       <c r="J35" s="26"/>
     </row>
     <row r="36" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
@@ -8943,7 +8973,7 @@
       <c r="J36" s="26"/>
     </row>
     <row r="37" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="59"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="25"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
@@ -8955,7 +8985,7 @@
       <c r="J37" s="26"/>
     </row>
     <row r="38" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="59"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="25"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -8967,7 +8997,7 @@
       <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="25"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -8979,7 +9009,7 @@
       <c r="J39" s="26"/>
     </row>
     <row r="40" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="58"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="25"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
@@ -8991,8 +9021,8 @@
       <c r="J40" s="26"/>
     </row>
     <row r="41" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="59"/>
-      <c r="B41" s="61"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="62"/>
       <c r="C41" s="9"/>
       <c r="D41" s="26"/>
       <c r="E41" s="26"/>
@@ -9003,8 +9033,8 @@
       <c r="J41" s="26"/>
     </row>
     <row r="42" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="59"/>
-      <c r="B42" s="62"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="63"/>
       <c r="C42" s="9"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
@@ -9015,7 +9045,7 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="25"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -9027,7 +9057,7 @@
       <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="25"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -11292,7 +11322,7 @@
       <c r="IX9" s="35"/>
     </row>
     <row r="10" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="64" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -11564,7 +11594,7 @@
       <c r="IX10" s="12"/>
     </row>
     <row r="11" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
@@ -11834,7 +11864,7 @@
       <c r="IX11" s="12"/>
     </row>
     <row r="12" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="29" t="s">
         <v>34</v>
       </c>
@@ -12632,7 +12662,7 @@
       <c r="IX14" s="35"/>
     </row>
     <row r="15" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="65" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -12904,7 +12934,7 @@
       <c r="IX15" s="12"/>
     </row>
     <row r="16" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="65"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="11" t="s">
         <v>39</v>
       </c>
@@ -13172,7 +13202,7 @@
       <c r="IX16" s="12"/>
     </row>
     <row r="17" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="29" t="s">
         <v>41</v>
       </c>
@@ -13453,7 +13483,7 @@
       <c r="IX18" s="46"/>
     </row>
     <row r="19" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="59" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -13477,7 +13507,7 @@
       <c r="J19" s="45"/>
     </row>
     <row r="20" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="11" t="s">
         <v>56</v>
       </c>
@@ -13498,7 +13528,7 @@
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="59"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="11" t="s">
         <v>51</v>
       </c>
@@ -13520,7 +13550,7 @@
       <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="29" t="s">
         <v>52</v>
       </c>
@@ -13802,7 +13832,7 @@
       <c r="IX23" s="46"/>
     </row>
     <row r="24" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="59" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="44" t="s">
@@ -13824,7 +13854,7 @@
       <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="59"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="25" t="s">
         <v>67</v>
       </c>
@@ -13846,7 +13876,7 @@
       <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="59"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="25" t="s">
         <v>70</v>
       </c>
@@ -13870,7 +13900,7 @@
       <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="25" t="s">
         <v>79</v>
       </c>
@@ -13892,7 +13922,7 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="25" t="s">
         <v>73</v>
       </c>
@@ -13916,7 +13946,7 @@
       <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="25" t="s">
         <v>75</v>
       </c>
@@ -13938,7 +13968,7 @@
       <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="59" t="s">
         <v>82</v>
       </c>
       <c r="B30" s="25" t="s">
@@ -13962,8 +13992,8 @@
       <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="59"/>
-      <c r="B31" s="61" t="s">
+      <c r="A31" s="60"/>
+      <c r="B31" s="62" t="s">
         <v>85</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -13984,8 +14014,8 @@
       <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="62"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="9" t="s">
         <v>86</v>
       </c>
@@ -14004,7 +14034,7 @@
       <c r="J32" s="26"/>
     </row>
     <row r="33" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="25" t="s">
         <v>91</v>
       </c>
@@ -14026,7 +14056,7 @@
       <c r="J33" s="26"/>
     </row>
     <row r="34" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="25" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
1. Update API doc 2. Add some new feature
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -797,22 +797,6 @@
 }</t>
   </si>
   <si>
-    <t>{
- "count": 100,
- "employees": [
-  {
-   "id": 1,
-   "realName": "",
-   "userName": "",
-   "email": "",
-   "phone": "",
-   "order": 22,
-   "department": ""
-  }
- ]
-}</t>
-  </si>
-  <si>
     <t>Delete departments</t>
   </si>
   <si>
@@ -827,9 +811,6 @@
     <t>{
   "userIds": [1,2,3]
 }</t>
-  </si>
-  <si>
-    <t>/departments/$id/employees?page=1&amp;pageSize=10</t>
   </si>
   <si>
     <t>Roles</t>
@@ -969,6 +950,25 @@
                     "departments": ["部门1", "部门2"]
                 }
             }</t>
+  </si>
+  <si>
+    <t>/departments/$id/users?page=1&amp;pageSize=10</t>
+  </si>
+  <si>
+    <t>{
+ "count": 100,
+ "users": [
+  {
+   "id": 1,
+   "realName": "",
+   "userName": "",
+   "email": "",
+   "phone": "",
+   "order": 22,
+   "department": ""
+  }
+ ]
+}</t>
   </si>
 </sst>
 </file>
@@ -1759,9 +1759,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IX51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -3424,7 +3424,7 @@
         <v>106</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>25</v>
@@ -3433,7 +3433,7 @@
       <c r="F8" s="28"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="29"/>
@@ -3700,7 +3700,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>114</v>
@@ -3961,7 +3961,7 @@
     <row r="10" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
       <c r="B10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>105</v>
@@ -3972,7 +3972,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>114</v>
@@ -4503,7 +4503,7 @@
     <row r="12" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="57"/>
       <c r="B12" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>109</v>
@@ -4514,7 +4514,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>114</v>
@@ -4773,10 +4773,10 @@
     <row r="13" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="57"/>
       <c r="B13" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>15</v>
@@ -4784,10 +4784,10 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="11"/>
@@ -5043,10 +5043,10 @@
     <row r="14" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="57"/>
       <c r="B14" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>25</v>
@@ -5055,7 +5055,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="11"/>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="17" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="39" t="s">
         <v>125</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>127</v>
       </c>
       <c r="D17" s="37" t="s">
         <v>25</v>
@@ -5857,7 +5857,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="38"/>
       <c r="H17" s="39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="39"/>
@@ -6113,10 +6113,10 @@
     <row r="18" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="66"/>
       <c r="B18" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>25</v>
@@ -6125,7 +6125,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="55"/>
       <c r="H18" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
@@ -6381,10 +6381,10 @@
     <row r="19" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="66"/>
       <c r="B19" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>25</v>
@@ -6393,7 +6393,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="55"/>
       <c r="H19" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
@@ -6649,10 +6649,10 @@
     <row r="20" spans="1:258" s="13" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="66"/>
       <c r="B20" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>25</v>
@@ -6661,7 +6661,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="55"/>
       <c r="H20" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="11"/>

</xml_diff>

<commit_message>
Add get pagination roles API.
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -700,18 +700,6 @@
   </si>
   <si>
     <t>/roles?page=1&amp;pageSize=10</t>
-  </si>
-  <si>
-    <t>{
- "count": 100,
- "roles":[{
-   "id": 1,
-   "name": "",
-   "category": "",
-   "creator": "",
-   "remark": ""
-  }]
-}</t>
   </si>
   <si>
     <t>Get role by id</t>
@@ -1555,6 +1543,18 @@
  "desc": ""
 }</t>
   </si>
+  <si>
+    <t>{
+ "count": 100,
+ "result":[{
+   "id": 1,
+   "name": "",
+   "category": "",
+   "creator": "",
+   "remark": ""
+  }]
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -2170,6 +2170,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2208,9 +2211,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2588,7 +2588,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75"/>
@@ -3712,7 +3712,7 @@
       <c r="IX5" s="24"/>
     </row>
     <row r="6" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="107" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="88" t="s">
@@ -3728,7 +3728,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="70"/>
@@ -3984,12 +3984,12 @@
       <c r="IX6" s="51"/>
     </row>
     <row r="7" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A7" s="107"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="87" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>26</v>
@@ -3998,7 +3998,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="20"/>
       <c r="H7" s="57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="69"/>
@@ -4254,12 +4254,12 @@
       <c r="IX7" s="51"/>
     </row>
     <row r="8" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A8" s="107"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="94" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>26</v>
@@ -4268,7 +4268,7 @@
       <c r="F8" s="36"/>
       <c r="G8" s="35"/>
       <c r="H8" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" s="35"/>
       <c r="J8" s="73"/>
@@ -4524,7 +4524,7 @@
       <c r="IX8" s="51"/>
     </row>
     <row r="9" spans="1:258" s="54" customFormat="1" ht="138" customHeight="1">
-      <c r="A9" s="107"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="92" t="s">
         <v>32</v>
       </c>
@@ -4537,7 +4537,7 @@
       <c r="E9" s="90"/>
       <c r="F9" s="90"/>
       <c r="G9" s="89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H9" s="89" t="s">
         <v>33</v>
@@ -4798,12 +4798,12 @@
       <c r="IX9" s="76"/>
     </row>
     <row r="10" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A10" s="107"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="95" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="59" t="s">
         <v>26</v>
@@ -5066,7 +5066,7 @@
       <c r="IX10" s="79"/>
     </row>
     <row r="11" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A11" s="107"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="87" t="s">
         <v>37</v>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="IX11" s="51"/>
     </row>
     <row r="12" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="107" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="99" t="s">
@@ -5612,12 +5612,12 @@
       <c r="IX12" s="51"/>
     </row>
     <row r="13" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A13" s="107"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="99" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="97" t="s">
         <v>26</v>
@@ -5632,7 +5632,7 @@
       <c r="J13" s="96"/>
       <c r="K13" s="98"/>
       <c r="L13" s="96" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M13" s="79"/>
       <c r="N13" s="79"/>
@@ -5882,7 +5882,7 @@
       <c r="IX13" s="79"/>
     </row>
     <row r="14" spans="1:258" s="56" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A14" s="108"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="99" t="s">
         <v>47</v>
       </c>
@@ -6154,9 +6154,9 @@
       <c r="IX14" s="81"/>
     </row>
     <row r="15" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A15" s="107"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="93" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="93" t="s">
         <v>49</v>
@@ -6426,12 +6426,12 @@
       <c r="IX15" s="79"/>
     </row>
     <row r="16" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A16" s="107"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="58" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="59" t="s">
         <v>26</v>
@@ -6694,7 +6694,7 @@
       <c r="IX16" s="79"/>
     </row>
     <row r="17" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A17" s="109"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="20" t="s">
         <v>54</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="IX18" s="24"/>
     </row>
     <row r="19" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="111" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -7244,7 +7244,7 @@
       <c r="F19" s="27"/>
       <c r="G19" s="29"/>
       <c r="H19" s="26" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="I19" s="26"/>
       <c r="J19" s="70"/>
@@ -7498,12 +7498,12 @@
       <c r="IX19" s="51"/>
     </row>
     <row r="20" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A20" s="111"/>
+      <c r="A20" s="112"/>
       <c r="B20" s="58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" s="59" t="s">
         <v>26</v>
@@ -7512,7 +7512,7 @@
       <c r="F20" s="59"/>
       <c r="G20" s="63"/>
       <c r="H20" s="58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="59"/>
       <c r="J20" s="58"/>
@@ -7766,20 +7766,20 @@
       <c r="IX20" s="79"/>
     </row>
     <row r="21" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A21" s="111"/>
+      <c r="A21" s="112"/>
       <c r="B21" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>161</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="78"/>
       <c r="F21" s="78"/>
-      <c r="G21" s="114" t="s">
-        <v>162</v>
+      <c r="G21" s="101" t="s">
+        <v>161</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>33</v>
@@ -8036,12 +8036,12 @@
       <c r="IX21" s="79"/>
     </row>
     <row r="22" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A22" s="111"/>
+      <c r="A22" s="112"/>
       <c r="B22" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="59" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="59" t="s">
-        <v>65</v>
       </c>
       <c r="D22" s="59" t="s">
         <v>26</v>
@@ -8050,7 +8050,7 @@
       <c r="F22" s="59"/>
       <c r="G22" s="63"/>
       <c r="H22" s="58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I22" s="59"/>
       <c r="J22" s="58"/>
@@ -8304,12 +8304,12 @@
       <c r="IX22" s="79"/>
     </row>
     <row r="23" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A23" s="112"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" s="59" t="s">
         <v>26</v>
@@ -8318,7 +8318,7 @@
       <c r="F23" s="59"/>
       <c r="G23" s="63"/>
       <c r="H23" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="59"/>
       <c r="J23" s="58"/>
@@ -8832,7 +8832,7 @@
       <c r="IX24" s="24"/>
     </row>
     <row r="25" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A25" s="113"/>
+      <c r="A25" s="114"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
@@ -9092,7 +9092,7 @@
       <c r="IX25" s="51"/>
     </row>
     <row r="26" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A26" s="113"/>
+      <c r="A26" s="114"/>
       <c r="B26" s="20"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -9352,7 +9352,7 @@
       <c r="IX26" s="51"/>
     </row>
     <row r="27" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A27" s="113"/>
+      <c r="A27" s="114"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
@@ -10132,7 +10132,7 @@
       <c r="IX29" s="24"/>
     </row>
     <row r="30" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A30" s="110"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="33"/>
@@ -10392,7 +10392,7 @@
       <c r="IX30" s="51"/>
     </row>
     <row r="31" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A31" s="111"/>
+      <c r="A31" s="112"/>
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -10652,7 +10652,7 @@
       <c r="IX31" s="51"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A32" s="112"/>
+      <c r="A32" s="113"/>
       <c r="B32" s="35"/>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
@@ -10926,7 +10926,7 @@
       <c r="IX33" s="39"/>
     </row>
     <row r="34" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A34" s="101"/>
+      <c r="A34" s="102"/>
       <c r="B34" s="32"/>
       <c r="C34" s="41"/>
       <c r="D34" s="41"/>
@@ -10940,7 +10940,7 @@
       <c r="L34" s="43"/>
     </row>
     <row r="35" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A35" s="102"/>
+      <c r="A35" s="103"/>
       <c r="B35" s="20"/>
       <c r="C35" s="43"/>
       <c r="D35" s="43"/>
@@ -10953,7 +10953,7 @@
       <c r="L35" s="43"/>
     </row>
     <row r="36" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A36" s="102"/>
+      <c r="A36" s="103"/>
       <c r="B36" s="20"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -10967,7 +10967,7 @@
       <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A37" s="103"/>
+      <c r="A37" s="104"/>
       <c r="B37" s="35"/>
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
@@ -11241,7 +11241,7 @@
       <c r="IX38" s="39"/>
     </row>
     <row r="39" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A39" s="101"/>
+      <c r="A39" s="102"/>
       <c r="B39" s="42"/>
       <c r="C39" s="41"/>
       <c r="D39" s="41"/>
@@ -11255,7 +11255,7 @@
       <c r="L39" s="43"/>
     </row>
     <row r="40" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A40" s="102"/>
+      <c r="A40" s="103"/>
       <c r="B40" s="44"/>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -11269,7 +11269,7 @@
       <c r="L40" s="43"/>
     </row>
     <row r="41" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A41" s="102"/>
+      <c r="A41" s="103"/>
       <c r="B41" s="44"/>
       <c r="C41" s="43"/>
       <c r="D41" s="43"/>
@@ -11283,7 +11283,7 @@
       <c r="L41" s="43"/>
     </row>
     <row r="42" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A42" s="102"/>
+      <c r="A42" s="103"/>
       <c r="B42" s="44"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -11297,7 +11297,7 @@
       <c r="L42" s="43"/>
     </row>
     <row r="43" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A43" s="102"/>
+      <c r="A43" s="103"/>
       <c r="B43" s="44"/>
       <c r="C43" s="43"/>
       <c r="D43" s="43"/>
@@ -11311,7 +11311,7 @@
       <c r="L43" s="43"/>
     </row>
     <row r="44" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A44" s="103"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="44"/>
       <c r="C44" s="43"/>
       <c r="D44" s="43"/>
@@ -11325,7 +11325,7 @@
       <c r="L44" s="43"/>
     </row>
     <row r="45" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A45" s="101"/>
+      <c r="A45" s="102"/>
       <c r="B45" s="44"/>
       <c r="C45" s="43"/>
       <c r="D45" s="43"/>
@@ -11339,8 +11339,8 @@
       <c r="L45" s="43"/>
     </row>
     <row r="46" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A46" s="102"/>
-      <c r="B46" s="104"/>
+      <c r="A46" s="103"/>
+      <c r="B46" s="105"/>
       <c r="C46" s="21"/>
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
@@ -11353,8 +11353,8 @@
       <c r="L46" s="43"/>
     </row>
     <row r="47" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A47" s="102"/>
-      <c r="B47" s="105"/>
+      <c r="A47" s="103"/>
+      <c r="B47" s="106"/>
       <c r="C47" s="21"/>
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
@@ -11367,7 +11367,7 @@
       <c r="L47" s="43"/>
     </row>
     <row r="48" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A48" s="102"/>
+      <c r="A48" s="103"/>
       <c r="B48" s="44"/>
       <c r="C48" s="43"/>
       <c r="D48" s="43"/>
@@ -11381,7 +11381,7 @@
       <c r="L48" s="43"/>
     </row>
     <row r="49" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A49" s="103"/>
+      <c r="A49" s="104"/>
       <c r="B49" s="44"/>
       <c r="C49" s="43"/>
       <c r="D49" s="43"/>
@@ -12078,7 +12078,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>21</v>
@@ -12597,13 +12597,13 @@
     </row>
     <row r="6" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A6" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>71</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>72</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>26</v>
@@ -12612,7 +12612,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="26"/>
@@ -13127,13 +13127,13 @@
     </row>
     <row r="8" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A8" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>26</v>
@@ -13142,7 +13142,7 @@
       <c r="F8" s="27"/>
       <c r="G8" s="29"/>
       <c r="H8" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="26"/>
@@ -13656,14 +13656,14 @@
       <c r="IX9" s="24"/>
     </row>
     <row r="10" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="C10" s="32" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>80</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>18</v>
@@ -13671,10 +13671,10 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="G10" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>81</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>82</v>
       </c>
       <c r="I10" s="33"/>
       <c r="J10" s="32"/>
@@ -13928,12 +13928,12 @@
       <c r="IX10" s="51"/>
     </row>
     <row r="11" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A11" s="113"/>
+      <c r="A11" s="114"/>
       <c r="B11" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>26</v>
@@ -13942,7 +13942,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="20"/>
@@ -14198,12 +14198,12 @@
       <c r="IX11" s="51"/>
     </row>
     <row r="12" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A12" s="113"/>
+      <c r="A12" s="114"/>
       <c r="B12" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>86</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>87</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>26</v>
@@ -14212,7 +14212,7 @@
       <c r="F12" s="36"/>
       <c r="G12" s="35"/>
       <c r="H12" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="36"/>
       <c r="J12" s="35"/>
@@ -14470,10 +14470,10 @@
     <row r="13" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>26</v>
@@ -14482,7 +14482,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I13" s="52"/>
       <c r="J13" s="53"/>
@@ -14996,14 +14996,14 @@
       <c r="IX14" s="24"/>
     </row>
     <row r="15" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="111" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="C15" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>94</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>18</v>
@@ -15011,10 +15011,10 @@
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="G15" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="32" t="s">
         <v>95</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>96</v>
       </c>
       <c r="I15" s="33"/>
       <c r="J15" s="32"/>
@@ -15268,12 +15268,12 @@
       <c r="IX15" s="51"/>
     </row>
     <row r="16" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A16" s="111"/>
+      <c r="A16" s="112"/>
       <c r="B16" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>97</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>26</v>
@@ -15282,7 +15282,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="20"/>
@@ -15536,12 +15536,12 @@
       <c r="IX16" s="51"/>
     </row>
     <row r="17" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A17" s="112"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>100</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>101</v>
       </c>
       <c r="D17" s="37" t="s">
         <v>26</v>
@@ -15550,7 +15550,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="37"/>
@@ -15817,90 +15817,90 @@
       <c r="IX18" s="39"/>
     </row>
     <row r="19" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="C19" s="41" t="s">
         <v>104</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>105</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="42" t="s">
         <v>106</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>107</v>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A20" s="102"/>
+      <c r="A20" s="103"/>
       <c r="B20" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="43" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" s="43" t="s">
-        <v>109</v>
       </c>
       <c r="D20" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="44" t="s">
         <v>106</v>
-      </c>
-      <c r="G20" s="44" t="s">
-        <v>107</v>
       </c>
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A21" s="102"/>
+      <c r="A21" s="103"/>
       <c r="B21" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="43" t="s">
         <v>110</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>111</v>
       </c>
       <c r="D21" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="43"/>
       <c r="F21" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="44"/>
       <c r="H21" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
     </row>
     <row r="22" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A22" s="103"/>
+      <c r="A22" s="104"/>
       <c r="B22" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>112</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>113</v>
       </c>
       <c r="D22" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="37"/>
       <c r="F22" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="38"/>
       <c r="H22" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I22" s="37"/>
       <c r="J22" s="37"/>
@@ -16166,247 +16166,247 @@
       <c r="IX23" s="39"/>
     </row>
     <row r="24" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="102" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>115</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>116</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" s="42"/>
       <c r="H24" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I24" s="41"/>
       <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A25" s="102"/>
+      <c r="A25" s="103"/>
       <c r="B25" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>119</v>
       </c>
       <c r="D25" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="44"/>
       <c r="H25" s="44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A26" s="102"/>
+      <c r="A26" s="103"/>
       <c r="B26" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="43"/>
       <c r="F26" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="H26" s="44" t="s">
-        <v>123</v>
       </c>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A27" s="102"/>
+      <c r="A27" s="103"/>
       <c r="B27" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="43" t="s">
         <v>124</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>125</v>
       </c>
       <c r="D27" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="43"/>
       <c r="F27" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" s="44"/>
       <c r="H27" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A28" s="102"/>
+      <c r="A28" s="103"/>
       <c r="B28" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="43" t="s">
         <v>127</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>128</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="43"/>
       <c r="F28" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I28" s="43"/>
       <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A29" s="103"/>
+      <c r="A29" s="104"/>
       <c r="B29" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" s="43" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="43"/>
       <c r="F29" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G29" s="44"/>
       <c r="H29" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="C30" s="43" t="s">
         <v>133</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>134</v>
       </c>
       <c r="D30" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="43"/>
       <c r="F30" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
     </row>
     <row r="31" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A31" s="102"/>
-      <c r="B31" s="104" t="s">
+      <c r="A31" s="103"/>
+      <c r="B31" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G31" s="44"/>
       <c r="H31" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="105"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G32" s="44"/>
       <c r="H32" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I32" s="43"/>
       <c r="J32" s="43"/>
     </row>
     <row r="33" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A33" s="102"/>
+      <c r="A33" s="103"/>
       <c r="B33" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="43" t="s">
         <v>141</v>
-      </c>
-      <c r="C33" s="43" t="s">
-        <v>142</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G33" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
       <c r="J33" s="43"/>
     </row>
     <row r="34" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A34" s="103"/>
+      <c r="A34" s="104"/>
       <c r="B34" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>144</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>145</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="43"/>
       <c r="F34" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G34" s="44"/>
       <c r="H34" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I34" s="43"/>
       <c r="J34" s="43"/>

</xml_diff>

<commit_message>
Implement get user actions API.
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -786,145 +786,6 @@
     <t>Get user roles information</t>
   </si>
   <si>
-    <t>/users/{userId}/roles</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>{
-                    id: 1,
-                    name: '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>周志德</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>',
-                    permissionCategories: [
-                        {
-                            id: 1,
-                            text: '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>督办</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>',
-                            nodes: [
-                                {
-                                    id: 1,
-                                    text: '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>督办</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>默认权限</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>'
-                                }
-                            ]
-                        }
-                    ],
-                    "departments": ["</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>长江证券</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>"],
-                    "remark": '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>备注</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>'
-                }</t>
-    </r>
-  </si>
-  <si>
     <t>Reset password</t>
   </si>
   <si>
@@ -1596,12 +1457,147 @@
   "status": "succeed"
 }</t>
   </si>
+  <si>
+    <r>
+      <t>{
+  user: {
+                    id: 1,
+                    name: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>周志德</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>',
+                    permissionCategories: [
+                        {
+                            id: 1,
+                            text: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>督办</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>',
+                            nodes: [
+                                {
+                                    id: 1,
+                                    text: '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>督办</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>默认权限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'
+                                }
+                            ]
+                        }
+                    ],
+                    "departments": ["</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>长江证券</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"],
+                    "remark": '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备注</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'
+  }
+                }</t>
+    </r>
+  </si>
+  <si>
+    <t>/users/{userId}/actions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1658,18 +1654,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -1890,7 +1874,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2089,13 +2073,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2119,7 +2097,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2128,7 +2106,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2164,6 +2142,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2187,21 +2180,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2331,7 +2309,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2366,7 +2344,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2578,8 +2556,8 @@
   <dimension ref="A1:IX55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75"/>
@@ -2631,7 +2609,7 @@
       <c r="J1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="67" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="43" t="s">
@@ -2654,11 +2632,11 @@
       <c r="G2" s="15"/>
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="70" t="s">
+      <c r="J2" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="71"/>
-      <c r="L2" s="72"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="50"/>
       <c r="N2" s="50"/>
       <c r="O2" s="50"/>
@@ -2917,7 +2895,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="73"/>
+      <c r="K3" s="71"/>
       <c r="L3" s="21"/>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
@@ -3190,8 +3168,8 @@
       <c r="I4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74" t="s">
+      <c r="J4" s="72"/>
+      <c r="K4" s="72" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="21"/>
@@ -3453,7 +3431,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
-      <c r="K5" s="74"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="21"/>
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
@@ -3703,7 +3681,7 @@
       <c r="IX5" s="24"/>
     </row>
     <row r="6" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="58" t="s">
@@ -3722,9 +3700,9 @@
         <v>27</v>
       </c>
       <c r="I6" s="26"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="76" t="s">
+      <c r="J6" s="73"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="74" t="s">
         <v>28</v>
       </c>
       <c r="M6" s="51"/>
@@ -3975,7 +3953,7 @@
       <c r="IX6" s="51"/>
     </row>
     <row r="7" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A7" s="92"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="56" t="s">
         <v>29</v>
       </c>
@@ -3992,9 +3970,9 @@
         <v>31</v>
       </c>
       <c r="I7" s="20"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="77" t="s">
+      <c r="J7" s="72"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="75" t="s">
         <v>32</v>
       </c>
       <c r="M7" s="51"/>
@@ -4245,7 +4223,7 @@
       <c r="IX7" s="51"/>
     </row>
     <row r="8" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A8" s="92"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="59" t="s">
         <v>33</v>
       </c>
@@ -4262,8 +4240,8 @@
         <v>35</v>
       </c>
       <c r="I8" s="35"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="79" t="s">
+      <c r="J8" s="76"/>
+      <c r="K8" s="77" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="21"/>
@@ -4515,7 +4493,7 @@
       <c r="IX8" s="51"/>
     </row>
     <row r="9" spans="1:258" s="54" customFormat="1" ht="138" customHeight="1">
-      <c r="A9" s="92"/>
+      <c r="A9" s="95"/>
       <c r="B9" s="60" t="s">
         <v>37</v>
       </c>
@@ -4536,260 +4514,260 @@
       <c r="I9" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="76" t="s">
+      <c r="J9" s="78"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="82"/>
-      <c r="U9" s="82"/>
-      <c r="V9" s="82"/>
-      <c r="W9" s="82"/>
-      <c r="X9" s="82"/>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="82"/>
-      <c r="AA9" s="82"/>
-      <c r="AB9" s="82"/>
-      <c r="AC9" s="82"/>
-      <c r="AD9" s="82"/>
-      <c r="AE9" s="82"/>
-      <c r="AF9" s="82"/>
-      <c r="AG9" s="82"/>
-      <c r="AH9" s="82"/>
-      <c r="AI9" s="82"/>
-      <c r="AJ9" s="82"/>
-      <c r="AK9" s="82"/>
-      <c r="AL9" s="82"/>
-      <c r="AM9" s="82"/>
-      <c r="AN9" s="82"/>
-      <c r="AO9" s="82"/>
-      <c r="AP9" s="82"/>
-      <c r="AQ9" s="82"/>
-      <c r="AR9" s="82"/>
-      <c r="AS9" s="82"/>
-      <c r="AT9" s="82"/>
-      <c r="AU9" s="82"/>
-      <c r="AV9" s="82"/>
-      <c r="AW9" s="82"/>
-      <c r="AX9" s="82"/>
-      <c r="AY9" s="82"/>
-      <c r="AZ9" s="82"/>
-      <c r="BA9" s="82"/>
-      <c r="BB9" s="82"/>
-      <c r="BC9" s="82"/>
-      <c r="BD9" s="82"/>
-      <c r="BE9" s="82"/>
-      <c r="BF9" s="82"/>
-      <c r="BG9" s="82"/>
-      <c r="BH9" s="82"/>
-      <c r="BI9" s="82"/>
-      <c r="BJ9" s="82"/>
-      <c r="BK9" s="82"/>
-      <c r="BL9" s="82"/>
-      <c r="BM9" s="82"/>
-      <c r="BN9" s="82"/>
-      <c r="BO9" s="82"/>
-      <c r="BP9" s="82"/>
-      <c r="BQ9" s="82"/>
-      <c r="BR9" s="82"/>
-      <c r="BS9" s="82"/>
-      <c r="BT9" s="82"/>
-      <c r="BU9" s="82"/>
-      <c r="BV9" s="82"/>
-      <c r="BW9" s="82"/>
-      <c r="BX9" s="82"/>
-      <c r="BY9" s="82"/>
-      <c r="BZ9" s="82"/>
-      <c r="CA9" s="82"/>
-      <c r="CB9" s="82"/>
-      <c r="CC9" s="82"/>
-      <c r="CD9" s="82"/>
-      <c r="CE9" s="82"/>
-      <c r="CF9" s="82"/>
-      <c r="CG9" s="82"/>
-      <c r="CH9" s="82"/>
-      <c r="CI9" s="82"/>
-      <c r="CJ9" s="82"/>
-      <c r="CK9" s="82"/>
-      <c r="CL9" s="82"/>
-      <c r="CM9" s="82"/>
-      <c r="CN9" s="82"/>
-      <c r="CO9" s="82"/>
-      <c r="CP9" s="82"/>
-      <c r="CQ9" s="82"/>
-      <c r="CR9" s="82"/>
-      <c r="CS9" s="82"/>
-      <c r="CT9" s="82"/>
-      <c r="CU9" s="82"/>
-      <c r="CV9" s="82"/>
-      <c r="CW9" s="82"/>
-      <c r="CX9" s="82"/>
-      <c r="CY9" s="82"/>
-      <c r="CZ9" s="82"/>
-      <c r="DA9" s="82"/>
-      <c r="DB9" s="82"/>
-      <c r="DC9" s="82"/>
-      <c r="DD9" s="82"/>
-      <c r="DE9" s="82"/>
-      <c r="DF9" s="82"/>
-      <c r="DG9" s="82"/>
-      <c r="DH9" s="82"/>
-      <c r="DI9" s="82"/>
-      <c r="DJ9" s="82"/>
-      <c r="DK9" s="82"/>
-      <c r="DL9" s="82"/>
-      <c r="DM9" s="82"/>
-      <c r="DN9" s="82"/>
-      <c r="DO9" s="82"/>
-      <c r="DP9" s="82"/>
-      <c r="DQ9" s="82"/>
-      <c r="DR9" s="82"/>
-      <c r="DS9" s="82"/>
-      <c r="DT9" s="82"/>
-      <c r="DU9" s="82"/>
-      <c r="DV9" s="82"/>
-      <c r="DW9" s="82"/>
-      <c r="DX9" s="82"/>
-      <c r="DY9" s="82"/>
-      <c r="DZ9" s="82"/>
-      <c r="EA9" s="82"/>
-      <c r="EB9" s="82"/>
-      <c r="EC9" s="82"/>
-      <c r="ED9" s="82"/>
-      <c r="EE9" s="82"/>
-      <c r="EF9" s="82"/>
-      <c r="EG9" s="82"/>
-      <c r="EH9" s="82"/>
-      <c r="EI9" s="82"/>
-      <c r="EJ9" s="82"/>
-      <c r="EK9" s="82"/>
-      <c r="EL9" s="82"/>
-      <c r="EM9" s="82"/>
-      <c r="EN9" s="82"/>
-      <c r="EO9" s="82"/>
-      <c r="EP9" s="82"/>
-      <c r="EQ9" s="82"/>
-      <c r="ER9" s="82"/>
-      <c r="ES9" s="82"/>
-      <c r="ET9" s="82"/>
-      <c r="EU9" s="82"/>
-      <c r="EV9" s="82"/>
-      <c r="EW9" s="82"/>
-      <c r="EX9" s="82"/>
-      <c r="EY9" s="82"/>
-      <c r="EZ9" s="82"/>
-      <c r="FA9" s="82"/>
-      <c r="FB9" s="82"/>
-      <c r="FC9" s="82"/>
-      <c r="FD9" s="82"/>
-      <c r="FE9" s="82"/>
-      <c r="FF9" s="82"/>
-      <c r="FG9" s="82"/>
-      <c r="FH9" s="82"/>
-      <c r="FI9" s="82"/>
-      <c r="FJ9" s="82"/>
-      <c r="FK9" s="82"/>
-      <c r="FL9" s="82"/>
-      <c r="FM9" s="82"/>
-      <c r="FN9" s="82"/>
-      <c r="FO9" s="82"/>
-      <c r="FP9" s="82"/>
-      <c r="FQ9" s="82"/>
-      <c r="FR9" s="82"/>
-      <c r="FS9" s="82"/>
-      <c r="FT9" s="82"/>
-      <c r="FU9" s="82"/>
-      <c r="FV9" s="82"/>
-      <c r="FW9" s="82"/>
-      <c r="FX9" s="82"/>
-      <c r="FY9" s="82"/>
-      <c r="FZ9" s="82"/>
-      <c r="GA9" s="82"/>
-      <c r="GB9" s="82"/>
-      <c r="GC9" s="82"/>
-      <c r="GD9" s="82"/>
-      <c r="GE9" s="82"/>
-      <c r="GF9" s="82"/>
-      <c r="GG9" s="82"/>
-      <c r="GH9" s="82"/>
-      <c r="GI9" s="82"/>
-      <c r="GJ9" s="82"/>
-      <c r="GK9" s="82"/>
-      <c r="GL9" s="82"/>
-      <c r="GM9" s="82"/>
-      <c r="GN9" s="82"/>
-      <c r="GO9" s="82"/>
-      <c r="GP9" s="82"/>
-      <c r="GQ9" s="82"/>
-      <c r="GR9" s="82"/>
-      <c r="GS9" s="82"/>
-      <c r="GT9" s="82"/>
-      <c r="GU9" s="82"/>
-      <c r="GV9" s="82"/>
-      <c r="GW9" s="82"/>
-      <c r="GX9" s="82"/>
-      <c r="GY9" s="82"/>
-      <c r="GZ9" s="82"/>
-      <c r="HA9" s="82"/>
-      <c r="HB9" s="82"/>
-      <c r="HC9" s="82"/>
-      <c r="HD9" s="82"/>
-      <c r="HE9" s="82"/>
-      <c r="HF9" s="82"/>
-      <c r="HG9" s="82"/>
-      <c r="HH9" s="82"/>
-      <c r="HI9" s="82"/>
-      <c r="HJ9" s="82"/>
-      <c r="HK9" s="82"/>
-      <c r="HL9" s="82"/>
-      <c r="HM9" s="82"/>
-      <c r="HN9" s="82"/>
-      <c r="HO9" s="82"/>
-      <c r="HP9" s="82"/>
-      <c r="HQ9" s="82"/>
-      <c r="HR9" s="82"/>
-      <c r="HS9" s="82"/>
-      <c r="HT9" s="82"/>
-      <c r="HU9" s="82"/>
-      <c r="HV9" s="82"/>
-      <c r="HW9" s="82"/>
-      <c r="HX9" s="82"/>
-      <c r="HY9" s="82"/>
-      <c r="HZ9" s="82"/>
-      <c r="IA9" s="82"/>
-      <c r="IB9" s="82"/>
-      <c r="IC9" s="82"/>
-      <c r="ID9" s="82"/>
-      <c r="IE9" s="82"/>
-      <c r="IF9" s="82"/>
-      <c r="IG9" s="82"/>
-      <c r="IH9" s="82"/>
-      <c r="II9" s="82"/>
-      <c r="IJ9" s="82"/>
-      <c r="IK9" s="82"/>
-      <c r="IL9" s="82"/>
-      <c r="IM9" s="82"/>
-      <c r="IN9" s="82"/>
-      <c r="IO9" s="82"/>
-      <c r="IP9" s="82"/>
-      <c r="IQ9" s="82"/>
-      <c r="IR9" s="82"/>
-      <c r="IS9" s="82"/>
-      <c r="IT9" s="82"/>
-      <c r="IU9" s="82"/>
-      <c r="IV9" s="82"/>
-      <c r="IW9" s="82"/>
-      <c r="IX9" s="82"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="80"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
+      <c r="AD9" s="80"/>
+      <c r="AE9" s="80"/>
+      <c r="AF9" s="80"/>
+      <c r="AG9" s="80"/>
+      <c r="AH9" s="80"/>
+      <c r="AI9" s="80"/>
+      <c r="AJ9" s="80"/>
+      <c r="AK9" s="80"/>
+      <c r="AL9" s="80"/>
+      <c r="AM9" s="80"/>
+      <c r="AN9" s="80"/>
+      <c r="AO9" s="80"/>
+      <c r="AP9" s="80"/>
+      <c r="AQ9" s="80"/>
+      <c r="AR9" s="80"/>
+      <c r="AS9" s="80"/>
+      <c r="AT9" s="80"/>
+      <c r="AU9" s="80"/>
+      <c r="AV9" s="80"/>
+      <c r="AW9" s="80"/>
+      <c r="AX9" s="80"/>
+      <c r="AY9" s="80"/>
+      <c r="AZ9" s="80"/>
+      <c r="BA9" s="80"/>
+      <c r="BB9" s="80"/>
+      <c r="BC9" s="80"/>
+      <c r="BD9" s="80"/>
+      <c r="BE9" s="80"/>
+      <c r="BF9" s="80"/>
+      <c r="BG9" s="80"/>
+      <c r="BH9" s="80"/>
+      <c r="BI9" s="80"/>
+      <c r="BJ9" s="80"/>
+      <c r="BK9" s="80"/>
+      <c r="BL9" s="80"/>
+      <c r="BM9" s="80"/>
+      <c r="BN9" s="80"/>
+      <c r="BO9" s="80"/>
+      <c r="BP9" s="80"/>
+      <c r="BQ9" s="80"/>
+      <c r="BR9" s="80"/>
+      <c r="BS9" s="80"/>
+      <c r="BT9" s="80"/>
+      <c r="BU9" s="80"/>
+      <c r="BV9" s="80"/>
+      <c r="BW9" s="80"/>
+      <c r="BX9" s="80"/>
+      <c r="BY9" s="80"/>
+      <c r="BZ9" s="80"/>
+      <c r="CA9" s="80"/>
+      <c r="CB9" s="80"/>
+      <c r="CC9" s="80"/>
+      <c r="CD9" s="80"/>
+      <c r="CE9" s="80"/>
+      <c r="CF9" s="80"/>
+      <c r="CG9" s="80"/>
+      <c r="CH9" s="80"/>
+      <c r="CI9" s="80"/>
+      <c r="CJ9" s="80"/>
+      <c r="CK9" s="80"/>
+      <c r="CL9" s="80"/>
+      <c r="CM9" s="80"/>
+      <c r="CN9" s="80"/>
+      <c r="CO9" s="80"/>
+      <c r="CP9" s="80"/>
+      <c r="CQ9" s="80"/>
+      <c r="CR9" s="80"/>
+      <c r="CS9" s="80"/>
+      <c r="CT9" s="80"/>
+      <c r="CU9" s="80"/>
+      <c r="CV9" s="80"/>
+      <c r="CW9" s="80"/>
+      <c r="CX9" s="80"/>
+      <c r="CY9" s="80"/>
+      <c r="CZ9" s="80"/>
+      <c r="DA9" s="80"/>
+      <c r="DB9" s="80"/>
+      <c r="DC9" s="80"/>
+      <c r="DD9" s="80"/>
+      <c r="DE9" s="80"/>
+      <c r="DF9" s="80"/>
+      <c r="DG9" s="80"/>
+      <c r="DH9" s="80"/>
+      <c r="DI9" s="80"/>
+      <c r="DJ9" s="80"/>
+      <c r="DK9" s="80"/>
+      <c r="DL9" s="80"/>
+      <c r="DM9" s="80"/>
+      <c r="DN9" s="80"/>
+      <c r="DO9" s="80"/>
+      <c r="DP9" s="80"/>
+      <c r="DQ9" s="80"/>
+      <c r="DR9" s="80"/>
+      <c r="DS9" s="80"/>
+      <c r="DT9" s="80"/>
+      <c r="DU9" s="80"/>
+      <c r="DV9" s="80"/>
+      <c r="DW9" s="80"/>
+      <c r="DX9" s="80"/>
+      <c r="DY9" s="80"/>
+      <c r="DZ9" s="80"/>
+      <c r="EA9" s="80"/>
+      <c r="EB9" s="80"/>
+      <c r="EC9" s="80"/>
+      <c r="ED9" s="80"/>
+      <c r="EE9" s="80"/>
+      <c r="EF9" s="80"/>
+      <c r="EG9" s="80"/>
+      <c r="EH9" s="80"/>
+      <c r="EI9" s="80"/>
+      <c r="EJ9" s="80"/>
+      <c r="EK9" s="80"/>
+      <c r="EL9" s="80"/>
+      <c r="EM9" s="80"/>
+      <c r="EN9" s="80"/>
+      <c r="EO9" s="80"/>
+      <c r="EP9" s="80"/>
+      <c r="EQ9" s="80"/>
+      <c r="ER9" s="80"/>
+      <c r="ES9" s="80"/>
+      <c r="ET9" s="80"/>
+      <c r="EU9" s="80"/>
+      <c r="EV9" s="80"/>
+      <c r="EW9" s="80"/>
+      <c r="EX9" s="80"/>
+      <c r="EY9" s="80"/>
+      <c r="EZ9" s="80"/>
+      <c r="FA9" s="80"/>
+      <c r="FB9" s="80"/>
+      <c r="FC9" s="80"/>
+      <c r="FD9" s="80"/>
+      <c r="FE9" s="80"/>
+      <c r="FF9" s="80"/>
+      <c r="FG9" s="80"/>
+      <c r="FH9" s="80"/>
+      <c r="FI9" s="80"/>
+      <c r="FJ9" s="80"/>
+      <c r="FK9" s="80"/>
+      <c r="FL9" s="80"/>
+      <c r="FM9" s="80"/>
+      <c r="FN9" s="80"/>
+      <c r="FO9" s="80"/>
+      <c r="FP9" s="80"/>
+      <c r="FQ9" s="80"/>
+      <c r="FR9" s="80"/>
+      <c r="FS9" s="80"/>
+      <c r="FT9" s="80"/>
+      <c r="FU9" s="80"/>
+      <c r="FV9" s="80"/>
+      <c r="FW9" s="80"/>
+      <c r="FX9" s="80"/>
+      <c r="FY9" s="80"/>
+      <c r="FZ9" s="80"/>
+      <c r="GA9" s="80"/>
+      <c r="GB9" s="80"/>
+      <c r="GC9" s="80"/>
+      <c r="GD9" s="80"/>
+      <c r="GE9" s="80"/>
+      <c r="GF9" s="80"/>
+      <c r="GG9" s="80"/>
+      <c r="GH9" s="80"/>
+      <c r="GI9" s="80"/>
+      <c r="GJ9" s="80"/>
+      <c r="GK9" s="80"/>
+      <c r="GL9" s="80"/>
+      <c r="GM9" s="80"/>
+      <c r="GN9" s="80"/>
+      <c r="GO9" s="80"/>
+      <c r="GP9" s="80"/>
+      <c r="GQ9" s="80"/>
+      <c r="GR9" s="80"/>
+      <c r="GS9" s="80"/>
+      <c r="GT9" s="80"/>
+      <c r="GU9" s="80"/>
+      <c r="GV9" s="80"/>
+      <c r="GW9" s="80"/>
+      <c r="GX9" s="80"/>
+      <c r="GY9" s="80"/>
+      <c r="GZ9" s="80"/>
+      <c r="HA9" s="80"/>
+      <c r="HB9" s="80"/>
+      <c r="HC9" s="80"/>
+      <c r="HD9" s="80"/>
+      <c r="HE9" s="80"/>
+      <c r="HF9" s="80"/>
+      <c r="HG9" s="80"/>
+      <c r="HH9" s="80"/>
+      <c r="HI9" s="80"/>
+      <c r="HJ9" s="80"/>
+      <c r="HK9" s="80"/>
+      <c r="HL9" s="80"/>
+      <c r="HM9" s="80"/>
+      <c r="HN9" s="80"/>
+      <c r="HO9" s="80"/>
+      <c r="HP9" s="80"/>
+      <c r="HQ9" s="80"/>
+      <c r="HR9" s="80"/>
+      <c r="HS9" s="80"/>
+      <c r="HT9" s="80"/>
+      <c r="HU9" s="80"/>
+      <c r="HV9" s="80"/>
+      <c r="HW9" s="80"/>
+      <c r="HX9" s="80"/>
+      <c r="HY9" s="80"/>
+      <c r="HZ9" s="80"/>
+      <c r="IA9" s="80"/>
+      <c r="IB9" s="80"/>
+      <c r="IC9" s="80"/>
+      <c r="ID9" s="80"/>
+      <c r="IE9" s="80"/>
+      <c r="IF9" s="80"/>
+      <c r="IG9" s="80"/>
+      <c r="IH9" s="80"/>
+      <c r="II9" s="80"/>
+      <c r="IJ9" s="80"/>
+      <c r="IK9" s="80"/>
+      <c r="IL9" s="80"/>
+      <c r="IM9" s="80"/>
+      <c r="IN9" s="80"/>
+      <c r="IO9" s="80"/>
+      <c r="IP9" s="80"/>
+      <c r="IQ9" s="80"/>
+      <c r="IR9" s="80"/>
+      <c r="IS9" s="80"/>
+      <c r="IT9" s="80"/>
+      <c r="IU9" s="80"/>
+      <c r="IV9" s="80"/>
+      <c r="IW9" s="80"/>
+      <c r="IX9" s="80"/>
     </row>
     <row r="10" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A10" s="92"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="56" t="s">
         <v>41</v>
       </c>
@@ -4807,7 +4785,7 @@
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="73"/>
+      <c r="K10" s="71"/>
       <c r="L10" s="21"/>
       <c r="M10" s="51"/>
       <c r="N10" s="51"/>
@@ -5057,7 +5035,7 @@
       <c r="IX10" s="51"/>
     </row>
     <row r="11" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A11" s="92"/>
+      <c r="A11" s="95"/>
       <c r="B11" s="56" t="s">
         <v>44</v>
       </c>
@@ -5076,8 +5054,8 @@
         <v>39</v>
       </c>
       <c r="I11" s="20"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="73"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="71"/>
       <c r="L11" s="21"/>
       <c r="M11" s="51"/>
       <c r="N11" s="51"/>
@@ -5327,7 +5305,7 @@
       <c r="IX11" s="51"/>
     </row>
     <row r="12" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="94" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="63" t="s">
@@ -5350,8 +5328,8 @@
       <c r="I12" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="83"/>
-      <c r="K12" s="84"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="65" t="s">
         <v>51</v>
       </c>
@@ -5603,7 +5581,7 @@
       <c r="IX12" s="51"/>
     </row>
     <row r="13" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A13" s="92"/>
+      <c r="A13" s="95"/>
       <c r="B13" s="63" t="s">
         <v>52</v>
       </c>
@@ -5621,7 +5599,7 @@
       </c>
       <c r="I13" s="65"/>
       <c r="J13" s="64"/>
-      <c r="K13" s="84"/>
+      <c r="K13" s="82"/>
       <c r="L13" s="64" t="s">
         <v>55</v>
       </c>
@@ -5873,7 +5851,7 @@
       <c r="IX13" s="51"/>
     </row>
     <row r="14" spans="1:258" s="55" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A14" s="93"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="63" t="s">
         <v>56</v>
       </c>
@@ -5892,260 +5870,260 @@
         <v>39</v>
       </c>
       <c r="I14" s="64"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="84"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="82"/>
       <c r="L14" s="65">
         <v>1</v>
       </c>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="85"/>
-      <c r="Y14" s="85"/>
-      <c r="Z14" s="85"/>
-      <c r="AA14" s="85"/>
-      <c r="AB14" s="85"/>
-      <c r="AC14" s="85"/>
-      <c r="AD14" s="85"/>
-      <c r="AE14" s="85"/>
-      <c r="AF14" s="85"/>
-      <c r="AG14" s="85"/>
-      <c r="AH14" s="85"/>
-      <c r="AI14" s="85"/>
-      <c r="AJ14" s="85"/>
-      <c r="AK14" s="85"/>
-      <c r="AL14" s="85"/>
-      <c r="AM14" s="85"/>
-      <c r="AN14" s="85"/>
-      <c r="AO14" s="85"/>
-      <c r="AP14" s="85"/>
-      <c r="AQ14" s="85"/>
-      <c r="AR14" s="85"/>
-      <c r="AS14" s="85"/>
-      <c r="AT14" s="85"/>
-      <c r="AU14" s="85"/>
-      <c r="AV14" s="85"/>
-      <c r="AW14" s="85"/>
-      <c r="AX14" s="85"/>
-      <c r="AY14" s="85"/>
-      <c r="AZ14" s="85"/>
-      <c r="BA14" s="85"/>
-      <c r="BB14" s="85"/>
-      <c r="BC14" s="85"/>
-      <c r="BD14" s="85"/>
-      <c r="BE14" s="85"/>
-      <c r="BF14" s="85"/>
-      <c r="BG14" s="85"/>
-      <c r="BH14" s="85"/>
-      <c r="BI14" s="85"/>
-      <c r="BJ14" s="85"/>
-      <c r="BK14" s="85"/>
-      <c r="BL14" s="85"/>
-      <c r="BM14" s="85"/>
-      <c r="BN14" s="85"/>
-      <c r="BO14" s="85"/>
-      <c r="BP14" s="85"/>
-      <c r="BQ14" s="85"/>
-      <c r="BR14" s="85"/>
-      <c r="BS14" s="85"/>
-      <c r="BT14" s="85"/>
-      <c r="BU14" s="85"/>
-      <c r="BV14" s="85"/>
-      <c r="BW14" s="85"/>
-      <c r="BX14" s="85"/>
-      <c r="BY14" s="85"/>
-      <c r="BZ14" s="85"/>
-      <c r="CA14" s="85"/>
-      <c r="CB14" s="85"/>
-      <c r="CC14" s="85"/>
-      <c r="CD14" s="85"/>
-      <c r="CE14" s="85"/>
-      <c r="CF14" s="85"/>
-      <c r="CG14" s="85"/>
-      <c r="CH14" s="85"/>
-      <c r="CI14" s="85"/>
-      <c r="CJ14" s="85"/>
-      <c r="CK14" s="85"/>
-      <c r="CL14" s="85"/>
-      <c r="CM14" s="85"/>
-      <c r="CN14" s="85"/>
-      <c r="CO14" s="85"/>
-      <c r="CP14" s="85"/>
-      <c r="CQ14" s="85"/>
-      <c r="CR14" s="85"/>
-      <c r="CS14" s="85"/>
-      <c r="CT14" s="85"/>
-      <c r="CU14" s="85"/>
-      <c r="CV14" s="85"/>
-      <c r="CW14" s="85"/>
-      <c r="CX14" s="85"/>
-      <c r="CY14" s="85"/>
-      <c r="CZ14" s="85"/>
-      <c r="DA14" s="85"/>
-      <c r="DB14" s="85"/>
-      <c r="DC14" s="85"/>
-      <c r="DD14" s="85"/>
-      <c r="DE14" s="85"/>
-      <c r="DF14" s="85"/>
-      <c r="DG14" s="85"/>
-      <c r="DH14" s="85"/>
-      <c r="DI14" s="85"/>
-      <c r="DJ14" s="85"/>
-      <c r="DK14" s="85"/>
-      <c r="DL14" s="85"/>
-      <c r="DM14" s="85"/>
-      <c r="DN14" s="85"/>
-      <c r="DO14" s="85"/>
-      <c r="DP14" s="85"/>
-      <c r="DQ14" s="85"/>
-      <c r="DR14" s="85"/>
-      <c r="DS14" s="85"/>
-      <c r="DT14" s="85"/>
-      <c r="DU14" s="85"/>
-      <c r="DV14" s="85"/>
-      <c r="DW14" s="85"/>
-      <c r="DX14" s="85"/>
-      <c r="DY14" s="85"/>
-      <c r="DZ14" s="85"/>
-      <c r="EA14" s="85"/>
-      <c r="EB14" s="85"/>
-      <c r="EC14" s="85"/>
-      <c r="ED14" s="85"/>
-      <c r="EE14" s="85"/>
-      <c r="EF14" s="85"/>
-      <c r="EG14" s="85"/>
-      <c r="EH14" s="85"/>
-      <c r="EI14" s="85"/>
-      <c r="EJ14" s="85"/>
-      <c r="EK14" s="85"/>
-      <c r="EL14" s="85"/>
-      <c r="EM14" s="85"/>
-      <c r="EN14" s="85"/>
-      <c r="EO14" s="85"/>
-      <c r="EP14" s="85"/>
-      <c r="EQ14" s="85"/>
-      <c r="ER14" s="85"/>
-      <c r="ES14" s="85"/>
-      <c r="ET14" s="85"/>
-      <c r="EU14" s="85"/>
-      <c r="EV14" s="85"/>
-      <c r="EW14" s="85"/>
-      <c r="EX14" s="85"/>
-      <c r="EY14" s="85"/>
-      <c r="EZ14" s="85"/>
-      <c r="FA14" s="85"/>
-      <c r="FB14" s="85"/>
-      <c r="FC14" s="85"/>
-      <c r="FD14" s="85"/>
-      <c r="FE14" s="85"/>
-      <c r="FF14" s="85"/>
-      <c r="FG14" s="85"/>
-      <c r="FH14" s="85"/>
-      <c r="FI14" s="85"/>
-      <c r="FJ14" s="85"/>
-      <c r="FK14" s="85"/>
-      <c r="FL14" s="85"/>
-      <c r="FM14" s="85"/>
-      <c r="FN14" s="85"/>
-      <c r="FO14" s="85"/>
-      <c r="FP14" s="85"/>
-      <c r="FQ14" s="85"/>
-      <c r="FR14" s="85"/>
-      <c r="FS14" s="85"/>
-      <c r="FT14" s="85"/>
-      <c r="FU14" s="85"/>
-      <c r="FV14" s="85"/>
-      <c r="FW14" s="85"/>
-      <c r="FX14" s="85"/>
-      <c r="FY14" s="85"/>
-      <c r="FZ14" s="85"/>
-      <c r="GA14" s="85"/>
-      <c r="GB14" s="85"/>
-      <c r="GC14" s="85"/>
-      <c r="GD14" s="85"/>
-      <c r="GE14" s="85"/>
-      <c r="GF14" s="85"/>
-      <c r="GG14" s="85"/>
-      <c r="GH14" s="85"/>
-      <c r="GI14" s="85"/>
-      <c r="GJ14" s="85"/>
-      <c r="GK14" s="85"/>
-      <c r="GL14" s="85"/>
-      <c r="GM14" s="85"/>
-      <c r="GN14" s="85"/>
-      <c r="GO14" s="85"/>
-      <c r="GP14" s="85"/>
-      <c r="GQ14" s="85"/>
-      <c r="GR14" s="85"/>
-      <c r="GS14" s="85"/>
-      <c r="GT14" s="85"/>
-      <c r="GU14" s="85"/>
-      <c r="GV14" s="85"/>
-      <c r="GW14" s="85"/>
-      <c r="GX14" s="85"/>
-      <c r="GY14" s="85"/>
-      <c r="GZ14" s="85"/>
-      <c r="HA14" s="85"/>
-      <c r="HB14" s="85"/>
-      <c r="HC14" s="85"/>
-      <c r="HD14" s="85"/>
-      <c r="HE14" s="85"/>
-      <c r="HF14" s="85"/>
-      <c r="HG14" s="85"/>
-      <c r="HH14" s="85"/>
-      <c r="HI14" s="85"/>
-      <c r="HJ14" s="85"/>
-      <c r="HK14" s="85"/>
-      <c r="HL14" s="85"/>
-      <c r="HM14" s="85"/>
-      <c r="HN14" s="85"/>
-      <c r="HO14" s="85"/>
-      <c r="HP14" s="85"/>
-      <c r="HQ14" s="85"/>
-      <c r="HR14" s="85"/>
-      <c r="HS14" s="85"/>
-      <c r="HT14" s="85"/>
-      <c r="HU14" s="85"/>
-      <c r="HV14" s="85"/>
-      <c r="HW14" s="85"/>
-      <c r="HX14" s="85"/>
-      <c r="HY14" s="85"/>
-      <c r="HZ14" s="85"/>
-      <c r="IA14" s="85"/>
-      <c r="IB14" s="85"/>
-      <c r="IC14" s="85"/>
-      <c r="ID14" s="85"/>
-      <c r="IE14" s="85"/>
-      <c r="IF14" s="85"/>
-      <c r="IG14" s="85"/>
-      <c r="IH14" s="85"/>
-      <c r="II14" s="85"/>
-      <c r="IJ14" s="85"/>
-      <c r="IK14" s="85"/>
-      <c r="IL14" s="85"/>
-      <c r="IM14" s="85"/>
-      <c r="IN14" s="85"/>
-      <c r="IO14" s="85"/>
-      <c r="IP14" s="85"/>
-      <c r="IQ14" s="85"/>
-      <c r="IR14" s="85"/>
-      <c r="IS14" s="85"/>
-      <c r="IT14" s="85"/>
-      <c r="IU14" s="85"/>
-      <c r="IV14" s="85"/>
-      <c r="IW14" s="85"/>
-      <c r="IX14" s="85"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="83"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="83"/>
+      <c r="X14" s="83"/>
+      <c r="Y14" s="83"/>
+      <c r="Z14" s="83"/>
+      <c r="AA14" s="83"/>
+      <c r="AB14" s="83"/>
+      <c r="AC14" s="83"/>
+      <c r="AD14" s="83"/>
+      <c r="AE14" s="83"/>
+      <c r="AF14" s="83"/>
+      <c r="AG14" s="83"/>
+      <c r="AH14" s="83"/>
+      <c r="AI14" s="83"/>
+      <c r="AJ14" s="83"/>
+      <c r="AK14" s="83"/>
+      <c r="AL14" s="83"/>
+      <c r="AM14" s="83"/>
+      <c r="AN14" s="83"/>
+      <c r="AO14" s="83"/>
+      <c r="AP14" s="83"/>
+      <c r="AQ14" s="83"/>
+      <c r="AR14" s="83"/>
+      <c r="AS14" s="83"/>
+      <c r="AT14" s="83"/>
+      <c r="AU14" s="83"/>
+      <c r="AV14" s="83"/>
+      <c r="AW14" s="83"/>
+      <c r="AX14" s="83"/>
+      <c r="AY14" s="83"/>
+      <c r="AZ14" s="83"/>
+      <c r="BA14" s="83"/>
+      <c r="BB14" s="83"/>
+      <c r="BC14" s="83"/>
+      <c r="BD14" s="83"/>
+      <c r="BE14" s="83"/>
+      <c r="BF14" s="83"/>
+      <c r="BG14" s="83"/>
+      <c r="BH14" s="83"/>
+      <c r="BI14" s="83"/>
+      <c r="BJ14" s="83"/>
+      <c r="BK14" s="83"/>
+      <c r="BL14" s="83"/>
+      <c r="BM14" s="83"/>
+      <c r="BN14" s="83"/>
+      <c r="BO14" s="83"/>
+      <c r="BP14" s="83"/>
+      <c r="BQ14" s="83"/>
+      <c r="BR14" s="83"/>
+      <c r="BS14" s="83"/>
+      <c r="BT14" s="83"/>
+      <c r="BU14" s="83"/>
+      <c r="BV14" s="83"/>
+      <c r="BW14" s="83"/>
+      <c r="BX14" s="83"/>
+      <c r="BY14" s="83"/>
+      <c r="BZ14" s="83"/>
+      <c r="CA14" s="83"/>
+      <c r="CB14" s="83"/>
+      <c r="CC14" s="83"/>
+      <c r="CD14" s="83"/>
+      <c r="CE14" s="83"/>
+      <c r="CF14" s="83"/>
+      <c r="CG14" s="83"/>
+      <c r="CH14" s="83"/>
+      <c r="CI14" s="83"/>
+      <c r="CJ14" s="83"/>
+      <c r="CK14" s="83"/>
+      <c r="CL14" s="83"/>
+      <c r="CM14" s="83"/>
+      <c r="CN14" s="83"/>
+      <c r="CO14" s="83"/>
+      <c r="CP14" s="83"/>
+      <c r="CQ14" s="83"/>
+      <c r="CR14" s="83"/>
+      <c r="CS14" s="83"/>
+      <c r="CT14" s="83"/>
+      <c r="CU14" s="83"/>
+      <c r="CV14" s="83"/>
+      <c r="CW14" s="83"/>
+      <c r="CX14" s="83"/>
+      <c r="CY14" s="83"/>
+      <c r="CZ14" s="83"/>
+      <c r="DA14" s="83"/>
+      <c r="DB14" s="83"/>
+      <c r="DC14" s="83"/>
+      <c r="DD14" s="83"/>
+      <c r="DE14" s="83"/>
+      <c r="DF14" s="83"/>
+      <c r="DG14" s="83"/>
+      <c r="DH14" s="83"/>
+      <c r="DI14" s="83"/>
+      <c r="DJ14" s="83"/>
+      <c r="DK14" s="83"/>
+      <c r="DL14" s="83"/>
+      <c r="DM14" s="83"/>
+      <c r="DN14" s="83"/>
+      <c r="DO14" s="83"/>
+      <c r="DP14" s="83"/>
+      <c r="DQ14" s="83"/>
+      <c r="DR14" s="83"/>
+      <c r="DS14" s="83"/>
+      <c r="DT14" s="83"/>
+      <c r="DU14" s="83"/>
+      <c r="DV14" s="83"/>
+      <c r="DW14" s="83"/>
+      <c r="DX14" s="83"/>
+      <c r="DY14" s="83"/>
+      <c r="DZ14" s="83"/>
+      <c r="EA14" s="83"/>
+      <c r="EB14" s="83"/>
+      <c r="EC14" s="83"/>
+      <c r="ED14" s="83"/>
+      <c r="EE14" s="83"/>
+      <c r="EF14" s="83"/>
+      <c r="EG14" s="83"/>
+      <c r="EH14" s="83"/>
+      <c r="EI14" s="83"/>
+      <c r="EJ14" s="83"/>
+      <c r="EK14" s="83"/>
+      <c r="EL14" s="83"/>
+      <c r="EM14" s="83"/>
+      <c r="EN14" s="83"/>
+      <c r="EO14" s="83"/>
+      <c r="EP14" s="83"/>
+      <c r="EQ14" s="83"/>
+      <c r="ER14" s="83"/>
+      <c r="ES14" s="83"/>
+      <c r="ET14" s="83"/>
+      <c r="EU14" s="83"/>
+      <c r="EV14" s="83"/>
+      <c r="EW14" s="83"/>
+      <c r="EX14" s="83"/>
+      <c r="EY14" s="83"/>
+      <c r="EZ14" s="83"/>
+      <c r="FA14" s="83"/>
+      <c r="FB14" s="83"/>
+      <c r="FC14" s="83"/>
+      <c r="FD14" s="83"/>
+      <c r="FE14" s="83"/>
+      <c r="FF14" s="83"/>
+      <c r="FG14" s="83"/>
+      <c r="FH14" s="83"/>
+      <c r="FI14" s="83"/>
+      <c r="FJ14" s="83"/>
+      <c r="FK14" s="83"/>
+      <c r="FL14" s="83"/>
+      <c r="FM14" s="83"/>
+      <c r="FN14" s="83"/>
+      <c r="FO14" s="83"/>
+      <c r="FP14" s="83"/>
+      <c r="FQ14" s="83"/>
+      <c r="FR14" s="83"/>
+      <c r="FS14" s="83"/>
+      <c r="FT14" s="83"/>
+      <c r="FU14" s="83"/>
+      <c r="FV14" s="83"/>
+      <c r="FW14" s="83"/>
+      <c r="FX14" s="83"/>
+      <c r="FY14" s="83"/>
+      <c r="FZ14" s="83"/>
+      <c r="GA14" s="83"/>
+      <c r="GB14" s="83"/>
+      <c r="GC14" s="83"/>
+      <c r="GD14" s="83"/>
+      <c r="GE14" s="83"/>
+      <c r="GF14" s="83"/>
+      <c r="GG14" s="83"/>
+      <c r="GH14" s="83"/>
+      <c r="GI14" s="83"/>
+      <c r="GJ14" s="83"/>
+      <c r="GK14" s="83"/>
+      <c r="GL14" s="83"/>
+      <c r="GM14" s="83"/>
+      <c r="GN14" s="83"/>
+      <c r="GO14" s="83"/>
+      <c r="GP14" s="83"/>
+      <c r="GQ14" s="83"/>
+      <c r="GR14" s="83"/>
+      <c r="GS14" s="83"/>
+      <c r="GT14" s="83"/>
+      <c r="GU14" s="83"/>
+      <c r="GV14" s="83"/>
+      <c r="GW14" s="83"/>
+      <c r="GX14" s="83"/>
+      <c r="GY14" s="83"/>
+      <c r="GZ14" s="83"/>
+      <c r="HA14" s="83"/>
+      <c r="HB14" s="83"/>
+      <c r="HC14" s="83"/>
+      <c r="HD14" s="83"/>
+      <c r="HE14" s="83"/>
+      <c r="HF14" s="83"/>
+      <c r="HG14" s="83"/>
+      <c r="HH14" s="83"/>
+      <c r="HI14" s="83"/>
+      <c r="HJ14" s="83"/>
+      <c r="HK14" s="83"/>
+      <c r="HL14" s="83"/>
+      <c r="HM14" s="83"/>
+      <c r="HN14" s="83"/>
+      <c r="HO14" s="83"/>
+      <c r="HP14" s="83"/>
+      <c r="HQ14" s="83"/>
+      <c r="HR14" s="83"/>
+      <c r="HS14" s="83"/>
+      <c r="HT14" s="83"/>
+      <c r="HU14" s="83"/>
+      <c r="HV14" s="83"/>
+      <c r="HW14" s="83"/>
+      <c r="HX14" s="83"/>
+      <c r="HY14" s="83"/>
+      <c r="HZ14" s="83"/>
+      <c r="IA14" s="83"/>
+      <c r="IB14" s="83"/>
+      <c r="IC14" s="83"/>
+      <c r="ID14" s="83"/>
+      <c r="IE14" s="83"/>
+      <c r="IF14" s="83"/>
+      <c r="IG14" s="83"/>
+      <c r="IH14" s="83"/>
+      <c r="II14" s="83"/>
+      <c r="IJ14" s="83"/>
+      <c r="IK14" s="83"/>
+      <c r="IL14" s="83"/>
+      <c r="IM14" s="83"/>
+      <c r="IN14" s="83"/>
+      <c r="IO14" s="83"/>
+      <c r="IP14" s="83"/>
+      <c r="IQ14" s="83"/>
+      <c r="IR14" s="83"/>
+      <c r="IS14" s="83"/>
+      <c r="IT14" s="83"/>
+      <c r="IU14" s="83"/>
+      <c r="IV14" s="83"/>
+      <c r="IW14" s="83"/>
+      <c r="IX14" s="83"/>
     </row>
     <row r="15" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A15" s="92"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="63" t="s">
         <v>58</v>
       </c>
@@ -6165,7 +6143,7 @@
       </c>
       <c r="I15" s="65"/>
       <c r="J15" s="64"/>
-      <c r="K15" s="84"/>
+      <c r="K15" s="82"/>
       <c r="L15" s="65" t="s">
         <v>51</v>
       </c>
@@ -6417,12 +6395,12 @@
       <c r="IX15" s="51"/>
     </row>
     <row r="16" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A16" s="92"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="95"/>
+      <c r="B16" s="56" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>26</v>
@@ -6430,12 +6408,12 @@
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="66" t="s">
-        <v>64</v>
+      <c r="H16" s="57" t="s">
+        <v>165</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="73"/>
+      <c r="K16" s="71"/>
       <c r="L16" s="21"/>
       <c r="M16" s="51"/>
       <c r="N16" s="51"/>
@@ -6685,12 +6663,12 @@
       <c r="IX16" s="51"/>
     </row>
     <row r="17" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A17" s="94"/>
+      <c r="A17" s="97"/>
       <c r="B17" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>18</v>
@@ -6698,7 +6676,7 @@
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
       <c r="G17" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H17" s="20" t="s">
         <v>39</v>
@@ -6706,10 +6684,10 @@
       <c r="I17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="74"/>
-      <c r="K17" s="73"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M17" s="51"/>
       <c r="N17" s="51"/>
@@ -6969,7 +6947,7 @@
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
-      <c r="K18" s="73"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="21"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
@@ -7219,14 +7197,14 @@
       <c r="IX18" s="24"/>
     </row>
     <row r="19" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>71</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>26</v>
@@ -7235,11 +7213,11 @@
       <c r="F19" s="27"/>
       <c r="G19" s="29"/>
       <c r="H19" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I19" s="26"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="86"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="84"/>
       <c r="L19" s="36"/>
       <c r="M19" s="51"/>
       <c r="N19" s="51"/>
@@ -7489,15 +7467,15 @@
       <c r="IX19" s="51"/>
     </row>
     <row r="20" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A20" s="96"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>75</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
@@ -7757,25 +7735,25 @@
       <c r="IX20" s="51"/>
     </row>
     <row r="21" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A21" s="96"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="68" t="s">
-        <v>78</v>
+      <c r="G21" s="66"/>
+      <c r="H21" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="I21" s="21"/>
       <c r="J21" s="20"/>
-      <c r="K21" s="73"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="21"/>
       <c r="M21" s="51"/>
       <c r="N21" s="51"/>
@@ -8025,12 +8003,12 @@
       <c r="IX21" s="51"/>
     </row>
     <row r="22" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A22" s="96"/>
-      <c r="B22" s="20" t="s">
-        <v>79</v>
+      <c r="A22" s="99"/>
+      <c r="B22" s="56" t="s">
+        <v>77</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>18</v>
@@ -8038,14 +8016,14 @@
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
       <c r="G22" s="64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" s="20" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="20"/>
-      <c r="K22" s="73"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="21"/>
       <c r="M22" s="51"/>
       <c r="N22" s="51"/>
@@ -8295,25 +8273,25 @@
       <c r="IX22" s="51"/>
     </row>
     <row r="23" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A23" s="96"/>
+      <c r="A23" s="99"/>
       <c r="B23" s="56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="66"/>
       <c r="H23" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="20"/>
-      <c r="K23" s="73"/>
+      <c r="K23" s="71"/>
       <c r="L23" s="21"/>
       <c r="M23" s="51"/>
       <c r="N23" s="51"/>
@@ -8563,25 +8541,25 @@
       <c r="IX23" s="51"/>
     </row>
     <row r="24" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A24" s="96"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="66"/>
       <c r="H24" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="20"/>
-      <c r="K24" s="73"/>
+      <c r="K24" s="71"/>
       <c r="L24" s="21"/>
       <c r="M24" s="51"/>
       <c r="N24" s="51"/>
@@ -8831,23 +8809,23 @@
       <c r="IX24" s="51"/>
     </row>
     <row r="25" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A25" s="97"/>
+      <c r="A25" s="100"/>
       <c r="B25" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="67"/>
+      <c r="G25" s="66"/>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
       <c r="J25" s="20"/>
-      <c r="K25" s="73"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="21"/>
       <c r="M25" s="51"/>
       <c r="N25" s="51"/>
@@ -9107,7 +9085,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="73"/>
+      <c r="K26" s="71"/>
       <c r="L26" s="21"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
@@ -9357,7 +9335,7 @@
       <c r="IX26" s="24"/>
     </row>
     <row r="27" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A27" s="98"/>
+      <c r="A27" s="101"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
       <c r="D27" s="33"/>
@@ -9366,8 +9344,8 @@
       <c r="G27" s="34"/>
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="73"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="71"/>
       <c r="L27" s="21"/>
       <c r="M27" s="51"/>
       <c r="N27" s="51"/>
@@ -9617,7 +9595,7 @@
       <c r="IX27" s="51"/>
     </row>
     <row r="28" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A28" s="98"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
@@ -9626,8 +9604,8 @@
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="73"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="71"/>
       <c r="L28" s="21"/>
       <c r="M28" s="51"/>
       <c r="N28" s="51"/>
@@ -9877,7 +9855,7 @@
       <c r="IX28" s="51"/>
     </row>
     <row r="29" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A29" s="98"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
@@ -9886,8 +9864,8 @@
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
       <c r="I29" s="35"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="73"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="71"/>
       <c r="L29" s="21"/>
       <c r="M29" s="51"/>
       <c r="N29" s="51"/>
@@ -10147,7 +10125,7 @@
       <c r="H30" s="20"/>
       <c r="I30" s="53"/>
       <c r="J30" s="53"/>
-      <c r="K30" s="73"/>
+      <c r="K30" s="71"/>
       <c r="L30" s="21"/>
       <c r="M30" s="51"/>
       <c r="N30" s="51"/>
@@ -10407,7 +10385,7 @@
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
-      <c r="K31" s="73"/>
+      <c r="K31" s="71"/>
       <c r="L31" s="21"/>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
@@ -10657,7 +10635,7 @@
       <c r="IX31" s="24"/>
     </row>
     <row r="32" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A32" s="95"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
       <c r="D32" s="33"/>
@@ -10666,8 +10644,8 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="73"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="71"/>
       <c r="L32" s="21"/>
       <c r="M32" s="51"/>
       <c r="N32" s="51"/>
@@ -10917,7 +10895,7 @@
       <c r="IX32" s="51"/>
     </row>
     <row r="33" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A33" s="96"/>
+      <c r="A33" s="99"/>
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
@@ -10926,8 +10904,8 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="73"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="71"/>
       <c r="L33" s="21"/>
       <c r="M33" s="51"/>
       <c r="N33" s="51"/>
@@ -11177,7 +11155,7 @@
       <c r="IX33" s="51"/>
     </row>
     <row r="34" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A34" s="97"/>
+      <c r="A34" s="100"/>
       <c r="B34" s="35"/>
       <c r="C34" s="37"/>
       <c r="D34" s="37"/>
@@ -11186,8 +11164,8 @@
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="89"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="87"/>
       <c r="L34" s="43"/>
     </row>
     <row r="35" spans="1:258" s="4" customFormat="1" ht="18.75" customHeight="1">
@@ -11201,7 +11179,7 @@
       <c r="H35" s="40"/>
       <c r="I35" s="40"/>
       <c r="J35" s="39"/>
-      <c r="K35" s="89"/>
+      <c r="K35" s="87"/>
       <c r="L35" s="43"/>
       <c r="M35" s="39"/>
       <c r="N35" s="39"/>
@@ -11451,7 +11429,7 @@
       <c r="IX35" s="39"/>
     </row>
     <row r="36" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A36" s="99"/>
+      <c r="A36" s="89"/>
       <c r="B36" s="32"/>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
@@ -11460,12 +11438,12 @@
       <c r="G36" s="42"/>
       <c r="H36" s="41"/>
       <c r="I36" s="42"/>
-      <c r="J36" s="90"/>
-      <c r="K36" s="89"/>
+      <c r="J36" s="88"/>
+      <c r="K36" s="87"/>
       <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A37" s="100"/>
+      <c r="A37" s="90"/>
       <c r="B37" s="20"/>
       <c r="C37" s="43"/>
       <c r="D37" s="43"/>
@@ -11473,12 +11451,12 @@
       <c r="F37" s="41"/>
       <c r="G37" s="44"/>
       <c r="I37" s="44"/>
-      <c r="J37" s="89"/>
-      <c r="K37" s="89"/>
+      <c r="J37" s="87"/>
+      <c r="K37" s="87"/>
       <c r="L37" s="43"/>
     </row>
     <row r="38" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A38" s="100"/>
+      <c r="A38" s="90"/>
       <c r="B38" s="20"/>
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
@@ -11487,12 +11465,12 @@
       <c r="G38" s="44"/>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="87"/>
       <c r="L38" s="43"/>
     </row>
     <row r="39" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A39" s="101"/>
+      <c r="A39" s="91"/>
       <c r="B39" s="35"/>
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
@@ -11501,8 +11479,8 @@
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
       <c r="I39" s="38"/>
-      <c r="J39" s="88"/>
-      <c r="K39" s="89"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="87"/>
       <c r="L39" s="43"/>
     </row>
     <row r="40" spans="1:258" s="4" customFormat="1" ht="15.75" customHeight="1">
@@ -11516,7 +11494,7 @@
       <c r="H40" s="39"/>
       <c r="I40" s="40"/>
       <c r="J40" s="39"/>
-      <c r="K40" s="89"/>
+      <c r="K40" s="87"/>
       <c r="L40" s="43"/>
       <c r="M40" s="39"/>
       <c r="N40" s="39"/>
@@ -11766,7 +11744,7 @@
       <c r="IX40" s="39"/>
     </row>
     <row r="41" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A41" s="99"/>
+      <c r="A41" s="89"/>
       <c r="B41" s="42"/>
       <c r="C41" s="41"/>
       <c r="D41" s="41"/>
@@ -11775,12 +11753,12 @@
       <c r="G41" s="42"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="89"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="87"/>
       <c r="L41" s="43"/>
     </row>
     <row r="42" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A42" s="100"/>
+      <c r="A42" s="90"/>
       <c r="B42" s="44"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -11789,12 +11767,12 @@
       <c r="G42" s="44"/>
       <c r="H42" s="44"/>
       <c r="I42" s="44"/>
-      <c r="J42" s="89"/>
-      <c r="K42" s="89"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="43"/>
     </row>
     <row r="43" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A43" s="100"/>
+      <c r="A43" s="90"/>
       <c r="B43" s="44"/>
       <c r="C43" s="43"/>
       <c r="D43" s="43"/>
@@ -11803,12 +11781,12 @@
       <c r="G43" s="44"/>
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
-      <c r="J43" s="89"/>
-      <c r="K43" s="89"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
       <c r="L43" s="43"/>
     </row>
     <row r="44" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A44" s="100"/>
+      <c r="A44" s="90"/>
       <c r="B44" s="44"/>
       <c r="C44" s="43"/>
       <c r="D44" s="43"/>
@@ -11817,12 +11795,12 @@
       <c r="G44" s="44"/>
       <c r="H44" s="20"/>
       <c r="I44" s="44"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="89"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
       <c r="L44" s="43"/>
     </row>
     <row r="45" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A45" s="100"/>
+      <c r="A45" s="90"/>
       <c r="B45" s="44"/>
       <c r="C45" s="43"/>
       <c r="D45" s="43"/>
@@ -11831,12 +11809,12 @@
       <c r="G45" s="20"/>
       <c r="H45" s="44"/>
       <c r="I45" s="44"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
       <c r="L45" s="43"/>
     </row>
     <row r="46" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A46" s="101"/>
+      <c r="A46" s="91"/>
       <c r="B46" s="44"/>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
@@ -11845,12 +11823,12 @@
       <c r="G46" s="44"/>
       <c r="H46" s="44"/>
       <c r="I46" s="44"/>
-      <c r="J46" s="89"/>
-      <c r="K46" s="89"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="87"/>
       <c r="L46" s="43"/>
     </row>
     <row r="47" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A47" s="99"/>
+      <c r="A47" s="89"/>
       <c r="B47" s="44"/>
       <c r="C47" s="43"/>
       <c r="D47" s="43"/>
@@ -11859,13 +11837,13 @@
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
       <c r="I47" s="44"/>
-      <c r="J47" s="89"/>
-      <c r="K47" s="89"/>
+      <c r="J47" s="87"/>
+      <c r="K47" s="87"/>
       <c r="L47" s="43"/>
     </row>
     <row r="48" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A48" s="100"/>
-      <c r="B48" s="102"/>
+      <c r="A48" s="90"/>
+      <c r="B48" s="92"/>
       <c r="C48" s="21"/>
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
@@ -11873,13 +11851,13 @@
       <c r="G48" s="44"/>
       <c r="H48" s="20"/>
       <c r="I48" s="44"/>
-      <c r="J48" s="89"/>
-      <c r="K48" s="89"/>
+      <c r="J48" s="87"/>
+      <c r="K48" s="87"/>
       <c r="L48" s="43"/>
     </row>
     <row r="49" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A49" s="100"/>
-      <c r="B49" s="103"/>
+      <c r="A49" s="90"/>
+      <c r="B49" s="93"/>
       <c r="C49" s="21"/>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
@@ -11887,12 +11865,12 @@
       <c r="G49" s="44"/>
       <c r="H49" s="20"/>
       <c r="I49" s="44"/>
-      <c r="J49" s="89"/>
-      <c r="K49" s="89"/>
+      <c r="J49" s="87"/>
+      <c r="K49" s="87"/>
       <c r="L49" s="43"/>
     </row>
     <row r="50" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A50" s="100"/>
+      <c r="A50" s="90"/>
       <c r="B50" s="44"/>
       <c r="C50" s="43"/>
       <c r="D50" s="43"/>
@@ -11901,12 +11879,12 @@
       <c r="G50" s="44"/>
       <c r="H50" s="43"/>
       <c r="I50" s="44"/>
-      <c r="J50" s="89"/>
-      <c r="K50" s="89"/>
+      <c r="J50" s="87"/>
+      <c r="K50" s="87"/>
       <c r="L50" s="43"/>
     </row>
     <row r="51" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A51" s="101"/>
+      <c r="A51" s="91"/>
       <c r="B51" s="44"/>
       <c r="C51" s="43"/>
       <c r="D51" s="43"/>
@@ -11915,8 +11893,8 @@
       <c r="G51" s="44"/>
       <c r="H51" s="44"/>
       <c r="I51" s="44"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="89"/>
+      <c r="J51" s="87"/>
+      <c r="K51" s="87"/>
       <c r="L51" s="43"/>
     </row>
     <row r="52" spans="1:12" ht="99.95" customHeight="1">
@@ -11929,8 +11907,8 @@
       <c r="G52" s="44"/>
       <c r="H52" s="43"/>
       <c r="I52" s="44"/>
-      <c r="J52" s="89"/>
-      <c r="K52" s="89"/>
+      <c r="J52" s="87"/>
+      <c r="K52" s="87"/>
       <c r="L52" s="43"/>
     </row>
     <row r="53" spans="1:12" ht="99.95" customHeight="1">
@@ -11943,8 +11921,8 @@
       <c r="G53" s="44"/>
       <c r="H53" s="43"/>
       <c r="I53" s="44"/>
-      <c r="J53" s="89"/>
-      <c r="K53" s="89"/>
+      <c r="J53" s="87"/>
+      <c r="K53" s="87"/>
       <c r="L53" s="43"/>
     </row>
     <row r="54" spans="1:12" ht="99.95" customHeight="1">
@@ -11957,8 +11935,8 @@
       <c r="G54" s="44"/>
       <c r="H54" s="43"/>
       <c r="I54" s="44"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="89"/>
+      <c r="J54" s="87"/>
+      <c r="K54" s="87"/>
       <c r="L54" s="43"/>
     </row>
     <row r="55" spans="1:12" ht="99.95" customHeight="1">
@@ -11971,8 +11949,8 @@
       <c r="G55" s="44"/>
       <c r="H55" s="43"/>
       <c r="I55" s="44"/>
-      <c r="J55" s="89"/>
-      <c r="K55" s="89"/>
+      <c r="J55" s="87"/>
+      <c r="K55" s="87"/>
       <c r="L55" s="43"/>
     </row>
   </sheetData>
@@ -12603,7 +12581,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>21</v>
@@ -13122,13 +13100,13 @@
     </row>
     <row r="6" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A6" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>90</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>92</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>26</v>
@@ -13137,7 +13115,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="26"/>
@@ -13652,13 +13630,13 @@
     </row>
     <row r="8" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A8" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>96</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>26</v>
@@ -13667,7 +13645,7 @@
       <c r="F8" s="27"/>
       <c r="G8" s="29"/>
       <c r="H8" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="26"/>
@@ -14181,14 +14159,14 @@
       <c r="IX9" s="24"/>
     </row>
     <row r="10" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>98</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>100</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>18</v>
@@ -14196,10 +14174,10 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="G10" s="34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I10" s="33"/>
       <c r="J10" s="32"/>
@@ -14453,12 +14431,12 @@
       <c r="IX10" s="51"/>
     </row>
     <row r="11" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A11" s="98"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>26</v>
@@ -14467,7 +14445,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="20"/>
@@ -14723,12 +14701,12 @@
       <c r="IX11" s="51"/>
     </row>
     <row r="12" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A12" s="98"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>26</v>
@@ -14737,7 +14715,7 @@
       <c r="F12" s="36"/>
       <c r="G12" s="35"/>
       <c r="H12" s="35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I12" s="36"/>
       <c r="J12" s="35"/>
@@ -14995,10 +14973,10 @@
     <row r="13" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>26</v>
@@ -15007,7 +14985,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I13" s="52"/>
       <c r="J13" s="53"/>
@@ -15521,14 +15499,14 @@
       <c r="IX14" s="24"/>
     </row>
     <row r="15" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>112</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>114</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>18</v>
@@ -15536,10 +15514,10 @@
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="G15" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I15" s="33"/>
       <c r="J15" s="32"/>
@@ -15793,12 +15771,12 @@
       <c r="IX15" s="51"/>
     </row>
     <row r="16" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
-      <c r="A16" s="96"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>26</v>
@@ -15807,7 +15785,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="20"/>
@@ -16061,12 +16039,12 @@
       <c r="IX16" s="51"/>
     </row>
     <row r="17" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A17" s="97"/>
+      <c r="A17" s="100"/>
       <c r="B17" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D17" s="37" t="s">
         <v>26</v>
@@ -16075,7 +16053,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="37"/>
@@ -16342,90 +16320,90 @@
       <c r="IX18" s="39"/>
     </row>
     <row r="19" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A19" s="99" t="s">
+      <c r="A19" s="89" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="41" t="s">
         <v>123</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>125</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A20" s="100"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D20" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A21" s="100"/>
+      <c r="A21" s="90"/>
       <c r="B21" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="43"/>
       <c r="F21" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G21" s="44"/>
       <c r="H21" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
     </row>
     <row r="22" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A22" s="101"/>
+      <c r="A22" s="91"/>
       <c r="B22" s="35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D22" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="37"/>
       <c r="F22" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G22" s="38"/>
       <c r="H22" s="38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I22" s="37"/>
       <c r="J22" s="37"/>
@@ -16691,247 +16669,247 @@
       <c r="IX23" s="39"/>
     </row>
     <row r="24" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="41" t="s">
         <v>134</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>136</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G24" s="42"/>
       <c r="H24" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I24" s="41"/>
       <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A25" s="100"/>
+      <c r="A25" s="90"/>
       <c r="B25" s="44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G25" s="44"/>
       <c r="H25" s="44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A26" s="100"/>
+      <c r="A26" s="90"/>
       <c r="B26" s="44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="43"/>
       <c r="F26" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G26" s="44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H26" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A27" s="100"/>
+      <c r="A27" s="90"/>
       <c r="B27" s="44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D27" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="43"/>
       <c r="F27" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G27" s="44"/>
       <c r="H27" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A28" s="100"/>
+      <c r="A28" s="90"/>
       <c r="B28" s="44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="43"/>
       <c r="F28" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I28" s="43"/>
       <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A29" s="101"/>
+      <c r="A29" s="91"/>
       <c r="B29" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D29" s="43" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="43"/>
       <c r="F29" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G29" s="44"/>
       <c r="H29" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="43" t="s">
         <v>152</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>154</v>
       </c>
       <c r="D30" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="43"/>
       <c r="F30" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
     </row>
     <row r="31" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A31" s="100"/>
-      <c r="B31" s="102" t="s">
-        <v>156</v>
+      <c r="A31" s="90"/>
+      <c r="B31" s="92" t="s">
+        <v>154</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G31" s="44"/>
       <c r="H31" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
     </row>
     <row r="32" spans="1:258" ht="99.95" customHeight="1">
-      <c r="A32" s="100"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="93"/>
       <c r="C32" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G32" s="44"/>
       <c r="H32" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I32" s="43"/>
       <c r="J32" s="43"/>
     </row>
     <row r="33" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A33" s="100"/>
+      <c r="A33" s="90"/>
       <c r="B33" s="44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G33" s="44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
       <c r="J33" s="43"/>
     </row>
     <row r="34" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A34" s="101"/>
+      <c r="A34" s="91"/>
       <c r="B34" s="44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="43"/>
       <c r="F34" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G34" s="44"/>
       <c r="H34" s="44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I34" s="43"/>
       <c r="J34" s="43"/>

</xml_diff>

<commit_message>
Implement get action API.
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -2556,8 +2556,8 @@
   <dimension ref="A1:IX55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="15.75"/>
@@ -7736,7 +7736,7 @@
     </row>
     <row r="21" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A21" s="99"/>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="56" t="s">
         <v>74</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -8542,7 +8542,7 @@
     </row>
     <row r="24" spans="1:258" s="2" customFormat="1" ht="99.95" customHeight="1">
       <c r="A24" s="99"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="56" t="s">
         <v>82</v>
       </c>
       <c r="C24" s="20" t="s">

</xml_diff>

<commit_message>
add record access configuration.
</commit_message>
<xml_diff>
--- a/code/s3d/document/design/API.xlsx
+++ b/code/s3d/document/design/API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="8865"/>
+    <workbookView windowWidth="19095" windowHeight="8865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>{"status":"succeed",
 "token":"",
 "user":{
@@ -1694,6 +1700,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1718,85 +1747,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1824,10 +1775,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1883,30 +1889,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1931,49 +1913,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2021,7 +1979,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2040,6 +2022,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2242,6 +2248,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2252,6 +2273,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2290,177 +2320,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3172,10 +3178,10 @@
   <sheetPr/>
   <dimension ref="A1:IX55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.2" defaultRowHeight="15.75"/>
@@ -3185,7 +3191,7 @@
     <col min="3" max="3" width="17.8" style="7" customWidth="1"/>
     <col min="4" max="4" width="6.3" style="7" customWidth="1"/>
     <col min="5" max="5" width="2.1" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.6" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.42" style="7" customWidth="1"/>
     <col min="7" max="7" width="37.2" style="6" customWidth="1"/>
     <col min="8" max="8" width="40.9" style="7" customWidth="1"/>
     <col min="9" max="9" width="35.4" style="6" customWidth="1"/>
@@ -12596,7 +12602,7 @@
   <sheetPr/>
   <dimension ref="A1:IX38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>